<commit_message>
Ostrava flights are saving in the excel file
</commit_message>
<xml_diff>
--- a/src/data/flights.xlsx
+++ b/src/data/flights.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="327">
   <si>
     <t>From (City)</t>
   </si>
@@ -830,93 +830,93 @@
     <t>Brno</t>
   </si>
   <si>
+    <t>ANTALYA</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Travel Service</t>
+  </si>
+  <si>
+    <t>LONDON LUTON</t>
+  </si>
+  <si>
+    <t>HERAKLION</t>
+  </si>
+  <si>
+    <t>MUNICH</t>
+  </si>
+  <si>
+    <t>bmi regional</t>
+  </si>
+  <si>
+    <t>ALMERIA / OSTRAVA</t>
+  </si>
+  <si>
+    <t>LONDON STANSTED</t>
+  </si>
+  <si>
+    <t>PALMA DE MALLORCA</t>
+  </si>
+  <si>
+    <t>RHODOS</t>
+  </si>
+  <si>
+    <t>CORFU</t>
+  </si>
+  <si>
+    <t>ENFIDHA</t>
+  </si>
+  <si>
+    <t>KOS</t>
+  </si>
+  <si>
+    <t>BURGAS</t>
+  </si>
+  <si>
+    <t>ZAKYNTHOS</t>
+  </si>
+  <si>
+    <t>PREVEZA</t>
+  </si>
+  <si>
     <t>HURGHADA</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>Travel Service</t>
-  </si>
-  <si>
-    <t>ANTALYA</t>
-  </si>
-  <si>
     <t>EINDHOVEN</t>
   </si>
   <si>
-    <t>HERAKLION</t>
-  </si>
-  <si>
-    <t>MUNICH</t>
-  </si>
-  <si>
-    <t>bmi regional</t>
-  </si>
-  <si>
-    <t>LONDON STANSTED</t>
-  </si>
-  <si>
-    <t>PALMA DE MALLORCA</t>
-  </si>
-  <si>
     <t>MARSA ALAM</t>
   </si>
   <si>
-    <t>BURGAS</t>
-  </si>
-  <si>
-    <t>RHODOS</t>
-  </si>
-  <si>
-    <t>LONDON LUTON</t>
-  </si>
-  <si>
-    <t>CORFU</t>
-  </si>
-  <si>
-    <t>KOS</t>
+    <t>VARNA / OSTRAVA</t>
+  </si>
+  <si>
+    <t>DJERBA / ENFIDHA</t>
+  </si>
+  <si>
+    <t>MONASTIR / OSTRAVA</t>
+  </si>
+  <si>
+    <t>LAMEZIA TERME</t>
+  </si>
+  <si>
+    <t>VARNA</t>
+  </si>
+  <si>
+    <t>ERCAN / ANTALYA</t>
+  </si>
+  <si>
+    <t>Tailwind Airlines</t>
+  </si>
+  <si>
+    <t>DJERBA / OSTRAVA</t>
   </si>
   <si>
     <t>KAVALA / OSTRAVA</t>
   </si>
   <si>
-    <t>ZAKYNTHOS</t>
-  </si>
-  <si>
-    <t>ERCAN / ANTALYA</t>
-  </si>
-  <si>
-    <t>Tailwind Airlines</t>
-  </si>
-  <si>
-    <t>ALMERIA / OSTRAVA</t>
-  </si>
-  <si>
-    <t>ENFIDHA</t>
-  </si>
-  <si>
-    <t>PREVEZA</t>
-  </si>
-  <si>
-    <t>VARNA / OSTRAVA</t>
-  </si>
-  <si>
-    <t>DJERBA / ENFIDHA</t>
-  </si>
-  <si>
-    <t>MONASTIR / OSTRAVA</t>
-  </si>
-  <si>
-    <t>LAMEZIA TERME</t>
-  </si>
-  <si>
-    <t>VARNA</t>
-  </si>
-  <si>
-    <t>DJERBA / OSTRAVA</t>
-  </si>
-  <si>
     <t>THESSALONIKI</t>
   </si>
   <si>
@@ -927,6 +927,84 @@
   </si>
   <si>
     <t>ANTALYA / BRATISLAVA</t>
+  </si>
+  <si>
+    <t>Prague, Václav Havel Airport Prague (PRG)</t>
+  </si>
+  <si>
+    <t>CZECH AIRLINES (CSA)</t>
+  </si>
+  <si>
+    <t>Crete / Heraklion, N. Kazantzakis Apt. (HER)</t>
+  </si>
+  <si>
+    <t>TRAVEL SERVICE / SMARTWINGS</t>
+  </si>
+  <si>
+    <t>ALMERIA</t>
+  </si>
+  <si>
+    <t>Mallorca, Palma de Mallorca (PMI)</t>
+  </si>
+  <si>
+    <t>Košice</t>
+  </si>
+  <si>
+    <t>Rhodes, Diagoras Airport (RHO)</t>
+  </si>
+  <si>
+    <t>Milan / Bergamo, Milan Bergamo Airport</t>
+  </si>
+  <si>
+    <t>RYANAIR</t>
+  </si>
+  <si>
+    <t>Corfu / Kerkyra, I. Kapodistrias (CFU)</t>
+  </si>
+  <si>
+    <t>London, Stansted (STN)</t>
+  </si>
+  <si>
+    <t>Antalya, Antayla (AYT)</t>
+  </si>
+  <si>
+    <t>ERCAN</t>
+  </si>
+  <si>
+    <t>TAILWIND</t>
+  </si>
+  <si>
+    <t>Burgas, Burgas Airport (BOJ)</t>
+  </si>
+  <si>
+    <t>Zakynthos, Zakinthos Is (ZTH)</t>
+  </si>
+  <si>
+    <t>Hurghada, Hurghada (HRG)</t>
+  </si>
+  <si>
+    <t>Marsa Alam, Marsa Alam (RMF)</t>
+  </si>
+  <si>
+    <t>Varna, Varna Airport (VAR)</t>
+  </si>
+  <si>
+    <t>Kos, Kos Island International Airport (KGS)</t>
+  </si>
+  <si>
+    <t>MONASTIR</t>
+  </si>
+  <si>
+    <t>BRATISLAVA</t>
+  </si>
+  <si>
+    <t>Djerba</t>
+  </si>
+  <si>
+    <t>KAVALA</t>
+  </si>
+  <si>
+    <t>Warsawa</t>
   </si>
 </sst>
 </file>
@@ -1289,8 +1367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
+      <selection activeCell="D228" sqref="D228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4210,7 +4288,7 @@
         <v>269</v>
       </c>
       <c r="D208" t="s">
-        <v>270</v>
+        <v>28</v>
       </c>
     </row>
     <row r="209">
@@ -4224,7 +4302,7 @@
         <v>269</v>
       </c>
       <c r="D209" t="s">
-        <v>28</v>
+        <v>270</v>
       </c>
     </row>
     <row r="210">
@@ -4238,7 +4316,7 @@
         <v>269</v>
       </c>
       <c r="D210" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
     </row>
     <row r="211">
@@ -4246,13 +4324,13 @@
         <v>267</v>
       </c>
       <c r="B211" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C211" t="s">
         <v>269</v>
       </c>
       <c r="D211" t="s">
-        <v>275</v>
+        <v>99</v>
       </c>
     </row>
     <row r="212">
@@ -4260,13 +4338,13 @@
         <v>267</v>
       </c>
       <c r="B212" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C212" t="s">
         <v>269</v>
       </c>
       <c r="D212" t="s">
-        <v>99</v>
+        <v>270</v>
       </c>
     </row>
     <row r="213">
@@ -4336,7 +4414,7 @@
         <v>269</v>
       </c>
       <c r="D217" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
     </row>
     <row r="218">
@@ -4350,7 +4428,7 @@
         <v>269</v>
       </c>
       <c r="D218" t="s">
-        <v>28</v>
+        <v>270</v>
       </c>
     </row>
     <row r="219">
@@ -4420,7 +4498,7 @@
         <v>269</v>
       </c>
       <c r="D223" t="s">
-        <v>287</v>
+        <v>28</v>
       </c>
     </row>
     <row r="224">
@@ -4428,7 +4506,7 @@
         <v>267</v>
       </c>
       <c r="B224" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C224" t="s">
         <v>269</v>
@@ -4442,13 +4520,13 @@
         <v>267</v>
       </c>
       <c r="B225" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C225" t="s">
         <v>269</v>
       </c>
       <c r="D225" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
     </row>
     <row r="226">
@@ -4456,7 +4534,7 @@
         <v>267</v>
       </c>
       <c r="B226" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C226" t="s">
         <v>269</v>
@@ -4470,13 +4548,13 @@
         <v>267</v>
       </c>
       <c r="B227" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C227" t="s">
         <v>269</v>
       </c>
       <c r="D227" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
     </row>
     <row r="228">
@@ -4484,7 +4562,7 @@
         <v>267</v>
       </c>
       <c r="B228" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C228" t="s">
         <v>269</v>
@@ -4498,13 +4576,13 @@
         <v>267</v>
       </c>
       <c r="B229" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C229" t="s">
         <v>269</v>
       </c>
       <c r="D229" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
     </row>
     <row r="230">
@@ -4512,13 +4590,13 @@
         <v>267</v>
       </c>
       <c r="B230" t="s">
+        <v>293</v>
+      </c>
+      <c r="C230" t="s">
+        <v>269</v>
+      </c>
+      <c r="D230" t="s">
         <v>294</v>
-      </c>
-      <c r="C230" t="s">
-        <v>269</v>
-      </c>
-      <c r="D230" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="231">
@@ -4532,7 +4610,7 @@
         <v>269</v>
       </c>
       <c r="D231" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
     </row>
     <row r="232">
@@ -4546,7 +4624,7 @@
         <v>269</v>
       </c>
       <c r="D232" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
     </row>
     <row r="233">
@@ -4602,7 +4680,749 @@
         <v>269</v>
       </c>
       <c r="D236" t="s">
-        <v>287</v>
+        <v>294</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="s">
+        <v>189</v>
+      </c>
+      <c r="B237" t="s">
+        <v>301</v>
+      </c>
+      <c r="C237" t="s">
+        <v>269</v>
+      </c>
+      <c r="D237" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="s">
+        <v>189</v>
+      </c>
+      <c r="B238" t="s">
+        <v>301</v>
+      </c>
+      <c r="C238" t="s">
+        <v>269</v>
+      </c>
+      <c r="D238"/>
+    </row>
+    <row r="239">
+      <c r="A239" t="s">
+        <v>189</v>
+      </c>
+      <c r="B239" t="s">
+        <v>301</v>
+      </c>
+      <c r="C239" t="s">
+        <v>269</v>
+      </c>
+      <c r="D239"/>
+    </row>
+    <row r="240">
+      <c r="A240" t="s">
+        <v>189</v>
+      </c>
+      <c r="B240" t="s">
+        <v>301</v>
+      </c>
+      <c r="C240" t="s">
+        <v>269</v>
+      </c>
+      <c r="D240"/>
+    </row>
+    <row r="241">
+      <c r="A241" t="s">
+        <v>189</v>
+      </c>
+      <c r="B241" t="s">
+        <v>301</v>
+      </c>
+      <c r="C241" t="s">
+        <v>269</v>
+      </c>
+      <c r="D241"/>
+    </row>
+    <row r="242">
+      <c r="A242" t="s">
+        <v>189</v>
+      </c>
+      <c r="B242" t="s">
+        <v>301</v>
+      </c>
+      <c r="C242" t="s">
+        <v>269</v>
+      </c>
+      <c r="D242"/>
+    </row>
+    <row r="243">
+      <c r="A243" t="s">
+        <v>189</v>
+      </c>
+      <c r="B243" t="s">
+        <v>303</v>
+      </c>
+      <c r="C243" t="s">
+        <v>269</v>
+      </c>
+      <c r="D243" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="s">
+        <v>189</v>
+      </c>
+      <c r="B244" t="s">
+        <v>301</v>
+      </c>
+      <c r="C244" t="s">
+        <v>269</v>
+      </c>
+      <c r="D244" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="s">
+        <v>189</v>
+      </c>
+      <c r="B245" t="s">
+        <v>301</v>
+      </c>
+      <c r="C245" t="s">
+        <v>269</v>
+      </c>
+      <c r="D245"/>
+    </row>
+    <row r="246">
+      <c r="A246" t="s">
+        <v>189</v>
+      </c>
+      <c r="B246" t="s">
+        <v>301</v>
+      </c>
+      <c r="C246" t="s">
+        <v>269</v>
+      </c>
+      <c r="D246"/>
+    </row>
+    <row r="247">
+      <c r="A247" t="s">
+        <v>189</v>
+      </c>
+      <c r="B247" t="s">
+        <v>301</v>
+      </c>
+      <c r="C247" t="s">
+        <v>269</v>
+      </c>
+      <c r="D247"/>
+    </row>
+    <row r="248">
+      <c r="A248" t="s">
+        <v>189</v>
+      </c>
+      <c r="B248" t="s">
+        <v>305</v>
+      </c>
+      <c r="C248" t="s">
+        <v>269</v>
+      </c>
+      <c r="D248" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="s">
+        <v>189</v>
+      </c>
+      <c r="B249" t="s">
+        <v>306</v>
+      </c>
+      <c r="C249" t="s">
+        <v>269</v>
+      </c>
+      <c r="D249" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="s">
+        <v>189</v>
+      </c>
+      <c r="B250" t="s">
+        <v>307</v>
+      </c>
+      <c r="C250" t="s">
+        <v>269</v>
+      </c>
+      <c r="D250" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="s">
+        <v>189</v>
+      </c>
+      <c r="B251" t="s">
+        <v>307</v>
+      </c>
+      <c r="C251" t="s">
+        <v>269</v>
+      </c>
+      <c r="D251"/>
+    </row>
+    <row r="252">
+      <c r="A252" t="s">
+        <v>189</v>
+      </c>
+      <c r="B252" t="s">
+        <v>307</v>
+      </c>
+      <c r="C252" t="s">
+        <v>269</v>
+      </c>
+      <c r="D252"/>
+    </row>
+    <row r="253">
+      <c r="A253" t="s">
+        <v>189</v>
+      </c>
+      <c r="B253" t="s">
+        <v>307</v>
+      </c>
+      <c r="C253" t="s">
+        <v>269</v>
+      </c>
+      <c r="D253"/>
+    </row>
+    <row r="254">
+      <c r="A254" t="s">
+        <v>189</v>
+      </c>
+      <c r="B254" t="s">
+        <v>308</v>
+      </c>
+      <c r="C254" t="s">
+        <v>269</v>
+      </c>
+      <c r="D254" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="s">
+        <v>189</v>
+      </c>
+      <c r="B255" t="s">
+        <v>307</v>
+      </c>
+      <c r="C255" t="s">
+        <v>269</v>
+      </c>
+      <c r="D255" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="s">
+        <v>189</v>
+      </c>
+      <c r="B256" t="s">
+        <v>307</v>
+      </c>
+      <c r="C256" t="s">
+        <v>269</v>
+      </c>
+      <c r="D256"/>
+    </row>
+    <row r="257">
+      <c r="A257" t="s">
+        <v>189</v>
+      </c>
+      <c r="B257" t="s">
+        <v>307</v>
+      </c>
+      <c r="C257" t="s">
+        <v>269</v>
+      </c>
+      <c r="D257"/>
+    </row>
+    <row r="258">
+      <c r="A258" t="s">
+        <v>189</v>
+      </c>
+      <c r="B258" t="s">
+        <v>307</v>
+      </c>
+      <c r="C258" t="s">
+        <v>269</v>
+      </c>
+      <c r="D258"/>
+    </row>
+    <row r="259">
+      <c r="A259" t="s">
+        <v>189</v>
+      </c>
+      <c r="B259" t="s">
+        <v>307</v>
+      </c>
+      <c r="C259" t="s">
+        <v>269</v>
+      </c>
+      <c r="D259"/>
+    </row>
+    <row r="260">
+      <c r="A260" t="s">
+        <v>189</v>
+      </c>
+      <c r="B260" t="s">
+        <v>309</v>
+      </c>
+      <c r="C260" t="s">
+        <v>269</v>
+      </c>
+      <c r="D260" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="s">
+        <v>189</v>
+      </c>
+      <c r="B261" t="s">
+        <v>311</v>
+      </c>
+      <c r="C261" t="s">
+        <v>269</v>
+      </c>
+      <c r="D261" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="s">
+        <v>189</v>
+      </c>
+      <c r="B262" t="s">
+        <v>312</v>
+      </c>
+      <c r="C262" t="s">
+        <v>269</v>
+      </c>
+      <c r="D262" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="s">
+        <v>189</v>
+      </c>
+      <c r="B263" t="s">
+        <v>313</v>
+      </c>
+      <c r="C263" t="s">
+        <v>269</v>
+      </c>
+      <c r="D263" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="s">
+        <v>189</v>
+      </c>
+      <c r="B264" t="s">
+        <v>314</v>
+      </c>
+      <c r="C264" t="s">
+        <v>269</v>
+      </c>
+      <c r="D264" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="s">
+        <v>189</v>
+      </c>
+      <c r="B265" t="s">
+        <v>316</v>
+      </c>
+      <c r="C265" t="s">
+        <v>269</v>
+      </c>
+      <c r="D265" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="s">
+        <v>189</v>
+      </c>
+      <c r="B266" t="s">
+        <v>317</v>
+      </c>
+      <c r="C266" t="s">
+        <v>269</v>
+      </c>
+      <c r="D266" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="s">
+        <v>189</v>
+      </c>
+      <c r="B267" t="s">
+        <v>308</v>
+      </c>
+      <c r="C267" t="s">
+        <v>269</v>
+      </c>
+      <c r="D267" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="s">
+        <v>189</v>
+      </c>
+      <c r="B268" t="s">
+        <v>228</v>
+      </c>
+      <c r="C268" t="s">
+        <v>269</v>
+      </c>
+      <c r="D268" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="s">
+        <v>189</v>
+      </c>
+      <c r="B269" t="s">
+        <v>318</v>
+      </c>
+      <c r="C269" t="s">
+        <v>269</v>
+      </c>
+      <c r="D269" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="s">
+        <v>189</v>
+      </c>
+      <c r="B270" t="s">
+        <v>316</v>
+      </c>
+      <c r="C270" t="s">
+        <v>269</v>
+      </c>
+      <c r="D270" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="s">
+        <v>189</v>
+      </c>
+      <c r="B271" t="s">
+        <v>319</v>
+      </c>
+      <c r="C271" t="s">
+        <v>269</v>
+      </c>
+      <c r="D271" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="s">
+        <v>189</v>
+      </c>
+      <c r="B272" t="s">
+        <v>316</v>
+      </c>
+      <c r="C272" t="s">
+        <v>269</v>
+      </c>
+      <c r="D272" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="s">
+        <v>189</v>
+      </c>
+      <c r="B273" t="s">
+        <v>320</v>
+      </c>
+      <c r="C273" t="s">
+        <v>269</v>
+      </c>
+      <c r="D273" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="s">
+        <v>189</v>
+      </c>
+      <c r="B274" t="s">
+        <v>316</v>
+      </c>
+      <c r="C274" t="s">
+        <v>269</v>
+      </c>
+      <c r="D274" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="s">
+        <v>189</v>
+      </c>
+      <c r="B275" t="s">
+        <v>301</v>
+      </c>
+      <c r="C275" t="s">
+        <v>269</v>
+      </c>
+      <c r="D275" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="s">
+        <v>189</v>
+      </c>
+      <c r="B276" t="s">
+        <v>321</v>
+      </c>
+      <c r="C276" t="s">
+        <v>269</v>
+      </c>
+      <c r="D276" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="s">
+        <v>189</v>
+      </c>
+      <c r="B277" t="s">
+        <v>320</v>
+      </c>
+      <c r="C277" t="s">
+        <v>269</v>
+      </c>
+      <c r="D277" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="s">
+        <v>189</v>
+      </c>
+      <c r="B278" t="s">
+        <v>322</v>
+      </c>
+      <c r="C278" t="s">
+        <v>269</v>
+      </c>
+      <c r="D278"/>
+    </row>
+    <row r="279">
+      <c r="A279" t="s">
+        <v>189</v>
+      </c>
+      <c r="B279" t="s">
+        <v>316</v>
+      </c>
+      <c r="C279" t="s">
+        <v>269</v>
+      </c>
+      <c r="D279" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="s">
+        <v>189</v>
+      </c>
+      <c r="B280" t="s">
+        <v>323</v>
+      </c>
+      <c r="C280" t="s">
+        <v>269</v>
+      </c>
+      <c r="D280" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="s">
+        <v>189</v>
+      </c>
+      <c r="B281" t="s">
+        <v>324</v>
+      </c>
+      <c r="C281" t="s">
+        <v>269</v>
+      </c>
+      <c r="D281"/>
+    </row>
+    <row r="282">
+      <c r="A282" t="s">
+        <v>189</v>
+      </c>
+      <c r="B282" t="s">
+        <v>325</v>
+      </c>
+      <c r="C282" t="s">
+        <v>269</v>
+      </c>
+      <c r="D282" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="s">
+        <v>189</v>
+      </c>
+      <c r="B283" t="s">
+        <v>197</v>
+      </c>
+      <c r="C283" t="s">
+        <v>269</v>
+      </c>
+      <c r="D283" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="s">
+        <v>189</v>
+      </c>
+      <c r="B284" t="s">
+        <v>316</v>
+      </c>
+      <c r="C284" t="s">
+        <v>269</v>
+      </c>
+      <c r="D284" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="s">
+        <v>189</v>
+      </c>
+      <c r="B285" t="s">
+        <v>316</v>
+      </c>
+      <c r="C285" t="s">
+        <v>269</v>
+      </c>
+      <c r="D285" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="s">
+        <v>189</v>
+      </c>
+      <c r="B286" t="s">
+        <v>326</v>
+      </c>
+      <c r="C286" t="s">
+        <v>269</v>
+      </c>
+      <c r="D286" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="s">
+        <v>189</v>
+      </c>
+      <c r="B287" t="s">
+        <v>326</v>
+      </c>
+      <c r="C287" t="s">
+        <v>269</v>
+      </c>
+      <c r="D287"/>
+    </row>
+    <row r="288">
+      <c r="A288" t="s">
+        <v>189</v>
+      </c>
+      <c r="B288" t="s">
+        <v>326</v>
+      </c>
+      <c r="C288" t="s">
+        <v>269</v>
+      </c>
+      <c r="D288"/>
+    </row>
+    <row r="289">
+      <c r="A289" t="s">
+        <v>189</v>
+      </c>
+      <c r="B289" t="s">
+        <v>326</v>
+      </c>
+      <c r="C289" t="s">
+        <v>269</v>
+      </c>
+      <c r="D289"/>
+    </row>
+    <row r="290">
+      <c r="A290" t="s">
+        <v>189</v>
+      </c>
+      <c r="B290" t="s">
+        <v>326</v>
+      </c>
+      <c r="C290" t="s">
+        <v>269</v>
+      </c>
+      <c r="D290"/>
+    </row>
+    <row r="291">
+      <c r="A291" t="s">
+        <v>189</v>
+      </c>
+      <c r="B291" t="s">
+        <v>301</v>
+      </c>
+      <c r="C291" t="s">
+        <v>269</v>
+      </c>
+      <c r="D291" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="s">
+        <v>189</v>
+      </c>
+      <c r="B292" t="s">
+        <v>197</v>
+      </c>
+      <c r="C292" t="s">
+        <v>269</v>
+      </c>
+      <c r="D292" t="s">
+        <v>304</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bug with empty airline string of Ostrava
</commit_message>
<xml_diff>
--- a/src/data/flights.xlsx
+++ b/src/data/flights.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="331">
   <si>
     <t>From (City)</t>
   </si>
@@ -830,178 +830,190 @@
     <t>Brno</t>
   </si>
   <si>
+    <t>RHODOS</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Travel Service</t>
+  </si>
+  <si>
+    <t>HERAKLION</t>
+  </si>
+  <si>
+    <t>MUNICH</t>
+  </si>
+  <si>
+    <t>bmi regional</t>
+  </si>
+  <si>
+    <t>LONDON STANSTED</t>
+  </si>
+  <si>
+    <t>CORFU</t>
+  </si>
+  <si>
+    <t>ENFIDHA</t>
+  </si>
+  <si>
     <t>ANTALYA</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>Travel Service</t>
+    <t>KOS</t>
+  </si>
+  <si>
+    <t>BURGAS</t>
   </si>
   <si>
     <t>LONDON LUTON</t>
   </si>
   <si>
-    <t>HERAKLION</t>
-  </si>
-  <si>
-    <t>MUNICH</t>
-  </si>
-  <si>
-    <t>bmi regional</t>
+    <t>ZAKYNTHOS</t>
+  </si>
+  <si>
+    <t>PREVEZA</t>
+  </si>
+  <si>
+    <t>HURGHADA</t>
+  </si>
+  <si>
+    <t>EINDHOVEN</t>
+  </si>
+  <si>
+    <t>PALMA DE MALLORCA</t>
+  </si>
+  <si>
+    <t>MARSA ALAM</t>
+  </si>
+  <si>
+    <t>VARNA / OSTRAVA</t>
+  </si>
+  <si>
+    <t>DJERBA / ENFIDHA</t>
+  </si>
+  <si>
+    <t>MONASTIR / OSTRAVA</t>
+  </si>
+  <si>
+    <t>LAMEZIA TERME</t>
+  </si>
+  <si>
+    <t>VARNA</t>
+  </si>
+  <si>
+    <t>ERCAN / ANTALYA</t>
+  </si>
+  <si>
+    <t>Tailwind Airlines</t>
+  </si>
+  <si>
+    <t>DJERBA / OSTRAVA</t>
+  </si>
+  <si>
+    <t>KAVALA / OSTRAVA</t>
+  </si>
+  <si>
+    <t>THESSALONIKI</t>
+  </si>
+  <si>
+    <t>PODGORICA</t>
   </si>
   <si>
     <t>ALMERIA / OSTRAVA</t>
   </si>
   <si>
-    <t>LONDON STANSTED</t>
-  </si>
-  <si>
-    <t>PALMA DE MALLORCA</t>
-  </si>
-  <si>
-    <t>RHODOS</t>
-  </si>
-  <si>
-    <t>CORFU</t>
-  </si>
-  <si>
-    <t>ENFIDHA</t>
-  </si>
-  <si>
-    <t>KOS</t>
-  </si>
-  <si>
-    <t>BURGAS</t>
-  </si>
-  <si>
-    <t>ZAKYNTHOS</t>
-  </si>
-  <si>
-    <t>PREVEZA</t>
-  </si>
-  <si>
-    <t>HURGHADA</t>
-  </si>
-  <si>
-    <t>EINDHOVEN</t>
-  </si>
-  <si>
-    <t>MARSA ALAM</t>
-  </si>
-  <si>
-    <t>VARNA / OSTRAVA</t>
-  </si>
-  <si>
-    <t>DJERBA / ENFIDHA</t>
-  </si>
-  <si>
-    <t>MONASTIR / OSTRAVA</t>
-  </si>
-  <si>
-    <t>LAMEZIA TERME</t>
-  </si>
-  <si>
-    <t>VARNA</t>
-  </si>
-  <si>
-    <t>ERCAN / ANTALYA</t>
-  </si>
-  <si>
-    <t>Tailwind Airlines</t>
-  </si>
-  <si>
-    <t>DJERBA / OSTRAVA</t>
-  </si>
-  <si>
-    <t>KAVALA / OSTRAVA</t>
-  </si>
-  <si>
-    <t>THESSALONIKI</t>
-  </si>
-  <si>
-    <t>PODGORICA</t>
-  </si>
-  <si>
     <t>TENERIFE</t>
   </si>
   <si>
     <t>ANTALYA / BRATISLAVA</t>
   </si>
   <si>
+    <t>Rhodes, Diagoras Airport (RHO)</t>
+  </si>
+  <si>
+    <t>TRAVEL SERVICE / SMARTWINGS</t>
+  </si>
+  <si>
     <t>Prague, Václav Havel Airport Prague (PRG)</t>
   </si>
   <si>
     <t>CZECH AIRLINES (CSA)</t>
   </si>
   <si>
+    <t>KLM ROYAL DUTCH AIRLINES</t>
+  </si>
+  <si>
+    <t>DELTA AIR LINES</t>
+  </si>
+  <si>
+    <t>KOREAN AIR</t>
+  </si>
+  <si>
+    <t>TAROM ROMANIAN AIRLINES</t>
+  </si>
+  <si>
     <t>Crete / Heraklion, N. Kazantzakis Apt. (HER)</t>
   </si>
   <si>
-    <t>TRAVEL SERVICE / SMARTWINGS</t>
+    <t>Košice</t>
+  </si>
+  <si>
+    <t>Milan / Bergamo, Milan Bergamo Airport</t>
+  </si>
+  <si>
+    <t>RYANAIR</t>
+  </si>
+  <si>
+    <t>Corfu / Kerkyra, I. Kapodistrias (CFU)</t>
+  </si>
+  <si>
+    <t>London, Stansted (STN)</t>
+  </si>
+  <si>
+    <t>Antalya, Antayla (AYT)</t>
+  </si>
+  <si>
+    <t>ERCAN</t>
+  </si>
+  <si>
+    <t>TAILWIND</t>
+  </si>
+  <si>
+    <t>Burgas, Burgas Airport (BOJ)</t>
+  </si>
+  <si>
+    <t>Zakynthos, Zakinthos Is (ZTH)</t>
+  </si>
+  <si>
+    <t>Hurghada, Hurghada (HRG)</t>
+  </si>
+  <si>
+    <t>Mallorca, Palma de Mallorca (PMI)</t>
+  </si>
+  <si>
+    <t>Marsa Alam, Marsa Alam (RMF)</t>
+  </si>
+  <si>
+    <t>Varna, Varna Airport (VAR)</t>
+  </si>
+  <si>
+    <t>Kos, Kos Island International Airport (KGS)</t>
+  </si>
+  <si>
+    <t>MONASTIR</t>
+  </si>
+  <si>
+    <t>BRATISLAVA</t>
+  </si>
+  <si>
+    <t>Djerba</t>
+  </si>
+  <si>
+    <t>KAVALA</t>
   </si>
   <si>
     <t>ALMERIA</t>
-  </si>
-  <si>
-    <t>Mallorca, Palma de Mallorca (PMI)</t>
-  </si>
-  <si>
-    <t>Košice</t>
-  </si>
-  <si>
-    <t>Rhodes, Diagoras Airport (RHO)</t>
-  </si>
-  <si>
-    <t>Milan / Bergamo, Milan Bergamo Airport</t>
-  </si>
-  <si>
-    <t>RYANAIR</t>
-  </si>
-  <si>
-    <t>Corfu / Kerkyra, I. Kapodistrias (CFU)</t>
-  </si>
-  <si>
-    <t>London, Stansted (STN)</t>
-  </si>
-  <si>
-    <t>Antalya, Antayla (AYT)</t>
-  </si>
-  <si>
-    <t>ERCAN</t>
-  </si>
-  <si>
-    <t>TAILWIND</t>
-  </si>
-  <si>
-    <t>Burgas, Burgas Airport (BOJ)</t>
-  </si>
-  <si>
-    <t>Zakynthos, Zakinthos Is (ZTH)</t>
-  </si>
-  <si>
-    <t>Hurghada, Hurghada (HRG)</t>
-  </si>
-  <si>
-    <t>Marsa Alam, Marsa Alam (RMF)</t>
-  </si>
-  <si>
-    <t>Varna, Varna Airport (VAR)</t>
-  </si>
-  <si>
-    <t>Kos, Kos Island International Airport (KGS)</t>
-  </si>
-  <si>
-    <t>MONASTIR</t>
-  </si>
-  <si>
-    <t>BRATISLAVA</t>
-  </si>
-  <si>
-    <t>Djerba</t>
-  </si>
-  <si>
-    <t>KAVALA</t>
   </si>
   <si>
     <t>Warsawa</t>
@@ -1367,8 +1379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="D228" sqref="D228"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4288,7 +4300,7 @@
         <v>269</v>
       </c>
       <c r="D208" t="s">
-        <v>28</v>
+        <v>270</v>
       </c>
     </row>
     <row r="209">
@@ -4302,7 +4314,7 @@
         <v>269</v>
       </c>
       <c r="D209" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="210">
@@ -4310,13 +4322,13 @@
         <v>267</v>
       </c>
       <c r="B210" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C210" t="s">
         <v>269</v>
       </c>
       <c r="D210" t="s">
-        <v>274</v>
+        <v>99</v>
       </c>
     </row>
     <row r="211">
@@ -4324,13 +4336,13 @@
         <v>267</v>
       </c>
       <c r="B211" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C211" t="s">
         <v>269</v>
       </c>
       <c r="D211" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
     </row>
     <row r="212">
@@ -4358,7 +4370,7 @@
         <v>269</v>
       </c>
       <c r="D213" t="s">
-        <v>59</v>
+        <v>250</v>
       </c>
     </row>
     <row r="214">
@@ -4414,7 +4426,7 @@
         <v>269</v>
       </c>
       <c r="D217" t="s">
-        <v>250</v>
+        <v>28</v>
       </c>
     </row>
     <row r="218">
@@ -4470,7 +4482,7 @@
         <v>269</v>
       </c>
       <c r="D221" t="s">
-        <v>270</v>
+        <v>28</v>
       </c>
     </row>
     <row r="222">
@@ -4498,7 +4510,7 @@
         <v>269</v>
       </c>
       <c r="D223" t="s">
-        <v>28</v>
+        <v>270</v>
       </c>
     </row>
     <row r="224">
@@ -4540,7 +4552,7 @@
         <v>269</v>
       </c>
       <c r="D226" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
     </row>
     <row r="227">
@@ -4554,7 +4566,7 @@
         <v>269</v>
       </c>
       <c r="D227" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
     </row>
     <row r="228">
@@ -4582,7 +4594,7 @@
         <v>269</v>
       </c>
       <c r="D229" t="s">
-        <v>270</v>
+        <v>293</v>
       </c>
     </row>
     <row r="230">
@@ -4590,13 +4602,13 @@
         <v>267</v>
       </c>
       <c r="B230" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C230" t="s">
         <v>269</v>
       </c>
       <c r="D230" t="s">
-        <v>294</v>
+        <v>250</v>
       </c>
     </row>
     <row r="231">
@@ -4610,7 +4622,7 @@
         <v>269</v>
       </c>
       <c r="D231" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
     </row>
     <row r="232">
@@ -4680,7 +4692,7 @@
         <v>269</v>
       </c>
       <c r="D236" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="237">
@@ -4702,60 +4714,70 @@
         <v>189</v>
       </c>
       <c r="B238" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C238" t="s">
         <v>269</v>
       </c>
-      <c r="D238"/>
+      <c r="D238" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="s">
         <v>189</v>
       </c>
       <c r="B239" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C239" t="s">
         <v>269</v>
       </c>
-      <c r="D239"/>
+      <c r="D239" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="s">
         <v>189</v>
       </c>
       <c r="B240" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C240" t="s">
         <v>269</v>
       </c>
-      <c r="D240"/>
+      <c r="D240" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="s">
         <v>189</v>
       </c>
       <c r="B241" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C241" t="s">
         <v>269</v>
       </c>
-      <c r="D241"/>
+      <c r="D241" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="s">
         <v>189</v>
       </c>
       <c r="B242" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C242" t="s">
         <v>269</v>
       </c>
-      <c r="D242"/>
+      <c r="D242" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" t="s">
@@ -4768,7 +4790,7 @@
         <v>269</v>
       </c>
       <c r="D243" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
     </row>
     <row r="244">
@@ -4776,7 +4798,7 @@
         <v>189</v>
       </c>
       <c r="B244" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="C244" t="s">
         <v>269</v>
@@ -4790,49 +4812,55 @@
         <v>189</v>
       </c>
       <c r="B245" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="C245" t="s">
         <v>269</v>
       </c>
-      <c r="D245"/>
+      <c r="D245" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246" t="s">
         <v>189</v>
       </c>
       <c r="B246" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="C246" t="s">
         <v>269</v>
       </c>
-      <c r="D246"/>
+      <c r="D246" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="247">
       <c r="A247" t="s">
         <v>189</v>
       </c>
       <c r="B247" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="C247" t="s">
         <v>269</v>
       </c>
-      <c r="D247"/>
+      <c r="D247" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="s">
         <v>189</v>
       </c>
       <c r="B248" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="C248" t="s">
         <v>269</v>
       </c>
       <c r="D248" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="249">
@@ -4840,13 +4868,13 @@
         <v>189</v>
       </c>
       <c r="B249" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="C249" t="s">
         <v>269</v>
       </c>
       <c r="D249" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
     </row>
     <row r="250">
@@ -4854,13 +4882,13 @@
         <v>189</v>
       </c>
       <c r="B250" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="C250" t="s">
         <v>269</v>
       </c>
       <c r="D250" t="s">
-        <v>302</v>
+        <v>312</v>
       </c>
     </row>
     <row r="251">
@@ -4868,49 +4896,55 @@
         <v>189</v>
       </c>
       <c r="B251" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="C251" t="s">
         <v>269</v>
       </c>
-      <c r="D251"/>
+      <c r="D251" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252" t="s">
         <v>189</v>
       </c>
       <c r="B252" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="C252" t="s">
         <v>269</v>
       </c>
-      <c r="D252"/>
+      <c r="D252" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="253">
       <c r="A253" t="s">
         <v>189</v>
       </c>
       <c r="B253" t="s">
+        <v>303</v>
+      </c>
+      <c r="C253" t="s">
+        <v>269</v>
+      </c>
+      <c r="D253" t="s">
         <v>307</v>
       </c>
-      <c r="C253" t="s">
-        <v>269</v>
-      </c>
-      <c r="D253"/>
     </row>
     <row r="254">
       <c r="A254" t="s">
         <v>189</v>
       </c>
       <c r="B254" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="C254" t="s">
         <v>269</v>
       </c>
       <c r="D254" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="255">
@@ -4918,7 +4952,7 @@
         <v>189</v>
       </c>
       <c r="B255" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="C255" t="s">
         <v>269</v>
@@ -4932,61 +4966,69 @@
         <v>189</v>
       </c>
       <c r="B256" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="C256" t="s">
         <v>269</v>
       </c>
-      <c r="D256"/>
+      <c r="D256" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="257">
       <c r="A257" t="s">
         <v>189</v>
       </c>
       <c r="B257" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="C257" t="s">
         <v>269</v>
       </c>
-      <c r="D257"/>
+      <c r="D257" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="258">
       <c r="A258" t="s">
         <v>189</v>
       </c>
       <c r="B258" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="C258" t="s">
         <v>269</v>
       </c>
-      <c r="D258"/>
+      <c r="D258" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="259">
       <c r="A259" t="s">
         <v>189</v>
       </c>
       <c r="B259" t="s">
-        <v>307</v>
+        <v>318</v>
       </c>
       <c r="C259" t="s">
         <v>269</v>
       </c>
-      <c r="D259"/>
+      <c r="D259" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="260">
       <c r="A260" t="s">
         <v>189</v>
       </c>
       <c r="B260" t="s">
-        <v>309</v>
+        <v>319</v>
       </c>
       <c r="C260" t="s">
         <v>269</v>
       </c>
       <c r="D260" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
     </row>
     <row r="261">
@@ -4994,13 +5036,13 @@
         <v>189</v>
       </c>
       <c r="B261" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="C261" t="s">
         <v>269</v>
       </c>
       <c r="D261" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="262">
@@ -5008,13 +5050,13 @@
         <v>189</v>
       </c>
       <c r="B262" t="s">
-        <v>312</v>
+        <v>228</v>
       </c>
       <c r="C262" t="s">
         <v>269</v>
       </c>
       <c r="D262" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
     <row r="263">
@@ -5022,13 +5064,13 @@
         <v>189</v>
       </c>
       <c r="B263" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="C263" t="s">
         <v>269</v>
       </c>
       <c r="D263" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="264">
@@ -5036,13 +5078,13 @@
         <v>189</v>
       </c>
       <c r="B264" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="C264" t="s">
         <v>269</v>
       </c>
       <c r="D264" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
     </row>
     <row r="265">
@@ -5050,13 +5092,13 @@
         <v>189</v>
       </c>
       <c r="B265" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="C265" t="s">
         <v>269</v>
       </c>
       <c r="D265" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="266">
@@ -5064,13 +5106,13 @@
         <v>189</v>
       </c>
       <c r="B266" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="C266" t="s">
         <v>269</v>
       </c>
       <c r="D266" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="267">
@@ -5078,13 +5120,13 @@
         <v>189</v>
       </c>
       <c r="B267" t="s">
-        <v>308</v>
+        <v>318</v>
       </c>
       <c r="C267" t="s">
         <v>269</v>
       </c>
       <c r="D267" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="268">
@@ -5092,7 +5134,7 @@
         <v>189</v>
       </c>
       <c r="B268" t="s">
-        <v>228</v>
+        <v>323</v>
       </c>
       <c r="C268" t="s">
         <v>269</v>
@@ -5112,7 +5154,7 @@
         <v>269</v>
       </c>
       <c r="D269" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="270">
@@ -5120,7 +5162,7 @@
         <v>189</v>
       </c>
       <c r="B270" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
       <c r="C270" t="s">
         <v>269</v>
@@ -5134,13 +5176,13 @@
         <v>189</v>
       </c>
       <c r="B271" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="C271" t="s">
         <v>269</v>
       </c>
       <c r="D271" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="272">
@@ -5148,13 +5190,13 @@
         <v>189</v>
       </c>
       <c r="B272" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
       <c r="C272" t="s">
         <v>269</v>
       </c>
       <c r="D272" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="273">
@@ -5162,27 +5204,25 @@
         <v>189</v>
       </c>
       <c r="B273" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="C273" t="s">
         <v>269</v>
       </c>
-      <c r="D273" t="s">
-        <v>304</v>
-      </c>
+      <c r="D273"/>
     </row>
     <row r="274">
       <c r="A274" t="s">
         <v>189</v>
       </c>
       <c r="B274" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C274" t="s">
         <v>269</v>
       </c>
       <c r="D274" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="275">
@@ -5190,13 +5230,13 @@
         <v>189</v>
       </c>
       <c r="B275" t="s">
-        <v>301</v>
+        <v>326</v>
       </c>
       <c r="C275" t="s">
         <v>269</v>
       </c>
       <c r="D275" t="s">
-        <v>302</v>
+        <v>317</v>
       </c>
     </row>
     <row r="276">
@@ -5204,27 +5244,25 @@
         <v>189</v>
       </c>
       <c r="B276" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="C276" t="s">
         <v>269</v>
       </c>
-      <c r="D276" t="s">
-        <v>304</v>
-      </c>
+      <c r="D276"/>
     </row>
     <row r="277">
       <c r="A277" t="s">
         <v>189</v>
       </c>
       <c r="B277" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="C277" t="s">
         <v>269</v>
       </c>
       <c r="D277" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="278">
@@ -5232,25 +5270,27 @@
         <v>189</v>
       </c>
       <c r="B278" t="s">
-        <v>322</v>
+        <v>329</v>
       </c>
       <c r="C278" t="s">
         <v>269</v>
       </c>
-      <c r="D278"/>
+      <c r="D278" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="279">
       <c r="A279" t="s">
         <v>189</v>
       </c>
       <c r="B279" t="s">
-        <v>316</v>
+        <v>197</v>
       </c>
       <c r="C279" t="s">
         <v>269</v>
       </c>
       <c r="D279" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="280">
@@ -5258,13 +5298,13 @@
         <v>189</v>
       </c>
       <c r="B280" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="C280" t="s">
         <v>269</v>
       </c>
       <c r="D280" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
     </row>
     <row r="281">
@@ -5272,19 +5312,21 @@
         <v>189</v>
       </c>
       <c r="B281" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="C281" t="s">
         <v>269</v>
       </c>
-      <c r="D281"/>
+      <c r="D281" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="282">
       <c r="A282" t="s">
         <v>189</v>
       </c>
       <c r="B282" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="C282" t="s">
         <v>269</v>
@@ -5298,13 +5340,13 @@
         <v>189</v>
       </c>
       <c r="B283" t="s">
-        <v>197</v>
+        <v>330</v>
       </c>
       <c r="C283" t="s">
         <v>269</v>
       </c>
       <c r="D283" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="284">
@@ -5312,13 +5354,13 @@
         <v>189</v>
       </c>
       <c r="B284" t="s">
-        <v>316</v>
+        <v>330</v>
       </c>
       <c r="C284" t="s">
         <v>269</v>
       </c>
       <c r="D284" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="285">
@@ -5326,13 +5368,13 @@
         <v>189</v>
       </c>
       <c r="B285" t="s">
-        <v>316</v>
+        <v>330</v>
       </c>
       <c r="C285" t="s">
         <v>269</v>
       </c>
       <c r="D285" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="286">
@@ -5340,13 +5382,13 @@
         <v>189</v>
       </c>
       <c r="B286" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="C286" t="s">
         <v>269</v>
       </c>
       <c r="D286" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
     </row>
     <row r="287">
@@ -5354,75 +5396,27 @@
         <v>189</v>
       </c>
       <c r="B287" t="s">
-        <v>326</v>
+        <v>303</v>
       </c>
       <c r="C287" t="s">
         <v>269</v>
       </c>
-      <c r="D287"/>
+      <c r="D287" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="288">
       <c r="A288" t="s">
         <v>189</v>
       </c>
       <c r="B288" t="s">
-        <v>326</v>
+        <v>197</v>
       </c>
       <c r="C288" t="s">
         <v>269</v>
       </c>
-      <c r="D288"/>
-    </row>
-    <row r="289">
-      <c r="A289" t="s">
-        <v>189</v>
-      </c>
-      <c r="B289" t="s">
-        <v>326</v>
-      </c>
-      <c r="C289" t="s">
-        <v>269</v>
-      </c>
-      <c r="D289"/>
-    </row>
-    <row r="290">
-      <c r="A290" t="s">
-        <v>189</v>
-      </c>
-      <c r="B290" t="s">
-        <v>326</v>
-      </c>
-      <c r="C290" t="s">
-        <v>269</v>
-      </c>
-      <c r="D290"/>
-    </row>
-    <row r="291">
-      <c r="A291" t="s">
-        <v>189</v>
-      </c>
-      <c r="B291" t="s">
-        <v>301</v>
-      </c>
-      <c r="C291" t="s">
-        <v>269</v>
-      </c>
-      <c r="D291" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="292">
-      <c r="A292" t="s">
-        <v>189</v>
-      </c>
-      <c r="B292" t="s">
-        <v>197</v>
-      </c>
-      <c r="C292" t="s">
-        <v>269</v>
-      </c>
-      <c r="D292" t="s">
-        <v>304</v>
+      <c r="D288" t="s">
+        <v>302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ryanair done, Wizzair in progress
</commit_message>
<xml_diff>
--- a/src/data/flights.xlsx
+++ b/src/data/flights.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="266">
   <si>
     <t>From (City)</t>
   </si>
@@ -41,63 +41,63 @@
     <t>Prague</t>
   </si>
   <si>
+    <t>Denmark</t>
+  </si>
+  <si>
     <t>Aarhus</t>
   </si>
   <si>
-    <t>Denmark</t>
-  </si>
-  <si>
     <t>Czech Airlines (ČSA)</t>
   </si>
   <si>
+    <t>Italy</t>
+  </si>
+  <si>
     <t>Alghero</t>
   </si>
   <si>
-    <t>Italy</t>
-  </si>
-  <si>
     <t>SmartWings</t>
   </si>
   <si>
+    <t>Spain</t>
+  </si>
+  <si>
     <t>Almeria</t>
   </si>
   <si>
-    <t>Spain</t>
+    <t>Netherlands</t>
   </si>
   <si>
     <t>Amsterdam</t>
   </si>
   <si>
-    <t>Netherlands</t>
-  </si>
-  <si>
     <t>easyJet</t>
   </si>
   <si>
     <t>KLM</t>
   </si>
   <si>
+    <t>Turkey</t>
+  </si>
+  <si>
     <t>Antalya</t>
   </si>
   <si>
-    <t>Turkey</t>
+    <t>Greece</t>
   </si>
   <si>
     <t>Athens</t>
   </si>
   <si>
-    <t>Greece</t>
-  </si>
-  <si>
     <t>Aegean Airlines</t>
   </si>
   <si>
+    <t>Azerbaijan</t>
+  </si>
+  <si>
     <t>Baku</t>
   </si>
   <si>
-    <t>Azerbaijan</t>
-  </si>
-  <si>
     <t>Azerbaijan Airlines</t>
   </si>
   <si>
@@ -113,96 +113,96 @@
     <t>Wizz Air</t>
   </si>
   <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
     <t>Basel/Mulhouse</t>
   </si>
   <si>
-    <t>Switzerland</t>
+    <t>China</t>
   </si>
   <si>
     <t>Beijing</t>
   </si>
   <si>
-    <t>China</t>
-  </si>
-  <si>
     <t>Hainan Airlines</t>
   </si>
   <si>
+    <t>Lebanon</t>
+  </si>
+  <si>
     <t>Beirut</t>
   </si>
   <si>
-    <t>Lebanon</t>
+    <t>Serbia</t>
   </si>
   <si>
     <t>Belgrade</t>
   </si>
   <si>
-    <t>Serbia</t>
-  </si>
-  <si>
     <t>Air Serbia</t>
   </si>
   <si>
+    <t>Norway</t>
+  </si>
+  <si>
     <t>Bergen</t>
   </si>
   <si>
-    <t>Norway</t>
-  </si>
-  <si>
     <t>Norwegian</t>
   </si>
   <si>
+    <t>Germany</t>
+  </si>
+  <si>
     <t>Berlin/Tegel</t>
   </si>
   <si>
-    <t>Germany</t>
-  </si>
-  <si>
     <t>Air Berlin</t>
   </si>
   <si>
     <t>Bilbao</t>
   </si>
   <si>
+    <t>Great Britain</t>
+  </si>
+  <si>
     <t>Birmingham</t>
   </si>
   <si>
-    <t>Great Britain</t>
-  </si>
-  <si>
     <t>Bologna</t>
   </si>
   <si>
+    <t>France</t>
+  </si>
+  <si>
     <t>Bordeaux</t>
   </si>
   <si>
-    <t>France</t>
-  </si>
-  <si>
     <t>Volotea</t>
   </si>
   <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
     <t>Bourgas</t>
   </si>
   <si>
-    <t>Bulgaria</t>
+    <t>Slovakia</t>
   </si>
   <si>
     <t>Bratislava</t>
   </si>
   <si>
-    <t>Slovakia</t>
-  </si>
-  <si>
     <t>Bristol</t>
   </si>
   <si>
+    <t>Belgium</t>
+  </si>
+  <si>
     <t>Brussels/Charleroi</t>
   </si>
   <si>
-    <t>Belgium</t>
-  </si>
-  <si>
     <t>Ryanair</t>
   </si>
   <si>
@@ -212,21 +212,21 @@
     <t>Brussels Airlines</t>
   </si>
   <si>
+    <t>Romania</t>
+  </si>
+  <si>
     <t>Bucharest</t>
   </si>
   <si>
-    <t>Romania</t>
-  </si>
-  <si>
     <t>Tarom</t>
   </si>
   <si>
+    <t>Hungary</t>
+  </si>
+  <si>
     <t>Budapest</t>
   </si>
   <si>
-    <t>Hungary</t>
-  </si>
-  <si>
     <t>Cagliari</t>
   </si>
   <si>
@@ -260,33 +260,33 @@
     <t>Corfu</t>
   </si>
   <si>
+    <t>United Arab Emirates</t>
+  </si>
+  <si>
     <t>Dubai</t>
   </si>
   <si>
-    <t>United Arab Emirates</t>
-  </si>
-  <si>
     <t>flydubai</t>
   </si>
   <si>
     <t>Emirates</t>
   </si>
   <si>
+    <t>Ireland</t>
+  </si>
+  <si>
     <t>Dublin</t>
   </si>
   <si>
-    <t>Ireland</t>
-  </si>
-  <si>
     <t>Aer Lingus</t>
   </si>
   <si>
+    <t>Croatia</t>
+  </si>
+  <si>
     <t>Dubrovnik</t>
   </si>
   <si>
-    <t>Croatia</t>
-  </si>
-  <si>
     <t>Dusseldorf</t>
   </si>
   <si>
@@ -305,21 +305,21 @@
     <t>Transavia</t>
   </si>
   <si>
+    <t>Russia</t>
+  </si>
+  <si>
     <t>Ekaterinburg</t>
   </si>
   <si>
-    <t>Russia</t>
-  </si>
-  <si>
     <t>Ural Airlines</t>
   </si>
   <si>
+    <t>Portugal</t>
+  </si>
+  <si>
     <t>Faro</t>
   </si>
   <si>
-    <t>Portugal</t>
-  </si>
-  <si>
     <t>Frankfurt</t>
   </si>
   <si>
@@ -338,21 +338,21 @@
     <t>Glasgow</t>
   </si>
   <si>
+    <t>Sweden</t>
+  </si>
+  <si>
     <t>Gothenburg</t>
   </si>
   <si>
-    <t>Sweden</t>
-  </si>
-  <si>
     <t>Hamburg</t>
   </si>
   <si>
+    <t>Finland</t>
+  </si>
+  <si>
     <t>Helsinki</t>
   </si>
   <si>
-    <t>Finland</t>
-  </si>
-  <si>
     <t>Finnair</t>
   </si>
   <si>
@@ -362,12 +362,12 @@
     <t>Hévíz/Balaton</t>
   </si>
   <si>
+    <t>Egypt</t>
+  </si>
+  <si>
     <t>Hurghada</t>
   </si>
   <si>
-    <t>Egypt</t>
-  </si>
-  <si>
     <t>Air Cairo</t>
   </si>
   <si>
@@ -392,18 +392,18 @@
     <t>Kefallinia</t>
   </si>
   <si>
+    <t>Iceland</t>
+  </si>
+  <si>
     <t>Keflavik</t>
   </si>
   <si>
-    <t>Iceland</t>
+    <t>Ukraine</t>
   </si>
   <si>
     <t>Kiev/Borispol</t>
   </si>
   <si>
-    <t>Ukraine</t>
-  </si>
-  <si>
     <t>Ukraine International Airlines</t>
   </si>
   <si>
@@ -425,12 +425,12 @@
     <t>Lanzarote</t>
   </si>
   <si>
+    <t>Cyprus</t>
+  </si>
+  <si>
     <t>Larnaca</t>
   </si>
   <si>
-    <t>Cyprus</t>
-  </si>
-  <si>
     <t>Las Palmas</t>
   </si>
   <si>
@@ -449,12 +449,12 @@
     <t>Liverpool</t>
   </si>
   <si>
+    <t>Slovenia</t>
+  </si>
+  <si>
     <t>Ljubljana</t>
   </si>
   <si>
-    <t>Slovenia</t>
-  </si>
-  <si>
     <t>Adria Airways</t>
   </si>
   <si>
@@ -503,9 +503,6 @@
     <t>Malaga</t>
   </si>
   <si>
-    <t>Malmo/Sturup</t>
-  </si>
-  <si>
     <t>Malta</t>
   </si>
   <si>
@@ -530,21 +527,21 @@
     <t>Milan/Malpensa</t>
   </si>
   <si>
+    <t>Belarus</t>
+  </si>
+  <si>
     <t>Minsk</t>
   </si>
   <si>
-    <t>Belarus</t>
-  </si>
-  <si>
     <t>Belavia</t>
   </si>
   <si>
+    <t>Canada</t>
+  </si>
+  <si>
     <t>Montreal</t>
   </si>
   <si>
-    <t>Canada</t>
-  </si>
-  <si>
     <t>Air Transat</t>
   </si>
   <si>
@@ -563,12 +560,12 @@
     <t>Naples</t>
   </si>
   <si>
+    <t>USA</t>
+  </si>
+  <si>
     <t>New York/JFK</t>
   </si>
   <si>
-    <t>USA</t>
-  </si>
-  <si>
     <t>Delta Air Lines</t>
   </si>
   <si>
@@ -593,12 +590,12 @@
     <t>Oslo</t>
   </si>
   <si>
+    <t>Czech Republic</t>
+  </si>
+  <si>
     <t>Ostrava</t>
   </si>
   <si>
-    <t>Czech Republic</t>
-  </si>
-  <si>
     <t>Palma Mallorca</t>
   </si>
   <si>
@@ -617,24 +614,24 @@
     <t>Pisa</t>
   </si>
   <si>
+    <t>Monte Negro</t>
+  </si>
+  <si>
     <t>Podgorica</t>
   </si>
   <si>
-    <t>Monte Negro</t>
-  </si>
-  <si>
     <t>Porto</t>
   </si>
   <si>
     <t>Preveza</t>
   </si>
   <si>
+    <t>Poland</t>
+  </si>
+  <si>
     <t>Radom</t>
   </si>
   <si>
-    <t>Poland</t>
-  </si>
-  <si>
     <t>SprintAir</t>
   </si>
   <si>
@@ -644,21 +641,21 @@
     <t>Rhodes</t>
   </si>
   <si>
+    <t>Latvia</t>
+  </si>
+  <si>
     <t>Riga</t>
   </si>
   <si>
-    <t>Latvia</t>
-  </si>
-  <si>
     <t>Air Baltic</t>
   </si>
   <si>
+    <t>Saudi Arabia</t>
+  </si>
+  <si>
     <t>Riyadh</t>
   </si>
   <si>
-    <t>Saudi Arabia</t>
-  </si>
-  <si>
     <t>Rome/Ciampino</t>
   </si>
   <si>
@@ -677,12 +674,12 @@
     <t>Samos</t>
   </si>
   <si>
+    <t>South Korea</t>
+  </si>
+  <si>
     <t>Seoul/Incheon</t>
   </si>
   <si>
-    <t>South Korea</t>
-  </si>
-  <si>
     <t>Korean Air</t>
   </si>
   <si>
@@ -698,12 +695,12 @@
     <t>Sharm El Sheikh</t>
   </si>
   <si>
+    <t>Macedonia</t>
+  </si>
+  <si>
     <t>Skopje</t>
   </si>
   <si>
-    <t>Macedonia</t>
-  </si>
-  <si>
     <t>Sofia</t>
   </si>
   <si>
@@ -728,21 +725,21 @@
     <t>Strasbourg</t>
   </si>
   <si>
+    <t>Georgia</t>
+  </si>
+  <si>
     <t>Tbilisi</t>
   </si>
   <si>
-    <t>Georgia</t>
-  </si>
-  <si>
     <t>Georgian Airways</t>
   </si>
   <si>
+    <t>Israel</t>
+  </si>
+  <si>
     <t>Tel Aviv</t>
   </si>
   <si>
-    <t>Israel</t>
-  </si>
-  <si>
     <t>UP by El Al</t>
   </si>
   <si>
@@ -752,12 +749,12 @@
     <t>Thessaloniki</t>
   </si>
   <si>
+    <t>Albania</t>
+  </si>
+  <si>
     <t>Tirana</t>
   </si>
   <si>
-    <t>Albania</t>
-  </si>
-  <si>
     <t>Toronto</t>
   </si>
   <si>
@@ -770,12 +767,12 @@
     <t>Trapani</t>
   </si>
   <si>
+    <t>Tunisia</t>
+  </si>
+  <si>
     <t>Tunis</t>
   </si>
   <si>
-    <t>Tunisia</t>
-  </si>
-  <si>
     <t>Tunisair</t>
   </si>
   <si>
@@ -800,12 +797,12 @@
     <t>Verona</t>
   </si>
   <si>
+    <t>Austria</t>
+  </si>
+  <si>
     <t>Vienna</t>
   </si>
   <si>
-    <t>Austria</t>
-  </si>
-  <si>
     <t>Austrian Airlines</t>
   </si>
   <si>
@@ -825,198 +822,6 @@
   </si>
   <si>
     <t>Zurich</t>
-  </si>
-  <si>
-    <t>Brno</t>
-  </si>
-  <si>
-    <t>RHODOS</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Travel Service</t>
-  </si>
-  <si>
-    <t>HERAKLION</t>
-  </si>
-  <si>
-    <t>MUNICH</t>
-  </si>
-  <si>
-    <t>bmi regional</t>
-  </si>
-  <si>
-    <t>LONDON STANSTED</t>
-  </si>
-  <si>
-    <t>CORFU</t>
-  </si>
-  <si>
-    <t>ENFIDHA</t>
-  </si>
-  <si>
-    <t>ANTALYA</t>
-  </si>
-  <si>
-    <t>KOS</t>
-  </si>
-  <si>
-    <t>BURGAS</t>
-  </si>
-  <si>
-    <t>LONDON LUTON</t>
-  </si>
-  <si>
-    <t>ZAKYNTHOS</t>
-  </si>
-  <si>
-    <t>PREVEZA</t>
-  </si>
-  <si>
-    <t>HURGHADA</t>
-  </si>
-  <si>
-    <t>EINDHOVEN</t>
-  </si>
-  <si>
-    <t>PALMA DE MALLORCA</t>
-  </si>
-  <si>
-    <t>MARSA ALAM</t>
-  </si>
-  <si>
-    <t>VARNA / OSTRAVA</t>
-  </si>
-  <si>
-    <t>DJERBA / ENFIDHA</t>
-  </si>
-  <si>
-    <t>MONASTIR / OSTRAVA</t>
-  </si>
-  <si>
-    <t>LAMEZIA TERME</t>
-  </si>
-  <si>
-    <t>VARNA</t>
-  </si>
-  <si>
-    <t>ERCAN / ANTALYA</t>
-  </si>
-  <si>
-    <t>Tailwind Airlines</t>
-  </si>
-  <si>
-    <t>DJERBA / OSTRAVA</t>
-  </si>
-  <si>
-    <t>KAVALA / OSTRAVA</t>
-  </si>
-  <si>
-    <t>THESSALONIKI</t>
-  </si>
-  <si>
-    <t>PODGORICA</t>
-  </si>
-  <si>
-    <t>ALMERIA / OSTRAVA</t>
-  </si>
-  <si>
-    <t>TENERIFE</t>
-  </si>
-  <si>
-    <t>ANTALYA / BRATISLAVA</t>
-  </si>
-  <si>
-    <t>Rhodes, Diagoras Airport (RHO)</t>
-  </si>
-  <si>
-    <t>TRAVEL SERVICE / SMARTWINGS</t>
-  </si>
-  <si>
-    <t>Prague, Václav Havel Airport Prague (PRG)</t>
-  </si>
-  <si>
-    <t>CZECH AIRLINES (CSA)</t>
-  </si>
-  <si>
-    <t>KLM ROYAL DUTCH AIRLINES</t>
-  </si>
-  <si>
-    <t>DELTA AIR LINES</t>
-  </si>
-  <si>
-    <t>KOREAN AIR</t>
-  </si>
-  <si>
-    <t>TAROM ROMANIAN AIRLINES</t>
-  </si>
-  <si>
-    <t>Crete / Heraklion, N. Kazantzakis Apt. (HER)</t>
-  </si>
-  <si>
-    <t>Košice</t>
-  </si>
-  <si>
-    <t>Milan / Bergamo, Milan Bergamo Airport</t>
-  </si>
-  <si>
-    <t>RYANAIR</t>
-  </si>
-  <si>
-    <t>Corfu / Kerkyra, I. Kapodistrias (CFU)</t>
-  </si>
-  <si>
-    <t>London, Stansted (STN)</t>
-  </si>
-  <si>
-    <t>Antalya, Antayla (AYT)</t>
-  </si>
-  <si>
-    <t>ERCAN</t>
-  </si>
-  <si>
-    <t>TAILWIND</t>
-  </si>
-  <si>
-    <t>Burgas, Burgas Airport (BOJ)</t>
-  </si>
-  <si>
-    <t>Zakynthos, Zakinthos Is (ZTH)</t>
-  </si>
-  <si>
-    <t>Hurghada, Hurghada (HRG)</t>
-  </si>
-  <si>
-    <t>Mallorca, Palma de Mallorca (PMI)</t>
-  </si>
-  <si>
-    <t>Marsa Alam, Marsa Alam (RMF)</t>
-  </si>
-  <si>
-    <t>Varna, Varna Airport (VAR)</t>
-  </si>
-  <si>
-    <t>Kos, Kos Island International Airport (KGS)</t>
-  </si>
-  <si>
-    <t>MONASTIR</t>
-  </si>
-  <si>
-    <t>BRATISLAVA</t>
-  </si>
-  <si>
-    <t>Djerba</t>
-  </si>
-  <si>
-    <t>KAVALA</t>
-  </si>
-  <si>
-    <t>ALMERIA</t>
-  </si>
-  <si>
-    <t>Warsawa</t>
   </si>
 </sst>
 </file>
@@ -1380,7 +1185,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1536,10 +1341,10 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
         <v>25</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
@@ -1550,10 +1355,10 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
         <v>25</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
@@ -1564,10 +1369,10 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
         <v>25</v>
-      </c>
-      <c r="C13" t="s">
-        <v>12</v>
       </c>
       <c r="D13" t="s">
         <v>26</v>
@@ -1578,10 +1383,10 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
         <v>27</v>
-      </c>
-      <c r="C14" t="s">
-        <v>9</v>
       </c>
       <c r="D14" t="s">
         <v>28</v>
@@ -1676,10 +1481,10 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
         <v>45</v>
-      </c>
-      <c r="C21" t="s">
-        <v>12</v>
       </c>
       <c r="D21" t="s">
         <v>7</v>
@@ -1704,10 +1509,10 @@
         <v>4</v>
       </c>
       <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s">
         <v>48</v>
-      </c>
-      <c r="C23" t="s">
-        <v>9</v>
       </c>
       <c r="D23" t="s">
         <v>7</v>
@@ -1760,10 +1565,10 @@
         <v>4</v>
       </c>
       <c r="B27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" t="s">
         <v>56</v>
-      </c>
-      <c r="C27" t="s">
-        <v>47</v>
       </c>
       <c r="D27" t="s">
         <v>15</v>
@@ -1788,10 +1593,10 @@
         <v>4</v>
       </c>
       <c r="B29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" t="s">
         <v>60</v>
-      </c>
-      <c r="C29" t="s">
-        <v>58</v>
       </c>
       <c r="D29" t="s">
         <v>7</v>
@@ -1802,10 +1607,10 @@
         <v>4</v>
       </c>
       <c r="B30" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" t="s">
         <v>60</v>
-      </c>
-      <c r="C30" t="s">
-        <v>58</v>
       </c>
       <c r="D30" t="s">
         <v>61</v>
@@ -1858,10 +1663,10 @@
         <v>4</v>
       </c>
       <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" t="s">
         <v>67</v>
-      </c>
-      <c r="C34" t="s">
-        <v>9</v>
       </c>
       <c r="D34" t="s">
         <v>10</v>
@@ -1872,10 +1677,10 @@
         <v>4</v>
       </c>
       <c r="B35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" t="s">
         <v>68</v>
-      </c>
-      <c r="C35" t="s">
-        <v>9</v>
       </c>
       <c r="D35" t="s">
         <v>10</v>
@@ -1886,10 +1691,10 @@
         <v>4</v>
       </c>
       <c r="B36" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" t="s">
         <v>69</v>
-      </c>
-      <c r="C36" t="s">
-        <v>20</v>
       </c>
       <c r="D36" t="s">
         <v>10</v>
@@ -1900,10 +1705,10 @@
         <v>4</v>
       </c>
       <c r="B37" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" t="s">
         <v>70</v>
-      </c>
-      <c r="C37" t="s">
-        <v>32</v>
       </c>
       <c r="D37" t="s">
         <v>71</v>
@@ -1914,10 +1719,10 @@
         <v>4</v>
       </c>
       <c r="B38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" t="s">
         <v>72</v>
-      </c>
-      <c r="C38" t="s">
-        <v>43</v>
       </c>
       <c r="D38" t="s">
         <v>73</v>
@@ -1928,10 +1733,10 @@
         <v>4</v>
       </c>
       <c r="B39" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" t="s">
         <v>72</v>
-      </c>
-      <c r="C39" t="s">
-        <v>43</v>
       </c>
       <c r="D39" t="s">
         <v>74</v>
@@ -1942,10 +1747,10 @@
         <v>4</v>
       </c>
       <c r="B40" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" t="s">
         <v>75</v>
-      </c>
-      <c r="C40" t="s">
-        <v>6</v>
       </c>
       <c r="D40" t="s">
         <v>7</v>
@@ -1956,10 +1761,10 @@
         <v>4</v>
       </c>
       <c r="B41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" t="s">
         <v>75</v>
-      </c>
-      <c r="C41" t="s">
-        <v>6</v>
       </c>
       <c r="D41" t="s">
         <v>41</v>
@@ -1970,10 +1775,10 @@
         <v>4</v>
       </c>
       <c r="B42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" t="s">
         <v>75</v>
-      </c>
-      <c r="C42" t="s">
-        <v>6</v>
       </c>
       <c r="D42" t="s">
         <v>76</v>
@@ -1984,10 +1789,10 @@
         <v>4</v>
       </c>
       <c r="B43" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" t="s">
         <v>77</v>
-      </c>
-      <c r="C43" t="s">
-        <v>20</v>
       </c>
       <c r="D43" t="s">
         <v>10</v>
@@ -2082,10 +1887,10 @@
         <v>4</v>
       </c>
       <c r="B50" t="s">
+        <v>42</v>
+      </c>
+      <c r="C50" t="s">
         <v>87</v>
-      </c>
-      <c r="C50" t="s">
-        <v>43</v>
       </c>
       <c r="D50" t="s">
         <v>73</v>
@@ -2096,10 +1901,10 @@
         <v>4</v>
       </c>
       <c r="B51" t="s">
+        <v>42</v>
+      </c>
+      <c r="C51" t="s">
         <v>87</v>
-      </c>
-      <c r="C51" t="s">
-        <v>43</v>
       </c>
       <c r="D51" t="s">
         <v>7</v>
@@ -2110,10 +1915,10 @@
         <v>4</v>
       </c>
       <c r="B52" t="s">
+        <v>42</v>
+      </c>
+      <c r="C52" t="s">
         <v>87</v>
-      </c>
-      <c r="C52" t="s">
-        <v>43</v>
       </c>
       <c r="D52" t="s">
         <v>74</v>
@@ -2124,10 +1929,10 @@
         <v>4</v>
       </c>
       <c r="B53" t="s">
+        <v>46</v>
+      </c>
+      <c r="C53" t="s">
         <v>88</v>
-      </c>
-      <c r="C53" t="s">
-        <v>47</v>
       </c>
       <c r="D53" t="s">
         <v>89</v>
@@ -2138,10 +1943,10 @@
         <v>4</v>
       </c>
       <c r="B54" t="s">
+        <v>46</v>
+      </c>
+      <c r="C54" t="s">
         <v>90</v>
-      </c>
-      <c r="C54" t="s">
-        <v>47</v>
       </c>
       <c r="D54" t="s">
         <v>15</v>
@@ -2152,10 +1957,10 @@
         <v>4</v>
       </c>
       <c r="B55" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55" t="s">
         <v>91</v>
-      </c>
-      <c r="C55" t="s">
-        <v>14</v>
       </c>
       <c r="D55" t="s">
         <v>92</v>
@@ -2208,10 +2013,10 @@
         <v>4</v>
       </c>
       <c r="B59" t="s">
+        <v>42</v>
+      </c>
+      <c r="C59" t="s">
         <v>98</v>
-      </c>
-      <c r="C59" t="s">
-        <v>43</v>
       </c>
       <c r="D59" t="s">
         <v>7</v>
@@ -2222,10 +2027,10 @@
         <v>4</v>
       </c>
       <c r="B60" t="s">
+        <v>42</v>
+      </c>
+      <c r="C60" t="s">
         <v>98</v>
-      </c>
-      <c r="C60" t="s">
-        <v>43</v>
       </c>
       <c r="D60" t="s">
         <v>99</v>
@@ -2236,10 +2041,10 @@
         <v>4</v>
       </c>
       <c r="B61" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61" t="s">
         <v>100</v>
-      </c>
-      <c r="C61" t="s">
-        <v>12</v>
       </c>
       <c r="D61" t="s">
         <v>10</v>
@@ -2250,10 +2055,10 @@
         <v>4</v>
       </c>
       <c r="B62" t="s">
+        <v>29</v>
+      </c>
+      <c r="C62" t="s">
         <v>101</v>
-      </c>
-      <c r="C62" t="s">
-        <v>30</v>
       </c>
       <c r="D62" t="s">
         <v>102</v>
@@ -2264,10 +2069,10 @@
         <v>4</v>
       </c>
       <c r="B63" t="s">
+        <v>46</v>
+      </c>
+      <c r="C63" t="s">
         <v>103</v>
-      </c>
-      <c r="C63" t="s">
-        <v>47</v>
       </c>
       <c r="D63" t="s">
         <v>89</v>
@@ -2292,10 +2097,10 @@
         <v>4</v>
       </c>
       <c r="B65" t="s">
+        <v>42</v>
+      </c>
+      <c r="C65" t="s">
         <v>106</v>
-      </c>
-      <c r="C65" t="s">
-        <v>43</v>
       </c>
       <c r="D65" t="s">
         <v>73</v>
@@ -2306,10 +2111,10 @@
         <v>4</v>
       </c>
       <c r="B66" t="s">
+        <v>42</v>
+      </c>
+      <c r="C66" t="s">
         <v>106</v>
-      </c>
-      <c r="C66" t="s">
-        <v>43</v>
       </c>
       <c r="D66" t="s">
         <v>7</v>
@@ -2320,10 +2125,10 @@
         <v>4</v>
       </c>
       <c r="B67" t="s">
+        <v>42</v>
+      </c>
+      <c r="C67" t="s">
         <v>106</v>
-      </c>
-      <c r="C67" t="s">
-        <v>43</v>
       </c>
       <c r="D67" t="s">
         <v>74</v>
@@ -2376,10 +2181,10 @@
         <v>4</v>
       </c>
       <c r="B71" t="s">
+        <v>19</v>
+      </c>
+      <c r="C71" t="s">
         <v>110</v>
-      </c>
-      <c r="C71" t="s">
-        <v>20</v>
       </c>
       <c r="D71" t="s">
         <v>10</v>
@@ -2390,10 +2195,10 @@
         <v>4</v>
       </c>
       <c r="B72" t="s">
+        <v>65</v>
+      </c>
+      <c r="C72" t="s">
         <v>111</v>
-      </c>
-      <c r="C72" t="s">
-        <v>66</v>
       </c>
       <c r="D72" t="s">
         <v>7</v>
@@ -2432,10 +2237,10 @@
         <v>4</v>
       </c>
       <c r="B75" t="s">
+        <v>11</v>
+      </c>
+      <c r="C75" t="s">
         <v>115</v>
-      </c>
-      <c r="C75" t="s">
-        <v>12</v>
       </c>
       <c r="D75" t="s">
         <v>10</v>
@@ -2446,10 +2251,10 @@
         <v>4</v>
       </c>
       <c r="B76" t="s">
+        <v>17</v>
+      </c>
+      <c r="C76" t="s">
         <v>116</v>
-      </c>
-      <c r="C76" t="s">
-        <v>18</v>
       </c>
       <c r="D76" t="s">
         <v>117</v>
@@ -2460,10 +2265,10 @@
         <v>4</v>
       </c>
       <c r="B77" t="s">
+        <v>17</v>
+      </c>
+      <c r="C77" t="s">
         <v>118</v>
-      </c>
-      <c r="C77" t="s">
-        <v>18</v>
       </c>
       <c r="D77" t="s">
         <v>119</v>
@@ -2474,10 +2279,10 @@
         <v>4</v>
       </c>
       <c r="B78" t="s">
+        <v>93</v>
+      </c>
+      <c r="C78" t="s">
         <v>120</v>
-      </c>
-      <c r="C78" t="s">
-        <v>94</v>
       </c>
       <c r="D78" t="s">
         <v>7</v>
@@ -2488,10 +2293,10 @@
         <v>4</v>
       </c>
       <c r="B79" t="s">
+        <v>19</v>
+      </c>
+      <c r="C79" t="s">
         <v>121</v>
-      </c>
-      <c r="C79" t="s">
-        <v>20</v>
       </c>
       <c r="D79" t="s">
         <v>10</v>
@@ -2558,10 +2363,10 @@
         <v>4</v>
       </c>
       <c r="B84" t="s">
+        <v>19</v>
+      </c>
+      <c r="C84" t="s">
         <v>127</v>
-      </c>
-      <c r="C84" t="s">
-        <v>20</v>
       </c>
       <c r="D84" t="s">
         <v>10</v>
@@ -2572,10 +2377,10 @@
         <v>4</v>
       </c>
       <c r="B85" t="s">
+        <v>54</v>
+      </c>
+      <c r="C85" t="s">
         <v>128</v>
-      </c>
-      <c r="C85" t="s">
-        <v>55</v>
       </c>
       <c r="D85" t="s">
         <v>7</v>
@@ -2586,10 +2391,10 @@
         <v>4</v>
       </c>
       <c r="B86" t="s">
+        <v>93</v>
+      </c>
+      <c r="C86" t="s">
         <v>129</v>
-      </c>
-      <c r="C86" t="s">
-        <v>94</v>
       </c>
       <c r="D86" t="s">
         <v>130</v>
@@ -2600,10 +2405,10 @@
         <v>4</v>
       </c>
       <c r="B87" t="s">
+        <v>8</v>
+      </c>
+      <c r="C87" t="s">
         <v>131</v>
-      </c>
-      <c r="C87" t="s">
-        <v>9</v>
       </c>
       <c r="D87" t="s">
         <v>10</v>
@@ -2614,10 +2419,10 @@
         <v>4</v>
       </c>
       <c r="B88" t="s">
+        <v>11</v>
+      </c>
+      <c r="C88" t="s">
         <v>132</v>
-      </c>
-      <c r="C88" t="s">
-        <v>12</v>
       </c>
       <c r="D88" t="s">
         <v>10</v>
@@ -2642,10 +2447,10 @@
         <v>4</v>
       </c>
       <c r="B90" t="s">
+        <v>11</v>
+      </c>
+      <c r="C90" t="s">
         <v>135</v>
-      </c>
-      <c r="C90" t="s">
-        <v>12</v>
       </c>
       <c r="D90" t="s">
         <v>10</v>
@@ -2656,10 +2461,10 @@
         <v>4</v>
       </c>
       <c r="B91" t="s">
+        <v>46</v>
+      </c>
+      <c r="C91" t="s">
         <v>136</v>
-      </c>
-      <c r="C91" t="s">
-        <v>47</v>
       </c>
       <c r="D91" t="s">
         <v>89</v>
@@ -2670,10 +2475,10 @@
         <v>4</v>
       </c>
       <c r="B92" t="s">
+        <v>104</v>
+      </c>
+      <c r="C92" t="s">
         <v>137</v>
-      </c>
-      <c r="C92" t="s">
-        <v>105</v>
       </c>
       <c r="D92" t="s">
         <v>7</v>
@@ -2684,10 +2489,10 @@
         <v>4</v>
       </c>
       <c r="B93" t="s">
+        <v>96</v>
+      </c>
+      <c r="C93" t="s">
         <v>138</v>
-      </c>
-      <c r="C93" t="s">
-        <v>97</v>
       </c>
       <c r="D93" t="s">
         <v>7</v>
@@ -2698,10 +2503,10 @@
         <v>4</v>
       </c>
       <c r="B94" t="s">
+        <v>96</v>
+      </c>
+      <c r="C94" t="s">
         <v>138</v>
-      </c>
-      <c r="C94" t="s">
-        <v>97</v>
       </c>
       <c r="D94" t="s">
         <v>139</v>
@@ -2712,10 +2517,10 @@
         <v>4</v>
       </c>
       <c r="B95" t="s">
+        <v>46</v>
+      </c>
+      <c r="C95" t="s">
         <v>140</v>
-      </c>
-      <c r="C95" t="s">
-        <v>47</v>
       </c>
       <c r="D95" t="s">
         <v>59</v>
@@ -2740,10 +2545,10 @@
         <v>4</v>
       </c>
       <c r="B97" t="s">
+        <v>46</v>
+      </c>
+      <c r="C97" t="s">
         <v>144</v>
-      </c>
-      <c r="C97" t="s">
-        <v>47</v>
       </c>
       <c r="D97" t="s">
         <v>10</v>
@@ -2754,10 +2559,10 @@
         <v>4</v>
       </c>
       <c r="B98" t="s">
+        <v>46</v>
+      </c>
+      <c r="C98" t="s">
         <v>144</v>
-      </c>
-      <c r="C98" t="s">
-        <v>47</v>
       </c>
       <c r="D98" t="s">
         <v>15</v>
@@ -2768,10 +2573,10 @@
         <v>4</v>
       </c>
       <c r="B99" t="s">
+        <v>46</v>
+      </c>
+      <c r="C99" t="s">
         <v>145</v>
-      </c>
-      <c r="C99" t="s">
-        <v>47</v>
       </c>
       <c r="D99" t="s">
         <v>146</v>
@@ -2782,10 +2587,10 @@
         <v>4</v>
       </c>
       <c r="B100" t="s">
+        <v>46</v>
+      </c>
+      <c r="C100" t="s">
         <v>147</v>
-      </c>
-      <c r="C100" t="s">
-        <v>47</v>
       </c>
       <c r="D100" t="s">
         <v>28</v>
@@ -2796,10 +2601,10 @@
         <v>4</v>
       </c>
       <c r="B101" t="s">
+        <v>46</v>
+      </c>
+      <c r="C101" t="s">
         <v>148</v>
-      </c>
-      <c r="C101" t="s">
-        <v>47</v>
       </c>
       <c r="D101" t="s">
         <v>149</v>
@@ -2810,10 +2615,10 @@
         <v>4</v>
       </c>
       <c r="B102" t="s">
+        <v>46</v>
+      </c>
+      <c r="C102" t="s">
         <v>150</v>
-      </c>
-      <c r="C102" t="s">
-        <v>47</v>
       </c>
       <c r="D102" t="s">
         <v>59</v>
@@ -2824,10 +2629,10 @@
         <v>4</v>
       </c>
       <c r="B103" t="s">
+        <v>46</v>
+      </c>
+      <c r="C103" t="s">
         <v>150</v>
-      </c>
-      <c r="C103" t="s">
-        <v>47</v>
       </c>
       <c r="D103" t="s">
         <v>15</v>
@@ -2852,10 +2657,10 @@
         <v>4</v>
       </c>
       <c r="B105" t="s">
+        <v>49</v>
+      </c>
+      <c r="C105" t="s">
         <v>153</v>
-      </c>
-      <c r="C105" t="s">
-        <v>50</v>
       </c>
       <c r="D105" t="s">
         <v>154</v>
@@ -2866,10 +2671,10 @@
         <v>4</v>
       </c>
       <c r="B106" t="s">
+        <v>96</v>
+      </c>
+      <c r="C106" t="s">
         <v>155</v>
-      </c>
-      <c r="C106" t="s">
-        <v>97</v>
       </c>
       <c r="D106" t="s">
         <v>10</v>
@@ -2880,10 +2685,10 @@
         <v>4</v>
       </c>
       <c r="B107" t="s">
+        <v>11</v>
+      </c>
+      <c r="C107" t="s">
         <v>156</v>
-      </c>
-      <c r="C107" t="s">
-        <v>12</v>
       </c>
       <c r="D107" t="s">
         <v>7</v>
@@ -2894,10 +2699,10 @@
         <v>4</v>
       </c>
       <c r="B108" t="s">
+        <v>11</v>
+      </c>
+      <c r="C108" t="s">
         <v>156</v>
-      </c>
-      <c r="C108" t="s">
-        <v>12</v>
       </c>
       <c r="D108" t="s">
         <v>157</v>
@@ -2908,10 +2713,10 @@
         <v>4</v>
       </c>
       <c r="B109" t="s">
+        <v>11</v>
+      </c>
+      <c r="C109" t="s">
         <v>158</v>
-      </c>
-      <c r="C109" t="s">
-        <v>12</v>
       </c>
       <c r="D109" t="s">
         <v>10</v>
@@ -2925,7 +2730,7 @@
         <v>159</v>
       </c>
       <c r="C110" t="s">
-        <v>105</v>
+        <v>159</v>
       </c>
       <c r="D110" t="s">
         <v>7</v>
@@ -2936,13 +2741,13 @@
         <v>4</v>
       </c>
       <c r="B111" t="s">
+        <v>159</v>
+      </c>
+      <c r="C111" t="s">
+        <v>159</v>
+      </c>
+      <c r="D111" t="s">
         <v>160</v>
-      </c>
-      <c r="C111" t="s">
-        <v>160</v>
-      </c>
-      <c r="D111" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="112">
@@ -2950,13 +2755,13 @@
         <v>4</v>
       </c>
       <c r="B112" t="s">
-        <v>160</v>
+        <v>46</v>
       </c>
       <c r="C112" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D112" t="s">
-        <v>161</v>
+        <v>15</v>
       </c>
     </row>
     <row r="113">
@@ -2964,13 +2769,13 @@
         <v>4</v>
       </c>
       <c r="B113" t="s">
-        <v>162</v>
+        <v>46</v>
       </c>
       <c r="C113" t="s">
-        <v>47</v>
+        <v>161</v>
       </c>
       <c r="D113" t="s">
-        <v>15</v>
+        <v>89</v>
       </c>
     </row>
     <row r="114">
@@ -2978,13 +2783,13 @@
         <v>4</v>
       </c>
       <c r="B114" t="s">
+        <v>112</v>
+      </c>
+      <c r="C114" t="s">
         <v>162</v>
       </c>
-      <c r="C114" t="s">
-        <v>47</v>
-      </c>
       <c r="D114" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
     </row>
     <row r="115">
@@ -2992,13 +2797,13 @@
         <v>4</v>
       </c>
       <c r="B115" t="s">
-        <v>163</v>
+        <v>112</v>
       </c>
       <c r="C115" t="s">
-        <v>113</v>
+        <v>162</v>
       </c>
       <c r="D115" t="s">
-        <v>114</v>
+        <v>10</v>
       </c>
     </row>
     <row r="116">
@@ -3006,13 +2811,13 @@
         <v>4</v>
       </c>
       <c r="B116" t="s">
+        <v>49</v>
+      </c>
+      <c r="C116" t="s">
         <v>163</v>
       </c>
-      <c r="C116" t="s">
-        <v>113</v>
-      </c>
       <c r="D116" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="117">
@@ -3020,13 +2825,13 @@
         <v>4</v>
       </c>
       <c r="B117" t="s">
+        <v>11</v>
+      </c>
+      <c r="C117" t="s">
         <v>164</v>
       </c>
-      <c r="C117" t="s">
-        <v>50</v>
-      </c>
       <c r="D117" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
     </row>
     <row r="118">
@@ -3034,13 +2839,13 @@
         <v>4</v>
       </c>
       <c r="B118" t="s">
+        <v>8</v>
+      </c>
+      <c r="C118" t="s">
         <v>165</v>
       </c>
-      <c r="C118" t="s">
-        <v>12</v>
-      </c>
       <c r="D118" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
     </row>
     <row r="119">
@@ -3048,13 +2853,13 @@
         <v>4</v>
       </c>
       <c r="B119" t="s">
-        <v>166</v>
+        <v>8</v>
       </c>
       <c r="C119" t="s">
-        <v>9</v>
+        <v>165</v>
       </c>
       <c r="D119" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
     </row>
     <row r="120">
@@ -3062,13 +2867,13 @@
         <v>4</v>
       </c>
       <c r="B120" t="s">
+        <v>8</v>
+      </c>
+      <c r="C120" t="s">
         <v>166</v>
       </c>
-      <c r="C120" t="s">
-        <v>9</v>
-      </c>
       <c r="D120" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="121">
@@ -3076,13 +2881,13 @@
         <v>4</v>
       </c>
       <c r="B121" t="s">
-        <v>167</v>
+        <v>8</v>
       </c>
       <c r="C121" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D121" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="122">
@@ -3093,10 +2898,10 @@
         <v>167</v>
       </c>
       <c r="C122" t="s">
-        <v>9</v>
+        <v>168</v>
       </c>
       <c r="D122" t="s">
-        <v>15</v>
+        <v>169</v>
       </c>
     </row>
     <row r="123">
@@ -3104,13 +2909,13 @@
         <v>4</v>
       </c>
       <c r="B123" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C123" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D123" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="124">
@@ -3118,13 +2923,13 @@
         <v>4</v>
       </c>
       <c r="B124" t="s">
-        <v>171</v>
+        <v>93</v>
       </c>
       <c r="C124" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D124" t="s">
-        <v>173</v>
+        <v>7</v>
       </c>
     </row>
     <row r="125">
@@ -3132,13 +2937,13 @@
         <v>4</v>
       </c>
       <c r="B125" t="s">
-        <v>174</v>
+        <v>93</v>
       </c>
       <c r="C125" t="s">
-        <v>94</v>
+        <v>173</v>
       </c>
       <c r="D125" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="126">
@@ -3146,13 +2951,13 @@
         <v>4</v>
       </c>
       <c r="B126" t="s">
+        <v>93</v>
+      </c>
+      <c r="C126" t="s">
+        <v>173</v>
+      </c>
+      <c r="D126" t="s">
         <v>174</v>
-      </c>
-      <c r="C126" t="s">
-        <v>94</v>
-      </c>
-      <c r="D126" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="127">
@@ -3160,13 +2965,13 @@
         <v>4</v>
       </c>
       <c r="B127" t="s">
-        <v>174</v>
+        <v>42</v>
       </c>
       <c r="C127" t="s">
-        <v>94</v>
+        <v>175</v>
       </c>
       <c r="D127" t="s">
-        <v>175</v>
+        <v>99</v>
       </c>
     </row>
     <row r="128">
@@ -3174,13 +2979,13 @@
         <v>4</v>
       </c>
       <c r="B128" t="s">
+        <v>49</v>
+      </c>
+      <c r="C128" t="s">
         <v>176</v>
       </c>
-      <c r="C128" t="s">
-        <v>43</v>
-      </c>
       <c r="D128" t="s">
-        <v>99</v>
+        <v>51</v>
       </c>
     </row>
     <row r="129">
@@ -3188,13 +2993,13 @@
         <v>4</v>
       </c>
       <c r="B129" t="s">
+        <v>8</v>
+      </c>
+      <c r="C129" t="s">
         <v>177</v>
       </c>
-      <c r="C129" t="s">
-        <v>50</v>
-      </c>
       <c r="D129" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
     </row>
     <row r="130">
@@ -3202,13 +3007,13 @@
         <v>4</v>
       </c>
       <c r="B130" t="s">
-        <v>178</v>
+        <v>8</v>
       </c>
       <c r="C130" t="s">
-        <v>9</v>
+        <v>177</v>
       </c>
       <c r="D130" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="131">
@@ -3216,13 +3021,13 @@
         <v>4</v>
       </c>
       <c r="B131" t="s">
-        <v>178</v>
+        <v>8</v>
       </c>
       <c r="C131" t="s">
-        <v>9</v>
+        <v>177</v>
       </c>
       <c r="D131" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="132">
@@ -3233,10 +3038,10 @@
         <v>178</v>
       </c>
       <c r="C132" t="s">
-        <v>9</v>
+        <v>179</v>
       </c>
       <c r="D132" t="s">
-        <v>28</v>
+        <v>180</v>
       </c>
     </row>
     <row r="133">
@@ -3244,13 +3049,13 @@
         <v>4</v>
       </c>
       <c r="B133" t="s">
-        <v>179</v>
+        <v>46</v>
       </c>
       <c r="C133" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D133" t="s">
-        <v>181</v>
+        <v>89</v>
       </c>
     </row>
     <row r="134">
@@ -3258,13 +3063,13 @@
         <v>4</v>
       </c>
       <c r="B134" t="s">
+        <v>49</v>
+      </c>
+      <c r="C134" t="s">
         <v>182</v>
       </c>
-      <c r="C134" t="s">
-        <v>47</v>
-      </c>
       <c r="D134" t="s">
-        <v>89</v>
+        <v>7</v>
       </c>
     </row>
     <row r="135">
@@ -3272,13 +3077,13 @@
         <v>4</v>
       </c>
       <c r="B135" t="s">
+        <v>93</v>
+      </c>
+      <c r="C135" t="s">
         <v>183</v>
       </c>
-      <c r="C135" t="s">
-        <v>50</v>
-      </c>
       <c r="D135" t="s">
-        <v>7</v>
+        <v>184</v>
       </c>
     </row>
     <row r="136">
@@ -3286,13 +3091,13 @@
         <v>4</v>
       </c>
       <c r="B136" t="s">
-        <v>184</v>
+        <v>124</v>
       </c>
       <c r="C136" t="s">
-        <v>94</v>
+        <v>185</v>
       </c>
       <c r="D136" t="s">
-        <v>185</v>
+        <v>7</v>
       </c>
     </row>
     <row r="137">
@@ -3300,13 +3105,13 @@
         <v>4</v>
       </c>
       <c r="B137" t="s">
+        <v>8</v>
+      </c>
+      <c r="C137" t="s">
         <v>186</v>
       </c>
-      <c r="C137" t="s">
-        <v>125</v>
-      </c>
       <c r="D137" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="138">
@@ -3314,13 +3119,13 @@
         <v>4</v>
       </c>
       <c r="B138" t="s">
+        <v>39</v>
+      </c>
+      <c r="C138" t="s">
         <v>187</v>
       </c>
-      <c r="C138" t="s">
-        <v>9</v>
-      </c>
       <c r="D138" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
     </row>
     <row r="139">
@@ -3331,10 +3136,10 @@
         <v>188</v>
       </c>
       <c r="C139" t="s">
-        <v>40</v>
+        <v>189</v>
       </c>
       <c r="D139" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
     </row>
     <row r="140">
@@ -3342,13 +3147,13 @@
         <v>4</v>
       </c>
       <c r="B140" t="s">
-        <v>189</v>
+        <v>11</v>
       </c>
       <c r="C140" t="s">
         <v>190</v>
       </c>
       <c r="D140" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="141">
@@ -3356,13 +3161,13 @@
         <v>4</v>
       </c>
       <c r="B141" t="s">
+        <v>49</v>
+      </c>
+      <c r="C141" t="s">
         <v>191</v>
       </c>
-      <c r="C141" t="s">
-        <v>12</v>
-      </c>
       <c r="D141" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="142">
@@ -3370,13 +3175,13 @@
         <v>4</v>
       </c>
       <c r="B142" t="s">
-        <v>192</v>
+        <v>49</v>
       </c>
       <c r="C142" t="s">
-        <v>50</v>
+        <v>191</v>
       </c>
       <c r="D142" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="143">
@@ -3384,13 +3189,13 @@
         <v>4</v>
       </c>
       <c r="B143" t="s">
+        <v>49</v>
+      </c>
+      <c r="C143" t="s">
+        <v>191</v>
+      </c>
+      <c r="D143" t="s">
         <v>192</v>
-      </c>
-      <c r="C143" t="s">
-        <v>50</v>
-      </c>
-      <c r="D143" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="144">
@@ -3398,13 +3203,13 @@
         <v>4</v>
       </c>
       <c r="B144" t="s">
-        <v>192</v>
+        <v>49</v>
       </c>
       <c r="C144" t="s">
-        <v>50</v>
+        <v>191</v>
       </c>
       <c r="D144" t="s">
-        <v>193</v>
+        <v>26</v>
       </c>
     </row>
     <row r="145">
@@ -3412,13 +3217,13 @@
         <v>4</v>
       </c>
       <c r="B145" t="s">
-        <v>192</v>
+        <v>49</v>
       </c>
       <c r="C145" t="s">
-        <v>50</v>
+        <v>193</v>
       </c>
       <c r="D145" t="s">
-        <v>26</v>
+        <v>194</v>
       </c>
     </row>
     <row r="146">
@@ -3426,13 +3231,13 @@
         <v>4</v>
       </c>
       <c r="B146" t="s">
-        <v>194</v>
+        <v>8</v>
       </c>
       <c r="C146" t="s">
-        <v>50</v>
+        <v>195</v>
       </c>
       <c r="D146" t="s">
-        <v>195</v>
+        <v>7</v>
       </c>
     </row>
     <row r="147">
@@ -3443,10 +3248,10 @@
         <v>196</v>
       </c>
       <c r="C147" t="s">
-        <v>9</v>
+        <v>197</v>
       </c>
       <c r="D147" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="148">
@@ -3454,13 +3259,13 @@
         <v>4</v>
       </c>
       <c r="B148" t="s">
-        <v>197</v>
+        <v>96</v>
       </c>
       <c r="C148" t="s">
         <v>198</v>
       </c>
       <c r="D148" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="149">
@@ -3468,13 +3273,13 @@
         <v>4</v>
       </c>
       <c r="B149" t="s">
+        <v>19</v>
+      </c>
+      <c r="C149" t="s">
         <v>199</v>
       </c>
-      <c r="C149" t="s">
-        <v>97</v>
-      </c>
       <c r="D149" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="150">
@@ -3485,10 +3290,10 @@
         <v>200</v>
       </c>
       <c r="C150" t="s">
-        <v>20</v>
+        <v>201</v>
       </c>
       <c r="D150" t="s">
-        <v>10</v>
+        <v>202</v>
       </c>
     </row>
     <row r="151">
@@ -3496,13 +3301,13 @@
         <v>4</v>
       </c>
       <c r="B151" t="s">
-        <v>201</v>
+        <v>78</v>
       </c>
       <c r="C151" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D151" t="s">
-        <v>203</v>
+        <v>10</v>
       </c>
     </row>
     <row r="152">
@@ -3510,10 +3315,10 @@
         <v>4</v>
       </c>
       <c r="B152" t="s">
+        <v>19</v>
+      </c>
+      <c r="C152" t="s">
         <v>204</v>
-      </c>
-      <c r="C152" t="s">
-        <v>79</v>
       </c>
       <c r="D152" t="s">
         <v>10</v>
@@ -3527,10 +3332,10 @@
         <v>205</v>
       </c>
       <c r="C153" t="s">
-        <v>20</v>
+        <v>206</v>
       </c>
       <c r="D153" t="s">
-        <v>10</v>
+        <v>207</v>
       </c>
     </row>
     <row r="154">
@@ -3538,13 +3343,13 @@
         <v>4</v>
       </c>
       <c r="B154" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C154" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D154" t="s">
-        <v>208</v>
+        <v>7</v>
       </c>
     </row>
     <row r="155">
@@ -3552,13 +3357,13 @@
         <v>4</v>
       </c>
       <c r="B155" t="s">
-        <v>209</v>
+        <v>8</v>
       </c>
       <c r="C155" t="s">
         <v>210</v>
       </c>
       <c r="D155" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
     </row>
     <row r="156">
@@ -3566,13 +3371,13 @@
         <v>4</v>
       </c>
       <c r="B156" t="s">
+        <v>8</v>
+      </c>
+      <c r="C156" t="s">
         <v>211</v>
       </c>
-      <c r="C156" t="s">
-        <v>9</v>
-      </c>
       <c r="D156" t="s">
-        <v>59</v>
+        <v>7</v>
       </c>
     </row>
     <row r="157">
@@ -3580,13 +3385,13 @@
         <v>4</v>
       </c>
       <c r="B157" t="s">
-        <v>212</v>
+        <v>8</v>
       </c>
       <c r="C157" t="s">
-        <v>9</v>
+        <v>211</v>
       </c>
       <c r="D157" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
     </row>
     <row r="158">
@@ -3594,13 +3399,13 @@
         <v>4</v>
       </c>
       <c r="B158" t="s">
+        <v>8</v>
+      </c>
+      <c r="C158" t="s">
+        <v>211</v>
+      </c>
+      <c r="D158" t="s">
         <v>212</v>
-      </c>
-      <c r="C158" t="s">
-        <v>9</v>
-      </c>
-      <c r="D158" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="159">
@@ -3608,13 +3413,13 @@
         <v>4</v>
       </c>
       <c r="B159" t="s">
-        <v>212</v>
+        <v>93</v>
       </c>
       <c r="C159" t="s">
-        <v>9</v>
+        <v>213</v>
       </c>
       <c r="D159" t="s">
-        <v>213</v>
+        <v>7</v>
       </c>
     </row>
     <row r="160">
@@ -3622,10 +3427,10 @@
         <v>4</v>
       </c>
       <c r="B160" t="s">
+        <v>93</v>
+      </c>
+      <c r="C160" t="s">
         <v>214</v>
-      </c>
-      <c r="C160" t="s">
-        <v>94</v>
       </c>
       <c r="D160" t="s">
         <v>7</v>
@@ -3636,13 +3441,13 @@
         <v>4</v>
       </c>
       <c r="B161" t="s">
+        <v>19</v>
+      </c>
+      <c r="C161" t="s">
         <v>215</v>
       </c>
-      <c r="C161" t="s">
-        <v>94</v>
-      </c>
       <c r="D161" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="162">
@@ -3653,10 +3458,10 @@
         <v>216</v>
       </c>
       <c r="C162" t="s">
-        <v>20</v>
+        <v>217</v>
       </c>
       <c r="D162" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="163">
@@ -3664,13 +3469,13 @@
         <v>4</v>
       </c>
       <c r="B163" t="s">
+        <v>216</v>
+      </c>
+      <c r="C163" t="s">
         <v>217</v>
       </c>
-      <c r="C163" t="s">
+      <c r="D163" t="s">
         <v>218</v>
-      </c>
-      <c r="D163" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="164">
@@ -3678,13 +3483,13 @@
         <v>4</v>
       </c>
       <c r="B164" t="s">
-        <v>217</v>
+        <v>11</v>
       </c>
       <c r="C164" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D164" t="s">
-        <v>219</v>
+        <v>10</v>
       </c>
     </row>
     <row r="165">
@@ -3692,13 +3497,13 @@
         <v>4</v>
       </c>
       <c r="B165" t="s">
+        <v>31</v>
+      </c>
+      <c r="C165" t="s">
         <v>220</v>
       </c>
-      <c r="C165" t="s">
-        <v>12</v>
-      </c>
       <c r="D165" t="s">
-        <v>10</v>
+        <v>221</v>
       </c>
     </row>
     <row r="166">
@@ -3706,13 +3511,13 @@
         <v>4</v>
       </c>
       <c r="B166" t="s">
-        <v>221</v>
+        <v>112</v>
       </c>
       <c r="C166" t="s">
-        <v>32</v>
+        <v>222</v>
       </c>
       <c r="D166" t="s">
-        <v>222</v>
+        <v>114</v>
       </c>
     </row>
     <row r="167">
@@ -3723,10 +3528,10 @@
         <v>223</v>
       </c>
       <c r="C167" t="s">
-        <v>113</v>
+        <v>224</v>
       </c>
       <c r="D167" t="s">
-        <v>114</v>
+        <v>7</v>
       </c>
     </row>
     <row r="168">
@@ -3734,13 +3539,13 @@
         <v>4</v>
       </c>
       <c r="B168" t="s">
-        <v>224</v>
+        <v>52</v>
       </c>
       <c r="C168" t="s">
         <v>225</v>
       </c>
       <c r="D168" t="s">
-        <v>7</v>
+        <v>226</v>
       </c>
     </row>
     <row r="169">
@@ -3748,13 +3553,13 @@
         <v>4</v>
       </c>
       <c r="B169" t="s">
-        <v>226</v>
+        <v>85</v>
       </c>
       <c r="C169" t="s">
-        <v>53</v>
+        <v>227</v>
       </c>
       <c r="D169" t="s">
-        <v>227</v>
+        <v>10</v>
       </c>
     </row>
     <row r="170">
@@ -3762,13 +3567,13 @@
         <v>4</v>
       </c>
       <c r="B170" t="s">
+        <v>93</v>
+      </c>
+      <c r="C170" t="s">
         <v>228</v>
       </c>
-      <c r="C170" t="s">
-        <v>86</v>
-      </c>
       <c r="D170" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="171">
@@ -3776,13 +3581,13 @@
         <v>4</v>
       </c>
       <c r="B171" t="s">
+        <v>93</v>
+      </c>
+      <c r="C171" t="s">
+        <v>228</v>
+      </c>
+      <c r="D171" t="s">
         <v>229</v>
-      </c>
-      <c r="C171" t="s">
-        <v>94</v>
-      </c>
-      <c r="D171" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="172">
@@ -3790,13 +3595,13 @@
         <v>4</v>
       </c>
       <c r="B172" t="s">
-        <v>229</v>
+        <v>39</v>
       </c>
       <c r="C172" t="s">
-        <v>94</v>
+        <v>230</v>
       </c>
       <c r="D172" t="s">
-        <v>230</v>
+        <v>41</v>
       </c>
     </row>
     <row r="173">
@@ -3804,13 +3609,13 @@
         <v>4</v>
       </c>
       <c r="B173" t="s">
+        <v>104</v>
+      </c>
+      <c r="C173" t="s">
         <v>231</v>
       </c>
-      <c r="C173" t="s">
-        <v>40</v>
-      </c>
       <c r="D173" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
     </row>
     <row r="174">
@@ -3818,13 +3623,13 @@
         <v>4</v>
       </c>
       <c r="B174" t="s">
-        <v>232</v>
+        <v>104</v>
       </c>
       <c r="C174" t="s">
-        <v>105</v>
+        <v>231</v>
       </c>
       <c r="D174" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
     </row>
     <row r="175">
@@ -3832,13 +3637,13 @@
         <v>4</v>
       </c>
       <c r="B175" t="s">
-        <v>232</v>
+        <v>104</v>
       </c>
       <c r="C175" t="s">
-        <v>105</v>
+        <v>231</v>
       </c>
       <c r="D175" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
     </row>
     <row r="176">
@@ -3846,13 +3651,13 @@
         <v>4</v>
       </c>
       <c r="B176" t="s">
+        <v>49</v>
+      </c>
+      <c r="C176" t="s">
         <v>232</v>
       </c>
-      <c r="C176" t="s">
-        <v>105</v>
-      </c>
       <c r="D176" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
     </row>
     <row r="177">
@@ -3863,10 +3668,10 @@
         <v>233</v>
       </c>
       <c r="C177" t="s">
-        <v>50</v>
+        <v>234</v>
       </c>
       <c r="D177" t="s">
-        <v>7</v>
+        <v>235</v>
       </c>
     </row>
     <row r="178">
@@ -3874,13 +3679,13 @@
         <v>4</v>
       </c>
       <c r="B178" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C178" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D178" t="s">
-        <v>236</v>
+        <v>10</v>
       </c>
     </row>
     <row r="179">
@@ -3888,13 +3693,13 @@
         <v>4</v>
       </c>
       <c r="B179" t="s">
+        <v>236</v>
+      </c>
+      <c r="C179" t="s">
         <v>237</v>
       </c>
-      <c r="C179" t="s">
-        <v>238</v>
-      </c>
       <c r="D179" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="180">
@@ -3902,13 +3707,13 @@
         <v>4</v>
       </c>
       <c r="B180" t="s">
+        <v>236</v>
+      </c>
+      <c r="C180" t="s">
         <v>237</v>
       </c>
-      <c r="C180" t="s">
+      <c r="D180" t="s">
         <v>238</v>
-      </c>
-      <c r="D180" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="181">
@@ -3916,13 +3721,13 @@
         <v>4</v>
       </c>
       <c r="B181" t="s">
-        <v>237</v>
+        <v>11</v>
       </c>
       <c r="C181" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D181" t="s">
-        <v>239</v>
+        <v>10</v>
       </c>
     </row>
     <row r="182">
@@ -3930,10 +3735,10 @@
         <v>4</v>
       </c>
       <c r="B182" t="s">
+        <v>19</v>
+      </c>
+      <c r="C182" t="s">
         <v>240</v>
-      </c>
-      <c r="C182" t="s">
-        <v>12</v>
       </c>
       <c r="D182" t="s">
         <v>10</v>
@@ -3947,7 +3752,7 @@
         <v>241</v>
       </c>
       <c r="C183" t="s">
-        <v>20</v>
+        <v>242</v>
       </c>
       <c r="D183" t="s">
         <v>10</v>
@@ -3958,13 +3763,13 @@
         <v>4</v>
       </c>
       <c r="B184" t="s">
-        <v>242</v>
+        <v>170</v>
       </c>
       <c r="C184" t="s">
         <v>243</v>
       </c>
       <c r="D184" t="s">
-        <v>10</v>
+        <v>172</v>
       </c>
     </row>
     <row r="185">
@@ -3972,13 +3777,13 @@
         <v>4</v>
       </c>
       <c r="B185" t="s">
+        <v>170</v>
+      </c>
+      <c r="C185" t="s">
+        <v>243</v>
+      </c>
+      <c r="D185" t="s">
         <v>244</v>
-      </c>
-      <c r="C185" t="s">
-        <v>172</v>
-      </c>
-      <c r="D185" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="186">
@@ -3986,13 +3791,13 @@
         <v>4</v>
       </c>
       <c r="B186" t="s">
-        <v>244</v>
+        <v>49</v>
       </c>
       <c r="C186" t="s">
-        <v>172</v>
+        <v>245</v>
       </c>
       <c r="D186" t="s">
-        <v>245</v>
+        <v>51</v>
       </c>
     </row>
     <row r="187">
@@ -4000,13 +3805,13 @@
         <v>4</v>
       </c>
       <c r="B187" t="s">
+        <v>8</v>
+      </c>
+      <c r="C187" t="s">
         <v>246</v>
       </c>
-      <c r="C187" t="s">
-        <v>50</v>
-      </c>
       <c r="D187" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="188">
@@ -4017,10 +3822,10 @@
         <v>247</v>
       </c>
       <c r="C188" t="s">
-        <v>9</v>
+        <v>248</v>
       </c>
       <c r="D188" t="s">
-        <v>59</v>
+        <v>249</v>
       </c>
     </row>
     <row r="189">
@@ -4028,13 +3833,13 @@
         <v>4</v>
       </c>
       <c r="B189" t="s">
-        <v>248</v>
+        <v>93</v>
       </c>
       <c r="C189" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D189" t="s">
-        <v>250</v>
+        <v>7</v>
       </c>
     </row>
     <row r="190">
@@ -4042,13 +3847,13 @@
         <v>4</v>
       </c>
       <c r="B190" t="s">
+        <v>11</v>
+      </c>
+      <c r="C190" t="s">
         <v>251</v>
       </c>
-      <c r="C190" t="s">
-        <v>94</v>
-      </c>
       <c r="D190" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="191">
@@ -4056,10 +3861,10 @@
         <v>4</v>
       </c>
       <c r="B191" t="s">
+        <v>52</v>
+      </c>
+      <c r="C191" t="s">
         <v>252</v>
-      </c>
-      <c r="C191" t="s">
-        <v>12</v>
       </c>
       <c r="D191" t="s">
         <v>10</v>
@@ -4070,13 +3875,13 @@
         <v>4</v>
       </c>
       <c r="B192" t="s">
+        <v>104</v>
+      </c>
+      <c r="C192" t="s">
         <v>253</v>
       </c>
-      <c r="C192" t="s">
-        <v>53</v>
-      </c>
       <c r="D192" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="193">
@@ -4084,13 +3889,13 @@
         <v>4</v>
       </c>
       <c r="B193" t="s">
+        <v>8</v>
+      </c>
+      <c r="C193" t="s">
         <v>254</v>
       </c>
-      <c r="C193" t="s">
-        <v>105</v>
-      </c>
       <c r="D193" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
     </row>
     <row r="194">
@@ -4098,13 +3903,13 @@
         <v>4</v>
       </c>
       <c r="B194" t="s">
-        <v>255</v>
+        <v>8</v>
       </c>
       <c r="C194" t="s">
-        <v>9</v>
+        <v>254</v>
       </c>
       <c r="D194" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
     </row>
     <row r="195">
@@ -4112,13 +3917,13 @@
         <v>4</v>
       </c>
       <c r="B195" t="s">
-        <v>255</v>
+        <v>8</v>
       </c>
       <c r="C195" t="s">
-        <v>9</v>
+        <v>254</v>
       </c>
       <c r="D195" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="196">
@@ -4126,13 +3931,13 @@
         <v>4</v>
       </c>
       <c r="B196" t="s">
+        <v>8</v>
+      </c>
+      <c r="C196" t="s">
         <v>255</v>
       </c>
-      <c r="C196" t="s">
-        <v>9</v>
-      </c>
       <c r="D196" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="197">
@@ -4140,13 +3945,13 @@
         <v>4</v>
       </c>
       <c r="B197" t="s">
+        <v>8</v>
+      </c>
+      <c r="C197" t="s">
         <v>256</v>
       </c>
-      <c r="C197" t="s">
-        <v>9</v>
-      </c>
       <c r="D197" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="198">
@@ -4157,10 +3962,10 @@
         <v>257</v>
       </c>
       <c r="C198" t="s">
-        <v>9</v>
+        <v>258</v>
       </c>
       <c r="D198" t="s">
-        <v>7</v>
+        <v>259</v>
       </c>
     </row>
     <row r="199">
@@ -4168,13 +3973,13 @@
         <v>4</v>
       </c>
       <c r="B199" t="s">
-        <v>258</v>
+        <v>200</v>
       </c>
       <c r="C199" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D199" t="s">
-        <v>260</v>
+        <v>7</v>
       </c>
     </row>
     <row r="200">
@@ -4182,13 +3987,13 @@
         <v>4</v>
       </c>
       <c r="B200" t="s">
+        <v>200</v>
+      </c>
+      <c r="C200" t="s">
+        <v>260</v>
+      </c>
+      <c r="D200" t="s">
         <v>261</v>
-      </c>
-      <c r="C200" t="s">
-        <v>202</v>
-      </c>
-      <c r="D200" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="201">
@@ -4196,13 +4001,13 @@
         <v>4</v>
       </c>
       <c r="B201" t="s">
-        <v>261</v>
+        <v>85</v>
       </c>
       <c r="C201" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
       <c r="D201" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="202">
@@ -4210,13 +4015,13 @@
         <v>4</v>
       </c>
       <c r="B202" t="s">
-        <v>263</v>
+        <v>85</v>
       </c>
       <c r="C202" t="s">
-        <v>86</v>
+        <v>262</v>
       </c>
       <c r="D202" t="s">
-        <v>264</v>
+        <v>7</v>
       </c>
     </row>
     <row r="203">
@@ -4224,13 +4029,13 @@
         <v>4</v>
       </c>
       <c r="B203" t="s">
-        <v>263</v>
+        <v>19</v>
       </c>
       <c r="C203" t="s">
-        <v>86</v>
+        <v>264</v>
       </c>
       <c r="D203" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="204">
@@ -4238,13 +4043,13 @@
         <v>4</v>
       </c>
       <c r="B204" t="s">
+        <v>29</v>
+      </c>
+      <c r="C204" t="s">
         <v>265</v>
       </c>
-      <c r="C204" t="s">
-        <v>20</v>
-      </c>
       <c r="D204" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="205">
@@ -4252,1171 +4057,13 @@
         <v>4</v>
       </c>
       <c r="B205" t="s">
-        <v>266</v>
+        <v>29</v>
       </c>
       <c r="C205" t="s">
-        <v>30</v>
+        <v>265</v>
       </c>
       <c r="D205" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="206">
-      <c r="A206" t="s">
-        <v>4</v>
-      </c>
-      <c r="B206" t="s">
-        <v>266</v>
-      </c>
-      <c r="C206" t="s">
-        <v>30</v>
-      </c>
-      <c r="D206" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="207">
-      <c r="A207" t="s">
-        <v>267</v>
-      </c>
-      <c r="B207" t="s">
-        <v>268</v>
-      </c>
-      <c r="C207" t="s">
-        <v>269</v>
-      </c>
-      <c r="D207" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="208">
-      <c r="A208" t="s">
-        <v>267</v>
-      </c>
-      <c r="B208" t="s">
-        <v>271</v>
-      </c>
-      <c r="C208" t="s">
-        <v>269</v>
-      </c>
-      <c r="D208" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="209">
-      <c r="A209" t="s">
-        <v>267</v>
-      </c>
-      <c r="B209" t="s">
-        <v>272</v>
-      </c>
-      <c r="C209" t="s">
-        <v>269</v>
-      </c>
-      <c r="D209" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="210">
-      <c r="A210" t="s">
-        <v>267</v>
-      </c>
-      <c r="B210" t="s">
-        <v>272</v>
-      </c>
-      <c r="C210" t="s">
-        <v>269</v>
-      </c>
-      <c r="D210" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="211">
-      <c r="A211" t="s">
-        <v>267</v>
-      </c>
-      <c r="B211" t="s">
-        <v>274</v>
-      </c>
-      <c r="C211" t="s">
-        <v>269</v>
-      </c>
-      <c r="D211" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="212">
-      <c r="A212" t="s">
-        <v>267</v>
-      </c>
-      <c r="B212" t="s">
-        <v>275</v>
-      </c>
-      <c r="C212" t="s">
-        <v>269</v>
-      </c>
-      <c r="D212" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="213">
-      <c r="A213" t="s">
-        <v>267</v>
-      </c>
-      <c r="B213" t="s">
-        <v>276</v>
-      </c>
-      <c r="C213" t="s">
-        <v>269</v>
-      </c>
-      <c r="D213" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="214">
-      <c r="A214" t="s">
-        <v>267</v>
-      </c>
-      <c r="B214" t="s">
-        <v>277</v>
-      </c>
-      <c r="C214" t="s">
-        <v>269</v>
-      </c>
-      <c r="D214" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="215">
-      <c r="A215" t="s">
-        <v>267</v>
-      </c>
-      <c r="B215" t="s">
-        <v>278</v>
-      </c>
-      <c r="C215" t="s">
-        <v>269</v>
-      </c>
-      <c r="D215" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="216">
-      <c r="A216" t="s">
-        <v>267</v>
-      </c>
-      <c r="B216" t="s">
-        <v>279</v>
-      </c>
-      <c r="C216" t="s">
-        <v>269</v>
-      </c>
-      <c r="D216" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="217">
-      <c r="A217" t="s">
-        <v>267</v>
-      </c>
-      <c r="B217" t="s">
-        <v>280</v>
-      </c>
-      <c r="C217" t="s">
-        <v>269</v>
-      </c>
-      <c r="D217" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="218">
-      <c r="A218" t="s">
-        <v>267</v>
-      </c>
-      <c r="B218" t="s">
-        <v>281</v>
-      </c>
-      <c r="C218" t="s">
-        <v>269</v>
-      </c>
-      <c r="D218" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="219">
-      <c r="A219" t="s">
-        <v>267</v>
-      </c>
-      <c r="B219" t="s">
-        <v>282</v>
-      </c>
-      <c r="C219" t="s">
-        <v>269</v>
-      </c>
-      <c r="D219" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="220">
-      <c r="A220" t="s">
-        <v>267</v>
-      </c>
-      <c r="B220" t="s">
-        <v>283</v>
-      </c>
-      <c r="C220" t="s">
-        <v>269</v>
-      </c>
-      <c r="D220" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="221">
-      <c r="A221" t="s">
-        <v>267</v>
-      </c>
-      <c r="B221" t="s">
-        <v>284</v>
-      </c>
-      <c r="C221" t="s">
-        <v>269</v>
-      </c>
-      <c r="D221" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="222">
-      <c r="A222" t="s">
-        <v>267</v>
-      </c>
-      <c r="B222" t="s">
-        <v>285</v>
-      </c>
-      <c r="C222" t="s">
-        <v>269</v>
-      </c>
-      <c r="D222" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="223">
-      <c r="A223" t="s">
-        <v>267</v>
-      </c>
-      <c r="B223" t="s">
-        <v>286</v>
-      </c>
-      <c r="C223" t="s">
-        <v>269</v>
-      </c>
-      <c r="D223" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="224">
-      <c r="A224" t="s">
-        <v>267</v>
-      </c>
-      <c r="B224" t="s">
-        <v>287</v>
-      </c>
-      <c r="C224" t="s">
-        <v>269</v>
-      </c>
-      <c r="D224" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="225">
-      <c r="A225" t="s">
-        <v>267</v>
-      </c>
-      <c r="B225" t="s">
-        <v>288</v>
-      </c>
-      <c r="C225" t="s">
-        <v>269</v>
-      </c>
-      <c r="D225" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="226">
-      <c r="A226" t="s">
-        <v>267</v>
-      </c>
-      <c r="B226" t="s">
-        <v>289</v>
-      </c>
-      <c r="C226" t="s">
-        <v>269</v>
-      </c>
-      <c r="D226" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="227">
-      <c r="A227" t="s">
-        <v>267</v>
-      </c>
-      <c r="B227" t="s">
-        <v>290</v>
-      </c>
-      <c r="C227" t="s">
-        <v>269</v>
-      </c>
-      <c r="D227" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="228">
-      <c r="A228" t="s">
-        <v>267</v>
-      </c>
-      <c r="B228" t="s">
-        <v>291</v>
-      </c>
-      <c r="C228" t="s">
-        <v>269</v>
-      </c>
-      <c r="D228" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="229">
-      <c r="A229" t="s">
-        <v>267</v>
-      </c>
-      <c r="B229" t="s">
-        <v>292</v>
-      </c>
-      <c r="C229" t="s">
-        <v>269</v>
-      </c>
-      <c r="D229" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="230">
-      <c r="A230" t="s">
-        <v>267</v>
-      </c>
-      <c r="B230" t="s">
-        <v>294</v>
-      </c>
-      <c r="C230" t="s">
-        <v>269</v>
-      </c>
-      <c r="D230" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="231">
-      <c r="A231" t="s">
-        <v>267</v>
-      </c>
-      <c r="B231" t="s">
-        <v>295</v>
-      </c>
-      <c r="C231" t="s">
-        <v>269</v>
-      </c>
-      <c r="D231" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="232">
-      <c r="A232" t="s">
-        <v>267</v>
-      </c>
-      <c r="B232" t="s">
-        <v>296</v>
-      </c>
-      <c r="C232" t="s">
-        <v>269</v>
-      </c>
-      <c r="D232" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="233">
-      <c r="A233" t="s">
-        <v>267</v>
-      </c>
-      <c r="B233" t="s">
-        <v>297</v>
-      </c>
-      <c r="C233" t="s">
-        <v>269</v>
-      </c>
-      <c r="D233" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="234">
-      <c r="A234" t="s">
-        <v>267</v>
-      </c>
-      <c r="B234" t="s">
-        <v>298</v>
-      </c>
-      <c r="C234" t="s">
-        <v>269</v>
-      </c>
-      <c r="D234" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="235">
-      <c r="A235" t="s">
-        <v>267</v>
-      </c>
-      <c r="B235" t="s">
-        <v>299</v>
-      </c>
-      <c r="C235" t="s">
-        <v>269</v>
-      </c>
-      <c r="D235" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="236">
-      <c r="A236" t="s">
-        <v>267</v>
-      </c>
-      <c r="B236" t="s">
-        <v>300</v>
-      </c>
-      <c r="C236" t="s">
-        <v>269</v>
-      </c>
-      <c r="D236" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="237">
-      <c r="A237" t="s">
-        <v>189</v>
-      </c>
-      <c r="B237" t="s">
-        <v>301</v>
-      </c>
-      <c r="C237" t="s">
-        <v>269</v>
-      </c>
-      <c r="D237" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="238">
-      <c r="A238" t="s">
-        <v>189</v>
-      </c>
-      <c r="B238" t="s">
-        <v>303</v>
-      </c>
-      <c r="C238" t="s">
-        <v>269</v>
-      </c>
-      <c r="D238" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="239">
-      <c r="A239" t="s">
-        <v>189</v>
-      </c>
-      <c r="B239" t="s">
-        <v>303</v>
-      </c>
-      <c r="C239" t="s">
-        <v>269</v>
-      </c>
-      <c r="D239" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="240">
-      <c r="A240" t="s">
-        <v>189</v>
-      </c>
-      <c r="B240" t="s">
-        <v>303</v>
-      </c>
-      <c r="C240" t="s">
-        <v>269</v>
-      </c>
-      <c r="D240" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="241">
-      <c r="A241" t="s">
-        <v>189</v>
-      </c>
-      <c r="B241" t="s">
-        <v>303</v>
-      </c>
-      <c r="C241" t="s">
-        <v>269</v>
-      </c>
-      <c r="D241" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="242">
-      <c r="A242" t="s">
-        <v>189</v>
-      </c>
-      <c r="B242" t="s">
-        <v>303</v>
-      </c>
-      <c r="C242" t="s">
-        <v>269</v>
-      </c>
-      <c r="D242" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="243">
-      <c r="A243" t="s">
-        <v>189</v>
-      </c>
-      <c r="B243" t="s">
-        <v>303</v>
-      </c>
-      <c r="C243" t="s">
-        <v>269</v>
-      </c>
-      <c r="D243" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="244">
-      <c r="A244" t="s">
-        <v>189</v>
-      </c>
-      <c r="B244" t="s">
-        <v>309</v>
-      </c>
-      <c r="C244" t="s">
-        <v>269</v>
-      </c>
-      <c r="D244" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="245">
-      <c r="A245" t="s">
-        <v>189</v>
-      </c>
-      <c r="B245" t="s">
-        <v>310</v>
-      </c>
-      <c r="C245" t="s">
-        <v>269</v>
-      </c>
-      <c r="D245" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="246">
-      <c r="A246" t="s">
-        <v>189</v>
-      </c>
-      <c r="B246" t="s">
-        <v>310</v>
-      </c>
-      <c r="C246" t="s">
-        <v>269</v>
-      </c>
-      <c r="D246" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="247">
-      <c r="A247" t="s">
-        <v>189</v>
-      </c>
-      <c r="B247" t="s">
-        <v>310</v>
-      </c>
-      <c r="C247" t="s">
-        <v>269</v>
-      </c>
-      <c r="D247" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="248">
-      <c r="A248" t="s">
-        <v>189</v>
-      </c>
-      <c r="B248" t="s">
-        <v>310</v>
-      </c>
-      <c r="C248" t="s">
-        <v>269</v>
-      </c>
-      <c r="D248" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="249">
-      <c r="A249" t="s">
-        <v>189</v>
-      </c>
-      <c r="B249" t="s">
-        <v>310</v>
-      </c>
-      <c r="C249" t="s">
-        <v>269</v>
-      </c>
-      <c r="D249" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="250">
-      <c r="A250" t="s">
-        <v>189</v>
-      </c>
-      <c r="B250" t="s">
-        <v>311</v>
-      </c>
-      <c r="C250" t="s">
-        <v>269</v>
-      </c>
-      <c r="D250" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="251">
-      <c r="A251" t="s">
-        <v>189</v>
-      </c>
-      <c r="B251" t="s">
-        <v>303</v>
-      </c>
-      <c r="C251" t="s">
-        <v>269</v>
-      </c>
-      <c r="D251" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="252">
-      <c r="A252" t="s">
-        <v>189</v>
-      </c>
-      <c r="B252" t="s">
-        <v>303</v>
-      </c>
-      <c r="C252" t="s">
-        <v>269</v>
-      </c>
-      <c r="D252" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="253">
-      <c r="A253" t="s">
-        <v>189</v>
-      </c>
-      <c r="B253" t="s">
-        <v>303</v>
-      </c>
-      <c r="C253" t="s">
-        <v>269</v>
-      </c>
-      <c r="D253" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="254">
-      <c r="A254" t="s">
-        <v>189</v>
-      </c>
-      <c r="B254" t="s">
-        <v>303</v>
-      </c>
-      <c r="C254" t="s">
-        <v>269</v>
-      </c>
-      <c r="D254" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="255">
-      <c r="A255" t="s">
-        <v>189</v>
-      </c>
-      <c r="B255" t="s">
-        <v>313</v>
-      </c>
-      <c r="C255" t="s">
-        <v>269</v>
-      </c>
-      <c r="D255" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="256">
-      <c r="A256" t="s">
-        <v>189</v>
-      </c>
-      <c r="B256" t="s">
-        <v>314</v>
-      </c>
-      <c r="C256" t="s">
-        <v>269</v>
-      </c>
-      <c r="D256" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="257">
-      <c r="A257" t="s">
-        <v>189</v>
-      </c>
-      <c r="B257" t="s">
-        <v>315</v>
-      </c>
-      <c r="C257" t="s">
-        <v>269</v>
-      </c>
-      <c r="D257" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="258">
-      <c r="A258" t="s">
-        <v>189</v>
-      </c>
-      <c r="B258" t="s">
-        <v>316</v>
-      </c>
-      <c r="C258" t="s">
-        <v>269</v>
-      </c>
-      <c r="D258" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="259">
-      <c r="A259" t="s">
-        <v>189</v>
-      </c>
-      <c r="B259" t="s">
-        <v>318</v>
-      </c>
-      <c r="C259" t="s">
-        <v>269</v>
-      </c>
-      <c r="D259" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="260">
-      <c r="A260" t="s">
-        <v>189</v>
-      </c>
-      <c r="B260" t="s">
-        <v>319</v>
-      </c>
-      <c r="C260" t="s">
-        <v>269</v>
-      </c>
-      <c r="D260" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="261">
-      <c r="A261" t="s">
-        <v>189</v>
-      </c>
-      <c r="B261" t="s">
-        <v>301</v>
-      </c>
-      <c r="C261" t="s">
-        <v>269</v>
-      </c>
-      <c r="D261" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="262">
-      <c r="A262" t="s">
-        <v>189</v>
-      </c>
-      <c r="B262" t="s">
-        <v>228</v>
-      </c>
-      <c r="C262" t="s">
-        <v>269</v>
-      </c>
-      <c r="D262" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="263">
-      <c r="A263" t="s">
-        <v>189</v>
-      </c>
-      <c r="B263" t="s">
-        <v>320</v>
-      </c>
-      <c r="C263" t="s">
-        <v>269</v>
-      </c>
-      <c r="D263" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="264">
-      <c r="A264" t="s">
-        <v>189</v>
-      </c>
-      <c r="B264" t="s">
-        <v>318</v>
-      </c>
-      <c r="C264" t="s">
-        <v>269</v>
-      </c>
-      <c r="D264" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="265">
-      <c r="A265" t="s">
-        <v>189</v>
-      </c>
-      <c r="B265" t="s">
-        <v>321</v>
-      </c>
-      <c r="C265" t="s">
-        <v>269</v>
-      </c>
-      <c r="D265" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="266">
-      <c r="A266" t="s">
-        <v>189</v>
-      </c>
-      <c r="B266" t="s">
-        <v>322</v>
-      </c>
-      <c r="C266" t="s">
-        <v>269</v>
-      </c>
-      <c r="D266" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="267">
-      <c r="A267" t="s">
-        <v>189</v>
-      </c>
-      <c r="B267" t="s">
-        <v>318</v>
-      </c>
-      <c r="C267" t="s">
-        <v>269</v>
-      </c>
-      <c r="D267" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="268">
-      <c r="A268" t="s">
-        <v>189</v>
-      </c>
-      <c r="B268" t="s">
-        <v>323</v>
-      </c>
-      <c r="C268" t="s">
-        <v>269</v>
-      </c>
-      <c r="D268" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="269">
-      <c r="A269" t="s">
-        <v>189</v>
-      </c>
-      <c r="B269" t="s">
-        <v>318</v>
-      </c>
-      <c r="C269" t="s">
-        <v>269</v>
-      </c>
-      <c r="D269" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="270">
-      <c r="A270" t="s">
-        <v>189</v>
-      </c>
-      <c r="B270" t="s">
-        <v>303</v>
-      </c>
-      <c r="C270" t="s">
-        <v>269</v>
-      </c>
-      <c r="D270" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="271">
-      <c r="A271" t="s">
-        <v>189</v>
-      </c>
-      <c r="B271" t="s">
-        <v>324</v>
-      </c>
-      <c r="C271" t="s">
-        <v>269</v>
-      </c>
-      <c r="D271" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="272">
-      <c r="A272" t="s">
-        <v>189</v>
-      </c>
-      <c r="B272" t="s">
-        <v>323</v>
-      </c>
-      <c r="C272" t="s">
-        <v>269</v>
-      </c>
-      <c r="D272" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="273">
-      <c r="A273" t="s">
-        <v>189</v>
-      </c>
-      <c r="B273" t="s">
-        <v>325</v>
-      </c>
-      <c r="C273" t="s">
-        <v>269</v>
-      </c>
-      <c r="D273"/>
-    </row>
-    <row r="274">
-      <c r="A274" t="s">
-        <v>189</v>
-      </c>
-      <c r="B274" t="s">
-        <v>318</v>
-      </c>
-      <c r="C274" t="s">
-        <v>269</v>
-      </c>
-      <c r="D274" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="275">
-      <c r="A275" t="s">
-        <v>189</v>
-      </c>
-      <c r="B275" t="s">
-        <v>326</v>
-      </c>
-      <c r="C275" t="s">
-        <v>269</v>
-      </c>
-      <c r="D275" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="276">
-      <c r="A276" t="s">
-        <v>189</v>
-      </c>
-      <c r="B276" t="s">
-        <v>327</v>
-      </c>
-      <c r="C276" t="s">
-        <v>269</v>
-      </c>
-      <c r="D276"/>
-    </row>
-    <row r="277">
-      <c r="A277" t="s">
-        <v>189</v>
-      </c>
-      <c r="B277" t="s">
-        <v>328</v>
-      </c>
-      <c r="C277" t="s">
-        <v>269</v>
-      </c>
-      <c r="D277" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="278">
-      <c r="A278" t="s">
-        <v>189</v>
-      </c>
-      <c r="B278" t="s">
-        <v>329</v>
-      </c>
-      <c r="C278" t="s">
-        <v>269</v>
-      </c>
-      <c r="D278" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="279">
-      <c r="A279" t="s">
-        <v>189</v>
-      </c>
-      <c r="B279" t="s">
-        <v>197</v>
-      </c>
-      <c r="C279" t="s">
-        <v>269</v>
-      </c>
-      <c r="D279" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="280">
-      <c r="A280" t="s">
-        <v>189</v>
-      </c>
-      <c r="B280" t="s">
-        <v>318</v>
-      </c>
-      <c r="C280" t="s">
-        <v>269</v>
-      </c>
-      <c r="D280" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="281">
-      <c r="A281" t="s">
-        <v>189</v>
-      </c>
-      <c r="B281" t="s">
-        <v>318</v>
-      </c>
-      <c r="C281" t="s">
-        <v>269</v>
-      </c>
-      <c r="D281" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="282">
-      <c r="A282" t="s">
-        <v>189</v>
-      </c>
-      <c r="B282" t="s">
-        <v>330</v>
-      </c>
-      <c r="C282" t="s">
-        <v>269</v>
-      </c>
-      <c r="D282" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="283">
-      <c r="A283" t="s">
-        <v>189</v>
-      </c>
-      <c r="B283" t="s">
-        <v>330</v>
-      </c>
-      <c r="C283" t="s">
-        <v>269</v>
-      </c>
-      <c r="D283" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="284">
-      <c r="A284" t="s">
-        <v>189</v>
-      </c>
-      <c r="B284" t="s">
-        <v>330</v>
-      </c>
-      <c r="C284" t="s">
-        <v>269</v>
-      </c>
-      <c r="D284" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="285">
-      <c r="A285" t="s">
-        <v>189</v>
-      </c>
-      <c r="B285" t="s">
-        <v>330</v>
-      </c>
-      <c r="C285" t="s">
-        <v>269</v>
-      </c>
-      <c r="D285" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="286">
-      <c r="A286" t="s">
-        <v>189</v>
-      </c>
-      <c r="B286" t="s">
-        <v>330</v>
-      </c>
-      <c r="C286" t="s">
-        <v>269</v>
-      </c>
-      <c r="D286" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="287">
-      <c r="A287" t="s">
-        <v>189</v>
-      </c>
-      <c r="B287" t="s">
-        <v>303</v>
-      </c>
-      <c r="C287" t="s">
-        <v>269</v>
-      </c>
-      <c r="D287" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="288">
-      <c r="A288" t="s">
-        <v>189</v>
-      </c>
-      <c r="B288" t="s">
-        <v>197</v>
-      </c>
-      <c r="C288" t="s">
-        <v>269</v>
-      </c>
-      <c r="D288" t="s">
-        <v>302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bug(cannot save flights from brno and ostrava in the excel file), started refactoring of ryanair finder logic due to layout change
</commit_message>
<xml_diff>
--- a/src/data/flights.xlsx
+++ b/src/data/flights.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="326">
   <si>
     <t>From (City)</t>
   </si>
@@ -41,63 +41,63 @@
     <t>Prague</t>
   </si>
   <si>
+    <t>Aarhus</t>
+  </si>
+  <si>
     <t>Denmark</t>
   </si>
   <si>
-    <t>Aarhus</t>
-  </si>
-  <si>
     <t>Czech Airlines (ČSA)</t>
   </si>
   <si>
+    <t>Alghero</t>
+  </si>
+  <si>
     <t>Italy</t>
   </si>
   <si>
-    <t>Alghero</t>
-  </si>
-  <si>
     <t>SmartWings</t>
   </si>
   <si>
+    <t>Almeria</t>
+  </si>
+  <si>
     <t>Spain</t>
   </si>
   <si>
-    <t>Almeria</t>
+    <t>Amsterdam</t>
   </si>
   <si>
     <t>Netherlands</t>
   </si>
   <si>
-    <t>Amsterdam</t>
-  </si>
-  <si>
     <t>easyJet</t>
   </si>
   <si>
     <t>KLM</t>
   </si>
   <si>
+    <t>Antalya</t>
+  </si>
+  <si>
     <t>Turkey</t>
   </si>
   <si>
-    <t>Antalya</t>
+    <t>Athens</t>
   </si>
   <si>
     <t>Greece</t>
   </si>
   <si>
-    <t>Athens</t>
-  </si>
-  <si>
     <t>Aegean Airlines</t>
   </si>
   <si>
+    <t>Baku</t>
+  </si>
+  <si>
     <t>Azerbaijan</t>
   </si>
   <si>
-    <t>Baku</t>
-  </si>
-  <si>
     <t>Azerbaijan Airlines</t>
   </si>
   <si>
@@ -113,96 +113,96 @@
     <t>Wizz Air</t>
   </si>
   <si>
+    <t>Basel/Mulhouse</t>
+  </si>
+  <si>
     <t>Switzerland</t>
   </si>
   <si>
-    <t>Basel/Mulhouse</t>
+    <t>Beijing</t>
   </si>
   <si>
     <t>China</t>
   </si>
   <si>
-    <t>Beijing</t>
-  </si>
-  <si>
     <t>Hainan Airlines</t>
   </si>
   <si>
+    <t>Beirut</t>
+  </si>
+  <si>
     <t>Lebanon</t>
   </si>
   <si>
-    <t>Beirut</t>
+    <t>Belgrade</t>
   </si>
   <si>
     <t>Serbia</t>
   </si>
   <si>
-    <t>Belgrade</t>
-  </si>
-  <si>
     <t>Air Serbia</t>
   </si>
   <si>
+    <t>Bergen</t>
+  </si>
+  <si>
     <t>Norway</t>
   </si>
   <si>
-    <t>Bergen</t>
-  </si>
-  <si>
     <t>Norwegian</t>
   </si>
   <si>
+    <t>Berlin/Tegel</t>
+  </si>
+  <si>
     <t>Germany</t>
   </si>
   <si>
-    <t>Berlin/Tegel</t>
-  </si>
-  <si>
     <t>Air Berlin</t>
   </si>
   <si>
     <t>Bilbao</t>
   </si>
   <si>
+    <t>Birmingham</t>
+  </si>
+  <si>
     <t>Great Britain</t>
   </si>
   <si>
-    <t>Birmingham</t>
-  </si>
-  <si>
     <t>Bologna</t>
   </si>
   <si>
+    <t>Bordeaux</t>
+  </si>
+  <si>
     <t>France</t>
   </si>
   <si>
-    <t>Bordeaux</t>
-  </si>
-  <si>
     <t>Volotea</t>
   </si>
   <si>
+    <t>Bourgas</t>
+  </si>
+  <si>
     <t>Bulgaria</t>
   </si>
   <si>
-    <t>Bourgas</t>
+    <t>Bratislava</t>
   </si>
   <si>
     <t>Slovakia</t>
   </si>
   <si>
-    <t>Bratislava</t>
-  </si>
-  <si>
     <t>Bristol</t>
   </si>
   <si>
+    <t>Brussels/Charleroi</t>
+  </si>
+  <si>
     <t>Belgium</t>
   </si>
   <si>
-    <t>Brussels/Charleroi</t>
-  </si>
-  <si>
     <t>Ryanair</t>
   </si>
   <si>
@@ -212,21 +212,21 @@
     <t>Brussels Airlines</t>
   </si>
   <si>
+    <t>Bucharest</t>
+  </si>
+  <si>
     <t>Romania</t>
   </si>
   <si>
-    <t>Bucharest</t>
-  </si>
-  <si>
     <t>Tarom</t>
   </si>
   <si>
+    <t>Budapest</t>
+  </si>
+  <si>
     <t>Hungary</t>
   </si>
   <si>
-    <t>Budapest</t>
-  </si>
-  <si>
     <t>Cagliari</t>
   </si>
   <si>
@@ -260,33 +260,33 @@
     <t>Corfu</t>
   </si>
   <si>
+    <t>Dubai</t>
+  </si>
+  <si>
     <t>United Arab Emirates</t>
   </si>
   <si>
-    <t>Dubai</t>
-  </si>
-  <si>
     <t>flydubai</t>
   </si>
   <si>
     <t>Emirates</t>
   </si>
   <si>
+    <t>Dublin</t>
+  </si>
+  <si>
     <t>Ireland</t>
   </si>
   <si>
-    <t>Dublin</t>
-  </si>
-  <si>
     <t>Aer Lingus</t>
   </si>
   <si>
+    <t>Dubrovnik</t>
+  </si>
+  <si>
     <t>Croatia</t>
   </si>
   <si>
-    <t>Dubrovnik</t>
-  </si>
-  <si>
     <t>Dusseldorf</t>
   </si>
   <si>
@@ -305,21 +305,21 @@
     <t>Transavia</t>
   </si>
   <si>
+    <t>Ekaterinburg</t>
+  </si>
+  <si>
     <t>Russia</t>
   </si>
   <si>
-    <t>Ekaterinburg</t>
-  </si>
-  <si>
     <t>Ural Airlines</t>
   </si>
   <si>
+    <t>Faro</t>
+  </si>
+  <si>
     <t>Portugal</t>
   </si>
   <si>
-    <t>Faro</t>
-  </si>
-  <si>
     <t>Frankfurt</t>
   </si>
   <si>
@@ -338,21 +338,21 @@
     <t>Glasgow</t>
   </si>
   <si>
+    <t>Gothenburg</t>
+  </si>
+  <si>
     <t>Sweden</t>
   </si>
   <si>
-    <t>Gothenburg</t>
-  </si>
-  <si>
     <t>Hamburg</t>
   </si>
   <si>
+    <t>Helsinki</t>
+  </si>
+  <si>
     <t>Finland</t>
   </si>
   <si>
-    <t>Helsinki</t>
-  </si>
-  <si>
     <t>Finnair</t>
   </si>
   <si>
@@ -362,12 +362,12 @@
     <t>Hévíz/Balaton</t>
   </si>
   <si>
+    <t>Hurghada</t>
+  </si>
+  <si>
     <t>Egypt</t>
   </si>
   <si>
-    <t>Hurghada</t>
-  </si>
-  <si>
     <t>Air Cairo</t>
   </si>
   <si>
@@ -392,18 +392,18 @@
     <t>Kefallinia</t>
   </si>
   <si>
+    <t>Keflavik</t>
+  </si>
+  <si>
     <t>Iceland</t>
   </si>
   <si>
-    <t>Keflavik</t>
+    <t>Kiev/Borispol</t>
   </si>
   <si>
     <t>Ukraine</t>
   </si>
   <si>
-    <t>Kiev/Borispol</t>
-  </si>
-  <si>
     <t>Ukraine International Airlines</t>
   </si>
   <si>
@@ -425,12 +425,12 @@
     <t>Lanzarote</t>
   </si>
   <si>
+    <t>Larnaca</t>
+  </si>
+  <si>
     <t>Cyprus</t>
   </si>
   <si>
-    <t>Larnaca</t>
-  </si>
-  <si>
     <t>Las Palmas</t>
   </si>
   <si>
@@ -449,12 +449,12 @@
     <t>Liverpool</t>
   </si>
   <si>
+    <t>Ljubljana</t>
+  </si>
+  <si>
     <t>Slovenia</t>
   </si>
   <si>
-    <t>Ljubljana</t>
-  </si>
-  <si>
     <t>Adria Airways</t>
   </si>
   <si>
@@ -527,21 +527,21 @@
     <t>Milan/Malpensa</t>
   </si>
   <si>
+    <t>Minsk</t>
+  </si>
+  <si>
     <t>Belarus</t>
   </si>
   <si>
-    <t>Minsk</t>
-  </si>
-  <si>
     <t>Belavia</t>
   </si>
   <si>
+    <t>Montreal</t>
+  </si>
+  <si>
     <t>Canada</t>
   </si>
   <si>
-    <t>Montreal</t>
-  </si>
-  <si>
     <t>Air Transat</t>
   </si>
   <si>
@@ -560,12 +560,12 @@
     <t>Naples</t>
   </si>
   <si>
+    <t>New York/JFK</t>
+  </si>
+  <si>
     <t>USA</t>
   </si>
   <si>
-    <t>New York/JFK</t>
-  </si>
-  <si>
     <t>Delta Air Lines</t>
   </si>
   <si>
@@ -590,12 +590,12 @@
     <t>Oslo</t>
   </si>
   <si>
+    <t>Ostrava</t>
+  </si>
+  <si>
     <t>Czech Republic</t>
   </si>
   <si>
-    <t>Ostrava</t>
-  </si>
-  <si>
     <t>Palma Mallorca</t>
   </si>
   <si>
@@ -614,24 +614,24 @@
     <t>Pisa</t>
   </si>
   <si>
+    <t>Podgorica</t>
+  </si>
+  <si>
     <t>Monte Negro</t>
   </si>
   <si>
-    <t>Podgorica</t>
-  </si>
-  <si>
     <t>Porto</t>
   </si>
   <si>
     <t>Preveza</t>
   </si>
   <si>
+    <t>Radom</t>
+  </si>
+  <si>
     <t>Poland</t>
   </si>
   <si>
-    <t>Radom</t>
-  </si>
-  <si>
     <t>SprintAir</t>
   </si>
   <si>
@@ -641,21 +641,21 @@
     <t>Rhodes</t>
   </si>
   <si>
+    <t>Riga</t>
+  </si>
+  <si>
     <t>Latvia</t>
   </si>
   <si>
-    <t>Riga</t>
-  </si>
-  <si>
     <t>Air Baltic</t>
   </si>
   <si>
+    <t>Riyadh</t>
+  </si>
+  <si>
     <t>Saudi Arabia</t>
   </si>
   <si>
-    <t>Riyadh</t>
-  </si>
-  <si>
     <t>Rome/Ciampino</t>
   </si>
   <si>
@@ -674,12 +674,12 @@
     <t>Samos</t>
   </si>
   <si>
+    <t>Seoul/Incheon</t>
+  </si>
+  <si>
     <t>South Korea</t>
   </si>
   <si>
-    <t>Seoul/Incheon</t>
-  </si>
-  <si>
     <t>Korean Air</t>
   </si>
   <si>
@@ -695,12 +695,12 @@
     <t>Sharm El Sheikh</t>
   </si>
   <si>
+    <t>Skopje</t>
+  </si>
+  <si>
     <t>Macedonia</t>
   </si>
   <si>
-    <t>Skopje</t>
-  </si>
-  <si>
     <t>Sofia</t>
   </si>
   <si>
@@ -725,21 +725,21 @@
     <t>Strasbourg</t>
   </si>
   <si>
+    <t>Tbilisi</t>
+  </si>
+  <si>
     <t>Georgia</t>
   </si>
   <si>
-    <t>Tbilisi</t>
-  </si>
-  <si>
     <t>Georgian Airways</t>
   </si>
   <si>
+    <t>Tel Aviv</t>
+  </si>
+  <si>
     <t>Israel</t>
   </si>
   <si>
-    <t>Tel Aviv</t>
-  </si>
-  <si>
     <t>UP by El Al</t>
   </si>
   <si>
@@ -749,12 +749,12 @@
     <t>Thessaloniki</t>
   </si>
   <si>
+    <t>Tirana</t>
+  </si>
+  <si>
     <t>Albania</t>
   </si>
   <si>
-    <t>Tirana</t>
-  </si>
-  <si>
     <t>Toronto</t>
   </si>
   <si>
@@ -767,12 +767,12 @@
     <t>Trapani</t>
   </si>
   <si>
+    <t>Tunis</t>
+  </si>
+  <si>
     <t>Tunisia</t>
   </si>
   <si>
-    <t>Tunis</t>
-  </si>
-  <si>
     <t>Tunisair</t>
   </si>
   <si>
@@ -797,12 +797,12 @@
     <t>Verona</t>
   </si>
   <si>
+    <t>Vienna</t>
+  </si>
+  <si>
     <t>Austria</t>
   </si>
   <si>
-    <t>Vienna</t>
-  </si>
-  <si>
     <t>Austrian Airlines</t>
   </si>
   <si>
@@ -822,6 +822,186 @@
   </si>
   <si>
     <t>Zurich</t>
+  </si>
+  <si>
+    <t>Brno</t>
+  </si>
+  <si>
+    <t>ANTALYA</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Travel Service</t>
+  </si>
+  <si>
+    <t>KOS</t>
+  </si>
+  <si>
+    <t>BURGAS</t>
+  </si>
+  <si>
+    <t>EINDHOVEN</t>
+  </si>
+  <si>
+    <t>MUNICH</t>
+  </si>
+  <si>
+    <t>bmi regional</t>
+  </si>
+  <si>
+    <t>ZAKYNTHOS</t>
+  </si>
+  <si>
+    <t>MONASTIR / OSTRAVA</t>
+  </si>
+  <si>
+    <t>LONDON STANSTED</t>
+  </si>
+  <si>
+    <t>LAMEZIA TERME</t>
+  </si>
+  <si>
+    <t>VARNA</t>
+  </si>
+  <si>
+    <t>RHODOS</t>
+  </si>
+  <si>
+    <t>LONDON LUTON</t>
+  </si>
+  <si>
+    <t>HERAKLION</t>
+  </si>
+  <si>
+    <t>PALMA DE MALLORCA</t>
+  </si>
+  <si>
+    <t>ERCAN / ANTALYA</t>
+  </si>
+  <si>
+    <t>Tailwind Airlines</t>
+  </si>
+  <si>
+    <t>CORFU</t>
+  </si>
+  <si>
+    <t>ENFIDHA</t>
+  </si>
+  <si>
+    <t>DJERBA / OSTRAVA</t>
+  </si>
+  <si>
+    <t>DJERBA / ENFIDHA</t>
+  </si>
+  <si>
+    <t>HURGHADA</t>
+  </si>
+  <si>
+    <t>PODGORICA</t>
+  </si>
+  <si>
+    <t>MARSA ALAM</t>
+  </si>
+  <si>
+    <t>VARNA / OSTRAVA</t>
+  </si>
+  <si>
+    <t>TENERIFE</t>
+  </si>
+  <si>
+    <t>THESSALONIKI</t>
+  </si>
+  <si>
+    <t>KAVALA / OSTRAVA</t>
+  </si>
+  <si>
+    <t>ALMERIA / OSTRAVA</t>
+  </si>
+  <si>
+    <t>PREVEZA</t>
+  </si>
+  <si>
+    <t>Antalya, Antayla (AYT)</t>
+  </si>
+  <si>
+    <t>TRAVEL SERVICE / SMARTWINGS</t>
+  </si>
+  <si>
+    <t>Prague, Václav Havel Airport Prague (PRG)</t>
+  </si>
+  <si>
+    <t>CZECH AIRLINES (CSA)</t>
+  </si>
+  <si>
+    <t>KLM ROYAL DUTCH AIRLINES</t>
+  </si>
+  <si>
+    <t>DELTA AIR LINES</t>
+  </si>
+  <si>
+    <t>KOREAN AIR</t>
+  </si>
+  <si>
+    <t>TAROM ROMANIAN AIRLINES</t>
+  </si>
+  <si>
+    <t>Burgas, Burgas Airport (BOJ)</t>
+  </si>
+  <si>
+    <t>Kos, Kos Island International Airport (KGS)</t>
+  </si>
+  <si>
+    <t>Varna, Varna Airport (VAR)</t>
+  </si>
+  <si>
+    <t>London, Stansted (STN)</t>
+  </si>
+  <si>
+    <t>RYANAIR</t>
+  </si>
+  <si>
+    <t>MONASTIR</t>
+  </si>
+  <si>
+    <t>Rhodes, Diagoras Airport (RHO)</t>
+  </si>
+  <si>
+    <t>Crete / Heraklion, N. Kazantzakis Apt. (HER)</t>
+  </si>
+  <si>
+    <t>Mallorca, Palma de Mallorca (PMI)</t>
+  </si>
+  <si>
+    <t>Milan / Bergamo, Milan Bergamo Airport</t>
+  </si>
+  <si>
+    <t>Corfu / Kerkyra, I. Kapodistrias (CFU)</t>
+  </si>
+  <si>
+    <t>Djerba</t>
+  </si>
+  <si>
+    <t>Zakynthos, Zakinthos Is (ZTH)</t>
+  </si>
+  <si>
+    <t>Hurghada, Hurghada (HRG)</t>
+  </si>
+  <si>
+    <t>Rotterdam</t>
+  </si>
+  <si>
+    <t>Marsa Alam, Marsa Alam (RMF)</t>
+  </si>
+  <si>
+    <t>Warsawa</t>
+  </si>
+  <si>
+    <t>KAVALA</t>
+  </si>
+  <si>
+    <t>ALMERIA</t>
   </si>
 </sst>
 </file>
@@ -1185,7 +1365,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1341,10 +1521,10 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
@@ -1355,10 +1535,10 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
@@ -1369,10 +1549,10 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
         <v>26</v>
@@ -1383,10 +1563,10 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="D14" t="s">
         <v>28</v>
@@ -1481,10 +1661,10 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="D21" t="s">
         <v>7</v>
@@ -1509,10 +1689,10 @@
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="D23" t="s">
         <v>7</v>
@@ -1565,10 +1745,10 @@
         <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C27" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D27" t="s">
         <v>15</v>
@@ -1593,10 +1773,10 @@
         <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D29" t="s">
         <v>7</v>
@@ -1607,10 +1787,10 @@
         <v>4</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C30" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D30" t="s">
         <v>61</v>
@@ -1663,10 +1843,10 @@
         <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="C34" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="D34" t="s">
         <v>10</v>
@@ -1677,10 +1857,10 @@
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="C35" t="s">
-        <v>68</v>
+        <v>9</v>
       </c>
       <c r="D35" t="s">
         <v>10</v>
@@ -1691,10 +1871,10 @@
         <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="C36" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="D36" t="s">
         <v>10</v>
@@ -1705,10 +1885,10 @@
         <v>4</v>
       </c>
       <c r="B37" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="C37" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="D37" t="s">
         <v>71</v>
@@ -1719,10 +1899,10 @@
         <v>4</v>
       </c>
       <c r="B38" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="C38" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="D38" t="s">
         <v>73</v>
@@ -1733,10 +1913,10 @@
         <v>4</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="C39" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="D39" t="s">
         <v>74</v>
@@ -1747,10 +1927,10 @@
         <v>4</v>
       </c>
       <c r="B40" t="s">
-        <v>5</v>
+        <v>75</v>
       </c>
       <c r="C40" t="s">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="D40" t="s">
         <v>7</v>
@@ -1761,10 +1941,10 @@
         <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>5</v>
+        <v>75</v>
       </c>
       <c r="C41" t="s">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="D41" t="s">
         <v>41</v>
@@ -1775,10 +1955,10 @@
         <v>4</v>
       </c>
       <c r="B42" t="s">
-        <v>5</v>
+        <v>75</v>
       </c>
       <c r="C42" t="s">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="D42" t="s">
         <v>76</v>
@@ -1789,10 +1969,10 @@
         <v>4</v>
       </c>
       <c r="B43" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="C43" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="D43" t="s">
         <v>10</v>
@@ -1887,10 +2067,10 @@
         <v>4</v>
       </c>
       <c r="B50" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="C50" t="s">
-        <v>87</v>
+        <v>43</v>
       </c>
       <c r="D50" t="s">
         <v>73</v>
@@ -1901,10 +2081,10 @@
         <v>4</v>
       </c>
       <c r="B51" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="C51" t="s">
-        <v>87</v>
+        <v>43</v>
       </c>
       <c r="D51" t="s">
         <v>7</v>
@@ -1915,10 +2095,10 @@
         <v>4</v>
       </c>
       <c r="B52" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="C52" t="s">
-        <v>87</v>
+        <v>43</v>
       </c>
       <c r="D52" t="s">
         <v>74</v>
@@ -1929,10 +2109,10 @@
         <v>4</v>
       </c>
       <c r="B53" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="C53" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="D53" t="s">
         <v>89</v>
@@ -1943,10 +2123,10 @@
         <v>4</v>
       </c>
       <c r="B54" t="s">
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="C54" t="s">
-        <v>90</v>
+        <v>47</v>
       </c>
       <c r="D54" t="s">
         <v>15</v>
@@ -1957,10 +2137,10 @@
         <v>4</v>
       </c>
       <c r="B55" t="s">
-        <v>13</v>
+        <v>91</v>
       </c>
       <c r="C55" t="s">
-        <v>91</v>
+        <v>14</v>
       </c>
       <c r="D55" t="s">
         <v>92</v>
@@ -2013,10 +2193,10 @@
         <v>4</v>
       </c>
       <c r="B59" t="s">
-        <v>42</v>
+        <v>98</v>
       </c>
       <c r="C59" t="s">
-        <v>98</v>
+        <v>43</v>
       </c>
       <c r="D59" t="s">
         <v>7</v>
@@ -2027,10 +2207,10 @@
         <v>4</v>
       </c>
       <c r="B60" t="s">
-        <v>42</v>
+        <v>98</v>
       </c>
       <c r="C60" t="s">
-        <v>98</v>
+        <v>43</v>
       </c>
       <c r="D60" t="s">
         <v>99</v>
@@ -2041,10 +2221,10 @@
         <v>4</v>
       </c>
       <c r="B61" t="s">
-        <v>11</v>
+        <v>100</v>
       </c>
       <c r="C61" t="s">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="D61" t="s">
         <v>10</v>
@@ -2055,10 +2235,10 @@
         <v>4</v>
       </c>
       <c r="B62" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="C62" t="s">
-        <v>101</v>
+        <v>30</v>
       </c>
       <c r="D62" t="s">
         <v>102</v>
@@ -2069,10 +2249,10 @@
         <v>4</v>
       </c>
       <c r="B63" t="s">
-        <v>46</v>
+        <v>103</v>
       </c>
       <c r="C63" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="D63" t="s">
         <v>89</v>
@@ -2097,10 +2277,10 @@
         <v>4</v>
       </c>
       <c r="B65" t="s">
-        <v>42</v>
+        <v>106</v>
       </c>
       <c r="C65" t="s">
-        <v>106</v>
+        <v>43</v>
       </c>
       <c r="D65" t="s">
         <v>73</v>
@@ -2111,10 +2291,10 @@
         <v>4</v>
       </c>
       <c r="B66" t="s">
-        <v>42</v>
+        <v>106</v>
       </c>
       <c r="C66" t="s">
-        <v>106</v>
+        <v>43</v>
       </c>
       <c r="D66" t="s">
         <v>7</v>
@@ -2125,10 +2305,10 @@
         <v>4</v>
       </c>
       <c r="B67" t="s">
-        <v>42</v>
+        <v>106</v>
       </c>
       <c r="C67" t="s">
-        <v>106</v>
+        <v>43</v>
       </c>
       <c r="D67" t="s">
         <v>74</v>
@@ -2181,10 +2361,10 @@
         <v>4</v>
       </c>
       <c r="B71" t="s">
-        <v>19</v>
+        <v>110</v>
       </c>
       <c r="C71" t="s">
-        <v>110</v>
+        <v>20</v>
       </c>
       <c r="D71" t="s">
         <v>10</v>
@@ -2195,10 +2375,10 @@
         <v>4</v>
       </c>
       <c r="B72" t="s">
-        <v>65</v>
+        <v>111</v>
       </c>
       <c r="C72" t="s">
-        <v>111</v>
+        <v>66</v>
       </c>
       <c r="D72" t="s">
         <v>7</v>
@@ -2237,10 +2417,10 @@
         <v>4</v>
       </c>
       <c r="B75" t="s">
-        <v>11</v>
+        <v>115</v>
       </c>
       <c r="C75" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="D75" t="s">
         <v>10</v>
@@ -2251,10 +2431,10 @@
         <v>4</v>
       </c>
       <c r="B76" t="s">
-        <v>17</v>
+        <v>116</v>
       </c>
       <c r="C76" t="s">
-        <v>116</v>
+        <v>18</v>
       </c>
       <c r="D76" t="s">
         <v>117</v>
@@ -2265,10 +2445,10 @@
         <v>4</v>
       </c>
       <c r="B77" t="s">
-        <v>17</v>
+        <v>118</v>
       </c>
       <c r="C77" t="s">
-        <v>118</v>
+        <v>18</v>
       </c>
       <c r="D77" t="s">
         <v>119</v>
@@ -2279,10 +2459,10 @@
         <v>4</v>
       </c>
       <c r="B78" t="s">
-        <v>93</v>
+        <v>120</v>
       </c>
       <c r="C78" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="D78" t="s">
         <v>7</v>
@@ -2293,10 +2473,10 @@
         <v>4</v>
       </c>
       <c r="B79" t="s">
-        <v>19</v>
+        <v>121</v>
       </c>
       <c r="C79" t="s">
-        <v>121</v>
+        <v>20</v>
       </c>
       <c r="D79" t="s">
         <v>10</v>
@@ -2363,10 +2543,10 @@
         <v>4</v>
       </c>
       <c r="B84" t="s">
-        <v>19</v>
+        <v>127</v>
       </c>
       <c r="C84" t="s">
-        <v>127</v>
+        <v>20</v>
       </c>
       <c r="D84" t="s">
         <v>10</v>
@@ -2377,10 +2557,10 @@
         <v>4</v>
       </c>
       <c r="B85" t="s">
-        <v>54</v>
+        <v>128</v>
       </c>
       <c r="C85" t="s">
-        <v>128</v>
+        <v>55</v>
       </c>
       <c r="D85" t="s">
         <v>7</v>
@@ -2391,10 +2571,10 @@
         <v>4</v>
       </c>
       <c r="B86" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="C86" t="s">
-        <v>129</v>
+        <v>94</v>
       </c>
       <c r="D86" t="s">
         <v>130</v>
@@ -2405,10 +2585,10 @@
         <v>4</v>
       </c>
       <c r="B87" t="s">
-        <v>8</v>
+        <v>131</v>
       </c>
       <c r="C87" t="s">
-        <v>131</v>
+        <v>9</v>
       </c>
       <c r="D87" t="s">
         <v>10</v>
@@ -2419,10 +2599,10 @@
         <v>4</v>
       </c>
       <c r="B88" t="s">
-        <v>11</v>
+        <v>132</v>
       </c>
       <c r="C88" t="s">
-        <v>132</v>
+        <v>12</v>
       </c>
       <c r="D88" t="s">
         <v>10</v>
@@ -2447,10 +2627,10 @@
         <v>4</v>
       </c>
       <c r="B90" t="s">
-        <v>11</v>
+        <v>135</v>
       </c>
       <c r="C90" t="s">
-        <v>135</v>
+        <v>12</v>
       </c>
       <c r="D90" t="s">
         <v>10</v>
@@ -2461,10 +2641,10 @@
         <v>4</v>
       </c>
       <c r="B91" t="s">
-        <v>46</v>
+        <v>136</v>
       </c>
       <c r="C91" t="s">
-        <v>136</v>
+        <v>47</v>
       </c>
       <c r="D91" t="s">
         <v>89</v>
@@ -2475,10 +2655,10 @@
         <v>4</v>
       </c>
       <c r="B92" t="s">
-        <v>104</v>
+        <v>137</v>
       </c>
       <c r="C92" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="D92" t="s">
         <v>7</v>
@@ -2489,10 +2669,10 @@
         <v>4</v>
       </c>
       <c r="B93" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="C93" t="s">
-        <v>138</v>
+        <v>97</v>
       </c>
       <c r="D93" t="s">
         <v>7</v>
@@ -2503,10 +2683,10 @@
         <v>4</v>
       </c>
       <c r="B94" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="C94" t="s">
-        <v>138</v>
+        <v>97</v>
       </c>
       <c r="D94" t="s">
         <v>139</v>
@@ -2517,10 +2697,10 @@
         <v>4</v>
       </c>
       <c r="B95" t="s">
-        <v>46</v>
+        <v>140</v>
       </c>
       <c r="C95" t="s">
-        <v>140</v>
+        <v>47</v>
       </c>
       <c r="D95" t="s">
         <v>59</v>
@@ -2545,10 +2725,10 @@
         <v>4</v>
       </c>
       <c r="B97" t="s">
-        <v>46</v>
+        <v>144</v>
       </c>
       <c r="C97" t="s">
-        <v>144</v>
+        <v>47</v>
       </c>
       <c r="D97" t="s">
         <v>10</v>
@@ -2559,10 +2739,10 @@
         <v>4</v>
       </c>
       <c r="B98" t="s">
-        <v>46</v>
+        <v>144</v>
       </c>
       <c r="C98" t="s">
-        <v>144</v>
+        <v>47</v>
       </c>
       <c r="D98" t="s">
         <v>15</v>
@@ -2573,10 +2753,10 @@
         <v>4</v>
       </c>
       <c r="B99" t="s">
-        <v>46</v>
+        <v>145</v>
       </c>
       <c r="C99" t="s">
-        <v>145</v>
+        <v>47</v>
       </c>
       <c r="D99" t="s">
         <v>146</v>
@@ -2587,10 +2767,10 @@
         <v>4</v>
       </c>
       <c r="B100" t="s">
-        <v>46</v>
+        <v>147</v>
       </c>
       <c r="C100" t="s">
-        <v>147</v>
+        <v>47</v>
       </c>
       <c r="D100" t="s">
         <v>28</v>
@@ -2601,10 +2781,10 @@
         <v>4</v>
       </c>
       <c r="B101" t="s">
-        <v>46</v>
+        <v>148</v>
       </c>
       <c r="C101" t="s">
-        <v>148</v>
+        <v>47</v>
       </c>
       <c r="D101" t="s">
         <v>149</v>
@@ -2615,10 +2795,10 @@
         <v>4</v>
       </c>
       <c r="B102" t="s">
-        <v>46</v>
+        <v>150</v>
       </c>
       <c r="C102" t="s">
-        <v>150</v>
+        <v>47</v>
       </c>
       <c r="D102" t="s">
         <v>59</v>
@@ -2629,10 +2809,10 @@
         <v>4</v>
       </c>
       <c r="B103" t="s">
-        <v>46</v>
+        <v>150</v>
       </c>
       <c r="C103" t="s">
-        <v>150</v>
+        <v>47</v>
       </c>
       <c r="D103" t="s">
         <v>15</v>
@@ -2657,10 +2837,10 @@
         <v>4</v>
       </c>
       <c r="B105" t="s">
-        <v>49</v>
+        <v>153</v>
       </c>
       <c r="C105" t="s">
-        <v>153</v>
+        <v>50</v>
       </c>
       <c r="D105" t="s">
         <v>154</v>
@@ -2671,10 +2851,10 @@
         <v>4</v>
       </c>
       <c r="B106" t="s">
-        <v>96</v>
+        <v>155</v>
       </c>
       <c r="C106" t="s">
-        <v>155</v>
+        <v>97</v>
       </c>
       <c r="D106" t="s">
         <v>10</v>
@@ -2685,10 +2865,10 @@
         <v>4</v>
       </c>
       <c r="B107" t="s">
-        <v>11</v>
+        <v>156</v>
       </c>
       <c r="C107" t="s">
-        <v>156</v>
+        <v>12</v>
       </c>
       <c r="D107" t="s">
         <v>7</v>
@@ -2699,10 +2879,10 @@
         <v>4</v>
       </c>
       <c r="B108" t="s">
-        <v>11</v>
+        <v>156</v>
       </c>
       <c r="C108" t="s">
-        <v>156</v>
+        <v>12</v>
       </c>
       <c r="D108" t="s">
         <v>157</v>
@@ -2713,10 +2893,10 @@
         <v>4</v>
       </c>
       <c r="B109" t="s">
-        <v>11</v>
+        <v>158</v>
       </c>
       <c r="C109" t="s">
-        <v>158</v>
+        <v>12</v>
       </c>
       <c r="D109" t="s">
         <v>10</v>
@@ -2755,10 +2935,10 @@
         <v>4</v>
       </c>
       <c r="B112" t="s">
-        <v>46</v>
+        <v>161</v>
       </c>
       <c r="C112" t="s">
-        <v>161</v>
+        <v>47</v>
       </c>
       <c r="D112" t="s">
         <v>15</v>
@@ -2769,10 +2949,10 @@
         <v>4</v>
       </c>
       <c r="B113" t="s">
-        <v>46</v>
+        <v>161</v>
       </c>
       <c r="C113" t="s">
-        <v>161</v>
+        <v>47</v>
       </c>
       <c r="D113" t="s">
         <v>89</v>
@@ -2783,10 +2963,10 @@
         <v>4</v>
       </c>
       <c r="B114" t="s">
-        <v>112</v>
+        <v>162</v>
       </c>
       <c r="C114" t="s">
-        <v>162</v>
+        <v>113</v>
       </c>
       <c r="D114" t="s">
         <v>114</v>
@@ -2797,10 +2977,10 @@
         <v>4</v>
       </c>
       <c r="B115" t="s">
-        <v>112</v>
+        <v>162</v>
       </c>
       <c r="C115" t="s">
-        <v>162</v>
+        <v>113</v>
       </c>
       <c r="D115" t="s">
         <v>10</v>
@@ -2811,10 +2991,10 @@
         <v>4</v>
       </c>
       <c r="B116" t="s">
-        <v>49</v>
+        <v>163</v>
       </c>
       <c r="C116" t="s">
-        <v>163</v>
+        <v>50</v>
       </c>
       <c r="D116" t="s">
         <v>51</v>
@@ -2825,10 +3005,10 @@
         <v>4</v>
       </c>
       <c r="B117" t="s">
-        <v>11</v>
+        <v>164</v>
       </c>
       <c r="C117" t="s">
-        <v>164</v>
+        <v>12</v>
       </c>
       <c r="D117" t="s">
         <v>10</v>
@@ -2839,10 +3019,10 @@
         <v>4</v>
       </c>
       <c r="B118" t="s">
-        <v>8</v>
+        <v>165</v>
       </c>
       <c r="C118" t="s">
-        <v>165</v>
+        <v>9</v>
       </c>
       <c r="D118" t="s">
         <v>59</v>
@@ -2853,10 +3033,10 @@
         <v>4</v>
       </c>
       <c r="B119" t="s">
-        <v>8</v>
+        <v>165</v>
       </c>
       <c r="C119" t="s">
-        <v>165</v>
+        <v>9</v>
       </c>
       <c r="D119" t="s">
         <v>28</v>
@@ -2867,10 +3047,10 @@
         <v>4</v>
       </c>
       <c r="B120" t="s">
-        <v>8</v>
+        <v>166</v>
       </c>
       <c r="C120" t="s">
-        <v>166</v>
+        <v>9</v>
       </c>
       <c r="D120" t="s">
         <v>7</v>
@@ -2881,10 +3061,10 @@
         <v>4</v>
       </c>
       <c r="B121" t="s">
-        <v>8</v>
+        <v>166</v>
       </c>
       <c r="C121" t="s">
-        <v>166</v>
+        <v>9</v>
       </c>
       <c r="D121" t="s">
         <v>15</v>
@@ -2923,10 +3103,10 @@
         <v>4</v>
       </c>
       <c r="B124" t="s">
-        <v>93</v>
+        <v>173</v>
       </c>
       <c r="C124" t="s">
-        <v>173</v>
+        <v>94</v>
       </c>
       <c r="D124" t="s">
         <v>7</v>
@@ -2937,10 +3117,10 @@
         <v>4</v>
       </c>
       <c r="B125" t="s">
-        <v>93</v>
+        <v>173</v>
       </c>
       <c r="C125" t="s">
-        <v>173</v>
+        <v>94</v>
       </c>
       <c r="D125" t="s">
         <v>10</v>
@@ -2951,10 +3131,10 @@
         <v>4</v>
       </c>
       <c r="B126" t="s">
-        <v>93</v>
+        <v>173</v>
       </c>
       <c r="C126" t="s">
-        <v>173</v>
+        <v>94</v>
       </c>
       <c r="D126" t="s">
         <v>174</v>
@@ -2965,10 +3145,10 @@
         <v>4</v>
       </c>
       <c r="B127" t="s">
-        <v>42</v>
+        <v>175</v>
       </c>
       <c r="C127" t="s">
-        <v>175</v>
+        <v>43</v>
       </c>
       <c r="D127" t="s">
         <v>99</v>
@@ -2979,10 +3159,10 @@
         <v>4</v>
       </c>
       <c r="B128" t="s">
-        <v>49</v>
+        <v>176</v>
       </c>
       <c r="C128" t="s">
-        <v>176</v>
+        <v>50</v>
       </c>
       <c r="D128" t="s">
         <v>51</v>
@@ -2993,10 +3173,10 @@
         <v>4</v>
       </c>
       <c r="B129" t="s">
-        <v>8</v>
+        <v>177</v>
       </c>
       <c r="C129" t="s">
-        <v>177</v>
+        <v>9</v>
       </c>
       <c r="D129" t="s">
         <v>10</v>
@@ -3007,10 +3187,10 @@
         <v>4</v>
       </c>
       <c r="B130" t="s">
-        <v>8</v>
+        <v>177</v>
       </c>
       <c r="C130" t="s">
-        <v>177</v>
+        <v>9</v>
       </c>
       <c r="D130" t="s">
         <v>15</v>
@@ -3021,10 +3201,10 @@
         <v>4</v>
       </c>
       <c r="B131" t="s">
-        <v>8</v>
+        <v>177</v>
       </c>
       <c r="C131" t="s">
-        <v>177</v>
+        <v>9</v>
       </c>
       <c r="D131" t="s">
         <v>28</v>
@@ -3049,10 +3229,10 @@
         <v>4</v>
       </c>
       <c r="B133" t="s">
-        <v>46</v>
+        <v>181</v>
       </c>
       <c r="C133" t="s">
-        <v>181</v>
+        <v>47</v>
       </c>
       <c r="D133" t="s">
         <v>89</v>
@@ -3063,10 +3243,10 @@
         <v>4</v>
       </c>
       <c r="B134" t="s">
-        <v>49</v>
+        <v>182</v>
       </c>
       <c r="C134" t="s">
-        <v>182</v>
+        <v>50</v>
       </c>
       <c r="D134" t="s">
         <v>7</v>
@@ -3077,10 +3257,10 @@
         <v>4</v>
       </c>
       <c r="B135" t="s">
-        <v>93</v>
+        <v>183</v>
       </c>
       <c r="C135" t="s">
-        <v>183</v>
+        <v>94</v>
       </c>
       <c r="D135" t="s">
         <v>184</v>
@@ -3091,10 +3271,10 @@
         <v>4</v>
       </c>
       <c r="B136" t="s">
-        <v>124</v>
+        <v>185</v>
       </c>
       <c r="C136" t="s">
-        <v>185</v>
+        <v>125</v>
       </c>
       <c r="D136" t="s">
         <v>7</v>
@@ -3105,10 +3285,10 @@
         <v>4</v>
       </c>
       <c r="B137" t="s">
-        <v>8</v>
+        <v>186</v>
       </c>
       <c r="C137" t="s">
-        <v>186</v>
+        <v>9</v>
       </c>
       <c r="D137" t="s">
         <v>10</v>
@@ -3119,10 +3299,10 @@
         <v>4</v>
       </c>
       <c r="B138" t="s">
-        <v>39</v>
+        <v>187</v>
       </c>
       <c r="C138" t="s">
-        <v>187</v>
+        <v>40</v>
       </c>
       <c r="D138" t="s">
         <v>41</v>
@@ -3147,10 +3327,10 @@
         <v>4</v>
       </c>
       <c r="B140" t="s">
-        <v>11</v>
+        <v>190</v>
       </c>
       <c r="C140" t="s">
-        <v>190</v>
+        <v>12</v>
       </c>
       <c r="D140" t="s">
         <v>10</v>
@@ -3161,10 +3341,10 @@
         <v>4</v>
       </c>
       <c r="B141" t="s">
-        <v>49</v>
+        <v>191</v>
       </c>
       <c r="C141" t="s">
-        <v>191</v>
+        <v>50</v>
       </c>
       <c r="D141" t="s">
         <v>7</v>
@@ -3175,10 +3355,10 @@
         <v>4</v>
       </c>
       <c r="B142" t="s">
-        <v>49</v>
+        <v>191</v>
       </c>
       <c r="C142" t="s">
-        <v>191</v>
+        <v>50</v>
       </c>
       <c r="D142" t="s">
         <v>15</v>
@@ -3189,10 +3369,10 @@
         <v>4</v>
       </c>
       <c r="B143" t="s">
-        <v>49</v>
+        <v>191</v>
       </c>
       <c r="C143" t="s">
-        <v>191</v>
+        <v>50</v>
       </c>
       <c r="D143" t="s">
         <v>192</v>
@@ -3203,10 +3383,10 @@
         <v>4</v>
       </c>
       <c r="B144" t="s">
-        <v>49</v>
+        <v>191</v>
       </c>
       <c r="C144" t="s">
-        <v>191</v>
+        <v>50</v>
       </c>
       <c r="D144" t="s">
         <v>26</v>
@@ -3217,10 +3397,10 @@
         <v>4</v>
       </c>
       <c r="B145" t="s">
-        <v>49</v>
+        <v>193</v>
       </c>
       <c r="C145" t="s">
-        <v>193</v>
+        <v>50</v>
       </c>
       <c r="D145" t="s">
         <v>194</v>
@@ -3231,10 +3411,10 @@
         <v>4</v>
       </c>
       <c r="B146" t="s">
-        <v>8</v>
+        <v>195</v>
       </c>
       <c r="C146" t="s">
-        <v>195</v>
+        <v>9</v>
       </c>
       <c r="D146" t="s">
         <v>7</v>
@@ -3259,10 +3439,10 @@
         <v>4</v>
       </c>
       <c r="B148" t="s">
-        <v>96</v>
+        <v>198</v>
       </c>
       <c r="C148" t="s">
-        <v>198</v>
+        <v>97</v>
       </c>
       <c r="D148" t="s">
         <v>7</v>
@@ -3273,10 +3453,10 @@
         <v>4</v>
       </c>
       <c r="B149" t="s">
-        <v>19</v>
+        <v>199</v>
       </c>
       <c r="C149" t="s">
-        <v>199</v>
+        <v>20</v>
       </c>
       <c r="D149" t="s">
         <v>10</v>
@@ -3301,10 +3481,10 @@
         <v>4</v>
       </c>
       <c r="B151" t="s">
-        <v>78</v>
+        <v>203</v>
       </c>
       <c r="C151" t="s">
-        <v>203</v>
+        <v>79</v>
       </c>
       <c r="D151" t="s">
         <v>10</v>
@@ -3315,10 +3495,10 @@
         <v>4</v>
       </c>
       <c r="B152" t="s">
-        <v>19</v>
+        <v>204</v>
       </c>
       <c r="C152" t="s">
-        <v>204</v>
+        <v>20</v>
       </c>
       <c r="D152" t="s">
         <v>10</v>
@@ -3357,10 +3537,10 @@
         <v>4</v>
       </c>
       <c r="B155" t="s">
-        <v>8</v>
+        <v>210</v>
       </c>
       <c r="C155" t="s">
-        <v>210</v>
+        <v>9</v>
       </c>
       <c r="D155" t="s">
         <v>59</v>
@@ -3371,10 +3551,10 @@
         <v>4</v>
       </c>
       <c r="B156" t="s">
-        <v>8</v>
+        <v>211</v>
       </c>
       <c r="C156" t="s">
-        <v>211</v>
+        <v>9</v>
       </c>
       <c r="D156" t="s">
         <v>7</v>
@@ -3385,10 +3565,10 @@
         <v>4</v>
       </c>
       <c r="B157" t="s">
-        <v>8</v>
+        <v>211</v>
       </c>
       <c r="C157" t="s">
-        <v>211</v>
+        <v>9</v>
       </c>
       <c r="D157" t="s">
         <v>26</v>
@@ -3399,10 +3579,10 @@
         <v>4</v>
       </c>
       <c r="B158" t="s">
-        <v>8</v>
+        <v>211</v>
       </c>
       <c r="C158" t="s">
-        <v>211</v>
+        <v>9</v>
       </c>
       <c r="D158" t="s">
         <v>212</v>
@@ -3413,10 +3593,10 @@
         <v>4</v>
       </c>
       <c r="B159" t="s">
-        <v>93</v>
+        <v>213</v>
       </c>
       <c r="C159" t="s">
-        <v>213</v>
+        <v>94</v>
       </c>
       <c r="D159" t="s">
         <v>7</v>
@@ -3427,10 +3607,10 @@
         <v>4</v>
       </c>
       <c r="B160" t="s">
-        <v>93</v>
+        <v>214</v>
       </c>
       <c r="C160" t="s">
-        <v>214</v>
+        <v>94</v>
       </c>
       <c r="D160" t="s">
         <v>7</v>
@@ -3441,10 +3621,10 @@
         <v>4</v>
       </c>
       <c r="B161" t="s">
-        <v>19</v>
+        <v>215</v>
       </c>
       <c r="C161" t="s">
-        <v>215</v>
+        <v>20</v>
       </c>
       <c r="D161" t="s">
         <v>10</v>
@@ -3483,10 +3663,10 @@
         <v>4</v>
       </c>
       <c r="B164" t="s">
-        <v>11</v>
+        <v>219</v>
       </c>
       <c r="C164" t="s">
-        <v>219</v>
+        <v>12</v>
       </c>
       <c r="D164" t="s">
         <v>10</v>
@@ -3497,10 +3677,10 @@
         <v>4</v>
       </c>
       <c r="B165" t="s">
-        <v>31</v>
+        <v>220</v>
       </c>
       <c r="C165" t="s">
-        <v>220</v>
+        <v>32</v>
       </c>
       <c r="D165" t="s">
         <v>221</v>
@@ -3511,10 +3691,10 @@
         <v>4</v>
       </c>
       <c r="B166" t="s">
-        <v>112</v>
+        <v>222</v>
       </c>
       <c r="C166" t="s">
-        <v>222</v>
+        <v>113</v>
       </c>
       <c r="D166" t="s">
         <v>114</v>
@@ -3539,10 +3719,10 @@
         <v>4</v>
       </c>
       <c r="B168" t="s">
-        <v>52</v>
+        <v>225</v>
       </c>
       <c r="C168" t="s">
-        <v>225</v>
+        <v>53</v>
       </c>
       <c r="D168" t="s">
         <v>226</v>
@@ -3553,10 +3733,10 @@
         <v>4</v>
       </c>
       <c r="B169" t="s">
-        <v>85</v>
+        <v>227</v>
       </c>
       <c r="C169" t="s">
-        <v>227</v>
+        <v>86</v>
       </c>
       <c r="D169" t="s">
         <v>10</v>
@@ -3567,10 +3747,10 @@
         <v>4</v>
       </c>
       <c r="B170" t="s">
-        <v>93</v>
+        <v>228</v>
       </c>
       <c r="C170" t="s">
-        <v>228</v>
+        <v>94</v>
       </c>
       <c r="D170" t="s">
         <v>7</v>
@@ -3581,10 +3761,10 @@
         <v>4</v>
       </c>
       <c r="B171" t="s">
-        <v>93</v>
+        <v>228</v>
       </c>
       <c r="C171" t="s">
-        <v>228</v>
+        <v>94</v>
       </c>
       <c r="D171" t="s">
         <v>229</v>
@@ -3595,10 +3775,10 @@
         <v>4</v>
       </c>
       <c r="B172" t="s">
-        <v>39</v>
+        <v>230</v>
       </c>
       <c r="C172" t="s">
-        <v>230</v>
+        <v>40</v>
       </c>
       <c r="D172" t="s">
         <v>41</v>
@@ -3609,10 +3789,10 @@
         <v>4</v>
       </c>
       <c r="B173" t="s">
-        <v>104</v>
+        <v>231</v>
       </c>
       <c r="C173" t="s">
-        <v>231</v>
+        <v>105</v>
       </c>
       <c r="D173" t="s">
         <v>7</v>
@@ -3623,10 +3803,10 @@
         <v>4</v>
       </c>
       <c r="B174" t="s">
-        <v>104</v>
+        <v>231</v>
       </c>
       <c r="C174" t="s">
-        <v>231</v>
+        <v>105</v>
       </c>
       <c r="D174" t="s">
         <v>41</v>
@@ -3637,10 +3817,10 @@
         <v>4</v>
       </c>
       <c r="B175" t="s">
-        <v>104</v>
+        <v>231</v>
       </c>
       <c r="C175" t="s">
-        <v>231</v>
+        <v>105</v>
       </c>
       <c r="D175" t="s">
         <v>76</v>
@@ -3651,10 +3831,10 @@
         <v>4</v>
       </c>
       <c r="B176" t="s">
-        <v>49</v>
+        <v>232</v>
       </c>
       <c r="C176" t="s">
-        <v>232</v>
+        <v>50</v>
       </c>
       <c r="D176" t="s">
         <v>7</v>
@@ -3721,10 +3901,10 @@
         <v>4</v>
       </c>
       <c r="B181" t="s">
-        <v>11</v>
+        <v>239</v>
       </c>
       <c r="C181" t="s">
-        <v>239</v>
+        <v>12</v>
       </c>
       <c r="D181" t="s">
         <v>10</v>
@@ -3735,10 +3915,10 @@
         <v>4</v>
       </c>
       <c r="B182" t="s">
-        <v>19</v>
+        <v>240</v>
       </c>
       <c r="C182" t="s">
-        <v>240</v>
+        <v>20</v>
       </c>
       <c r="D182" t="s">
         <v>10</v>
@@ -3763,10 +3943,10 @@
         <v>4</v>
       </c>
       <c r="B184" t="s">
-        <v>170</v>
+        <v>243</v>
       </c>
       <c r="C184" t="s">
-        <v>243</v>
+        <v>171</v>
       </c>
       <c r="D184" t="s">
         <v>172</v>
@@ -3777,10 +3957,10 @@
         <v>4</v>
       </c>
       <c r="B185" t="s">
-        <v>170</v>
+        <v>243</v>
       </c>
       <c r="C185" t="s">
-        <v>243</v>
+        <v>171</v>
       </c>
       <c r="D185" t="s">
         <v>244</v>
@@ -3791,10 +3971,10 @@
         <v>4</v>
       </c>
       <c r="B186" t="s">
-        <v>49</v>
+        <v>245</v>
       </c>
       <c r="C186" t="s">
-        <v>245</v>
+        <v>50</v>
       </c>
       <c r="D186" t="s">
         <v>51</v>
@@ -3805,10 +3985,10 @@
         <v>4</v>
       </c>
       <c r="B187" t="s">
-        <v>8</v>
+        <v>246</v>
       </c>
       <c r="C187" t="s">
-        <v>246</v>
+        <v>9</v>
       </c>
       <c r="D187" t="s">
         <v>59</v>
@@ -3833,10 +4013,10 @@
         <v>4</v>
       </c>
       <c r="B189" t="s">
-        <v>93</v>
+        <v>250</v>
       </c>
       <c r="C189" t="s">
-        <v>250</v>
+        <v>94</v>
       </c>
       <c r="D189" t="s">
         <v>7</v>
@@ -3847,10 +4027,10 @@
         <v>4</v>
       </c>
       <c r="B190" t="s">
-        <v>11</v>
+        <v>251</v>
       </c>
       <c r="C190" t="s">
-        <v>251</v>
+        <v>12</v>
       </c>
       <c r="D190" t="s">
         <v>10</v>
@@ -3861,10 +4041,10 @@
         <v>4</v>
       </c>
       <c r="B191" t="s">
-        <v>52</v>
+        <v>252</v>
       </c>
       <c r="C191" t="s">
-        <v>252</v>
+        <v>53</v>
       </c>
       <c r="D191" t="s">
         <v>10</v>
@@ -3875,10 +4055,10 @@
         <v>4</v>
       </c>
       <c r="B192" t="s">
-        <v>104</v>
+        <v>253</v>
       </c>
       <c r="C192" t="s">
-        <v>253</v>
+        <v>105</v>
       </c>
       <c r="D192" t="s">
         <v>7</v>
@@ -3889,10 +4069,10 @@
         <v>4</v>
       </c>
       <c r="B193" t="s">
-        <v>8</v>
+        <v>254</v>
       </c>
       <c r="C193" t="s">
-        <v>254</v>
+        <v>9</v>
       </c>
       <c r="D193" t="s">
         <v>51</v>
@@ -3903,10 +4083,10 @@
         <v>4</v>
       </c>
       <c r="B194" t="s">
-        <v>8</v>
+        <v>254</v>
       </c>
       <c r="C194" t="s">
-        <v>254</v>
+        <v>9</v>
       </c>
       <c r="D194" t="s">
         <v>7</v>
@@ -3917,10 +4097,10 @@
         <v>4</v>
       </c>
       <c r="B195" t="s">
-        <v>8</v>
+        <v>254</v>
       </c>
       <c r="C195" t="s">
-        <v>254</v>
+        <v>9</v>
       </c>
       <c r="D195" t="s">
         <v>15</v>
@@ -3931,10 +4111,10 @@
         <v>4</v>
       </c>
       <c r="B196" t="s">
-        <v>8</v>
+        <v>255</v>
       </c>
       <c r="C196" t="s">
-        <v>255</v>
+        <v>9</v>
       </c>
       <c r="D196" t="s">
         <v>28</v>
@@ -3945,10 +4125,10 @@
         <v>4</v>
       </c>
       <c r="B197" t="s">
-        <v>8</v>
+        <v>256</v>
       </c>
       <c r="C197" t="s">
-        <v>256</v>
+        <v>9</v>
       </c>
       <c r="D197" t="s">
         <v>7</v>
@@ -3973,10 +4153,10 @@
         <v>4</v>
       </c>
       <c r="B199" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="C199" t="s">
-        <v>260</v>
+        <v>201</v>
       </c>
       <c r="D199" t="s">
         <v>7</v>
@@ -3987,10 +4167,10 @@
         <v>4</v>
       </c>
       <c r="B200" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="C200" t="s">
-        <v>260</v>
+        <v>201</v>
       </c>
       <c r="D200" t="s">
         <v>261</v>
@@ -4001,10 +4181,10 @@
         <v>4</v>
       </c>
       <c r="B201" t="s">
-        <v>85</v>
+        <v>262</v>
       </c>
       <c r="C201" t="s">
-        <v>262</v>
+        <v>86</v>
       </c>
       <c r="D201" t="s">
         <v>263</v>
@@ -4015,10 +4195,10 @@
         <v>4</v>
       </c>
       <c r="B202" t="s">
-        <v>85</v>
+        <v>262</v>
       </c>
       <c r="C202" t="s">
-        <v>262</v>
+        <v>86</v>
       </c>
       <c r="D202" t="s">
         <v>7</v>
@@ -4029,10 +4209,10 @@
         <v>4</v>
       </c>
       <c r="B203" t="s">
-        <v>19</v>
+        <v>264</v>
       </c>
       <c r="C203" t="s">
-        <v>264</v>
+        <v>20</v>
       </c>
       <c r="D203" t="s">
         <v>10</v>
@@ -4043,10 +4223,10 @@
         <v>4</v>
       </c>
       <c r="B204" t="s">
-        <v>29</v>
+        <v>265</v>
       </c>
       <c r="C204" t="s">
-        <v>265</v>
+        <v>30</v>
       </c>
       <c r="D204" t="s">
         <v>102</v>
@@ -4057,13 +4237,1001 @@
         <v>4</v>
       </c>
       <c r="B205" t="s">
-        <v>29</v>
+        <v>265</v>
       </c>
       <c r="C205" t="s">
-        <v>265</v>
+        <v>30</v>
       </c>
       <c r="D205" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="s">
+        <v>266</v>
+      </c>
+      <c r="B206" t="s">
+        <v>267</v>
+      </c>
+      <c r="C206" t="s">
+        <v>268</v>
+      </c>
+      <c r="D206" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="s">
+        <v>266</v>
+      </c>
+      <c r="B207" t="s">
+        <v>270</v>
+      </c>
+      <c r="C207" t="s">
+        <v>268</v>
+      </c>
+      <c r="D207" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="s">
+        <v>266</v>
+      </c>
+      <c r="B208" t="s">
+        <v>271</v>
+      </c>
+      <c r="C208" t="s">
+        <v>268</v>
+      </c>
+      <c r="D208" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="s">
+        <v>266</v>
+      </c>
+      <c r="B209" t="s">
+        <v>272</v>
+      </c>
+      <c r="C209" t="s">
+        <v>268</v>
+      </c>
+      <c r="D209" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="s">
+        <v>266</v>
+      </c>
+      <c r="B210" t="s">
+        <v>273</v>
+      </c>
+      <c r="C210" t="s">
+        <v>268</v>
+      </c>
+      <c r="D210" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="s">
+        <v>266</v>
+      </c>
+      <c r="B211" t="s">
+        <v>273</v>
+      </c>
+      <c r="C211" t="s">
+        <v>268</v>
+      </c>
+      <c r="D211" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="s">
+        <v>266</v>
+      </c>
+      <c r="B212" t="s">
+        <v>275</v>
+      </c>
+      <c r="C212" t="s">
+        <v>268</v>
+      </c>
+      <c r="D212" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="s">
+        <v>266</v>
+      </c>
+      <c r="B213" t="s">
+        <v>276</v>
+      </c>
+      <c r="C213" t="s">
+        <v>268</v>
+      </c>
+      <c r="D213" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="s">
+        <v>266</v>
+      </c>
+      <c r="B214" t="s">
+        <v>277</v>
+      </c>
+      <c r="C214" t="s">
+        <v>268</v>
+      </c>
+      <c r="D214" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="s">
+        <v>266</v>
+      </c>
+      <c r="B215" t="s">
+        <v>278</v>
+      </c>
+      <c r="C215" t="s">
+        <v>268</v>
+      </c>
+      <c r="D215" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="s">
+        <v>266</v>
+      </c>
+      <c r="B216" t="s">
+        <v>279</v>
+      </c>
+      <c r="C216" t="s">
+        <v>268</v>
+      </c>
+      <c r="D216" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="s">
+        <v>266</v>
+      </c>
+      <c r="B217" t="s">
+        <v>280</v>
+      </c>
+      <c r="C217" t="s">
+        <v>268</v>
+      </c>
+      <c r="D217" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="s">
+        <v>266</v>
+      </c>
+      <c r="B218" t="s">
+        <v>281</v>
+      </c>
+      <c r="C218" t="s">
+        <v>268</v>
+      </c>
+      <c r="D218" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="s">
+        <v>266</v>
+      </c>
+      <c r="B219" t="s">
+        <v>282</v>
+      </c>
+      <c r="C219" t="s">
+        <v>268</v>
+      </c>
+      <c r="D219" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="s">
+        <v>266</v>
+      </c>
+      <c r="B220" t="s">
+        <v>283</v>
+      </c>
+      <c r="C220" t="s">
+        <v>268</v>
+      </c>
+      <c r="D220" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="s">
+        <v>266</v>
+      </c>
+      <c r="B221" t="s">
+        <v>284</v>
+      </c>
+      <c r="C221" t="s">
+        <v>268</v>
+      </c>
+      <c r="D221" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="s">
+        <v>266</v>
+      </c>
+      <c r="B222" t="s">
+        <v>286</v>
+      </c>
+      <c r="C222" t="s">
+        <v>268</v>
+      </c>
+      <c r="D222" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="s">
+        <v>266</v>
+      </c>
+      <c r="B223" t="s">
+        <v>287</v>
+      </c>
+      <c r="C223" t="s">
+        <v>268</v>
+      </c>
+      <c r="D223" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="s">
+        <v>266</v>
+      </c>
+      <c r="B224" t="s">
+        <v>288</v>
+      </c>
+      <c r="C224" t="s">
+        <v>268</v>
+      </c>
+      <c r="D224" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="s">
+        <v>266</v>
+      </c>
+      <c r="B225" t="s">
+        <v>289</v>
+      </c>
+      <c r="C225" t="s">
+        <v>268</v>
+      </c>
+      <c r="D225" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="s">
+        <v>266</v>
+      </c>
+      <c r="B226" t="s">
+        <v>290</v>
+      </c>
+      <c r="C226" t="s">
+        <v>268</v>
+      </c>
+      <c r="D226" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="s">
+        <v>266</v>
+      </c>
+      <c r="B227" t="s">
+        <v>291</v>
+      </c>
+      <c r="C227" t="s">
+        <v>268</v>
+      </c>
+      <c r="D227" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="s">
+        <v>266</v>
+      </c>
+      <c r="B228" t="s">
+        <v>292</v>
+      </c>
+      <c r="C228" t="s">
+        <v>268</v>
+      </c>
+      <c r="D228" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="s">
+        <v>266</v>
+      </c>
+      <c r="B229" t="s">
+        <v>293</v>
+      </c>
+      <c r="C229" t="s">
+        <v>268</v>
+      </c>
+      <c r="D229" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="s">
+        <v>266</v>
+      </c>
+      <c r="B230" t="s">
+        <v>294</v>
+      </c>
+      <c r="C230" t="s">
+        <v>268</v>
+      </c>
+      <c r="D230" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="s">
+        <v>266</v>
+      </c>
+      <c r="B231" t="s">
+        <v>295</v>
+      </c>
+      <c r="C231" t="s">
+        <v>268</v>
+      </c>
+      <c r="D231" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="s">
+        <v>266</v>
+      </c>
+      <c r="B232" t="s">
+        <v>296</v>
+      </c>
+      <c r="C232" t="s">
+        <v>268</v>
+      </c>
+      <c r="D232" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="s">
+        <v>266</v>
+      </c>
+      <c r="B233" t="s">
+        <v>297</v>
+      </c>
+      <c r="C233" t="s">
+        <v>268</v>
+      </c>
+      <c r="D233" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="s">
+        <v>266</v>
+      </c>
+      <c r="B234" t="s">
+        <v>298</v>
+      </c>
+      <c r="C234" t="s">
+        <v>268</v>
+      </c>
+      <c r="D234" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="s">
+        <v>188</v>
+      </c>
+      <c r="B235" t="s">
+        <v>299</v>
+      </c>
+      <c r="C235" t="s">
+        <v>268</v>
+      </c>
+      <c r="D235" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="s">
+        <v>188</v>
+      </c>
+      <c r="B236" t="s">
+        <v>301</v>
+      </c>
+      <c r="C236" t="s">
+        <v>268</v>
+      </c>
+      <c r="D236" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="s">
+        <v>188</v>
+      </c>
+      <c r="B237" t="s">
+        <v>301</v>
+      </c>
+      <c r="C237" t="s">
+        <v>268</v>
+      </c>
+      <c r="D237" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="s">
+        <v>188</v>
+      </c>
+      <c r="B238" t="s">
+        <v>301</v>
+      </c>
+      <c r="C238" t="s">
+        <v>268</v>
+      </c>
+      <c r="D238" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="s">
+        <v>188</v>
+      </c>
+      <c r="B239" t="s">
+        <v>301</v>
+      </c>
+      <c r="C239" t="s">
+        <v>268</v>
+      </c>
+      <c r="D239" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="s">
+        <v>188</v>
+      </c>
+      <c r="B240" t="s">
+        <v>301</v>
+      </c>
+      <c r="C240" t="s">
+        <v>268</v>
+      </c>
+      <c r="D240" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="s">
+        <v>188</v>
+      </c>
+      <c r="B241" t="s">
+        <v>301</v>
+      </c>
+      <c r="C241" t="s">
+        <v>268</v>
+      </c>
+      <c r="D241" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="s">
+        <v>188</v>
+      </c>
+      <c r="B242" t="s">
+        <v>307</v>
+      </c>
+      <c r="C242" t="s">
+        <v>268</v>
+      </c>
+      <c r="D242" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="s">
+        <v>188</v>
+      </c>
+      <c r="B243" t="s">
+        <v>308</v>
+      </c>
+      <c r="C243" t="s">
+        <v>268</v>
+      </c>
+      <c r="D243" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="s">
+        <v>188</v>
+      </c>
+      <c r="B244" t="s">
+        <v>309</v>
+      </c>
+      <c r="C244" t="s">
+        <v>268</v>
+      </c>
+      <c r="D244" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="s">
+        <v>188</v>
+      </c>
+      <c r="B245" t="s">
+        <v>301</v>
+      </c>
+      <c r="C245" t="s">
+        <v>268</v>
+      </c>
+      <c r="D245" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="s">
+        <v>188</v>
+      </c>
+      <c r="B246" t="s">
+        <v>301</v>
+      </c>
+      <c r="C246" t="s">
+        <v>268</v>
+      </c>
+      <c r="D246" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="s">
+        <v>188</v>
+      </c>
+      <c r="B247" t="s">
+        <v>301</v>
+      </c>
+      <c r="C247" t="s">
+        <v>268</v>
+      </c>
+      <c r="D247" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="s">
+        <v>188</v>
+      </c>
+      <c r="B248" t="s">
+        <v>301</v>
+      </c>
+      <c r="C248" t="s">
+        <v>268</v>
+      </c>
+      <c r="D248" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="s">
+        <v>188</v>
+      </c>
+      <c r="B249" t="s">
+        <v>310</v>
+      </c>
+      <c r="C249" t="s">
+        <v>268</v>
+      </c>
+      <c r="D249" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="s">
+        <v>188</v>
+      </c>
+      <c r="B250" t="s">
+        <v>312</v>
+      </c>
+      <c r="C250" t="s">
+        <v>268</v>
+      </c>
+      <c r="D250"/>
+    </row>
+    <row r="251">
+      <c r="A251" t="s">
+        <v>188</v>
+      </c>
+      <c r="B251" t="s">
+        <v>313</v>
+      </c>
+      <c r="C251" t="s">
+        <v>268</v>
+      </c>
+      <c r="D251" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="s">
+        <v>188</v>
+      </c>
+      <c r="B252" t="s">
+        <v>314</v>
+      </c>
+      <c r="C252" t="s">
+        <v>268</v>
+      </c>
+      <c r="D252" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="s">
+        <v>188</v>
+      </c>
+      <c r="B253" t="s">
+        <v>307</v>
+      </c>
+      <c r="C253" t="s">
+        <v>268</v>
+      </c>
+      <c r="D253" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="s">
+        <v>188</v>
+      </c>
+      <c r="B254" t="s">
+        <v>315</v>
+      </c>
+      <c r="C254" t="s">
+        <v>268</v>
+      </c>
+      <c r="D254" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="s">
+        <v>188</v>
+      </c>
+      <c r="B255" t="s">
+        <v>313</v>
+      </c>
+      <c r="C255" t="s">
+        <v>268</v>
+      </c>
+      <c r="D255" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="s">
+        <v>188</v>
+      </c>
+      <c r="B256" t="s">
+        <v>316</v>
+      </c>
+      <c r="C256" t="s">
+        <v>268</v>
+      </c>
+      <c r="D256" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="s">
+        <v>188</v>
+      </c>
+      <c r="B257" t="s">
+        <v>317</v>
+      </c>
+      <c r="C257" t="s">
+        <v>268</v>
+      </c>
+      <c r="D257" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="s">
+        <v>188</v>
+      </c>
+      <c r="B258" t="s">
+        <v>318</v>
+      </c>
+      <c r="C258" t="s">
+        <v>268</v>
+      </c>
+      <c r="D258"/>
+    </row>
+    <row r="259">
+      <c r="A259" t="s">
+        <v>188</v>
+      </c>
+      <c r="B259" t="s">
+        <v>319</v>
+      </c>
+      <c r="C259" t="s">
+        <v>268</v>
+      </c>
+      <c r="D259" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="s">
+        <v>188</v>
+      </c>
+      <c r="B260" t="s">
+        <v>227</v>
+      </c>
+      <c r="C260" t="s">
+        <v>268</v>
+      </c>
+      <c r="D260" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="s">
+        <v>188</v>
+      </c>
+      <c r="B261" t="s">
+        <v>320</v>
+      </c>
+      <c r="C261" t="s">
+        <v>268</v>
+      </c>
+      <c r="D261" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="s">
+        <v>188</v>
+      </c>
+      <c r="B262" t="s">
+        <v>307</v>
+      </c>
+      <c r="C262" t="s">
+        <v>268</v>
+      </c>
+      <c r="D262" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="s">
+        <v>188</v>
+      </c>
+      <c r="B263" t="s">
+        <v>196</v>
+      </c>
+      <c r="C263" t="s">
+        <v>268</v>
+      </c>
+      <c r="D263" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="s">
+        <v>188</v>
+      </c>
+      <c r="B264" t="s">
+        <v>307</v>
+      </c>
+      <c r="C264" t="s">
+        <v>268</v>
+      </c>
+      <c r="D264" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="s">
+        <v>188</v>
+      </c>
+      <c r="B265" t="s">
+        <v>321</v>
+      </c>
+      <c r="C265" t="s">
+        <v>268</v>
+      </c>
+      <c r="D265"/>
+    </row>
+    <row r="266">
+      <c r="A266" t="s">
+        <v>188</v>
+      </c>
+      <c r="B266" t="s">
+        <v>322</v>
+      </c>
+      <c r="C266" t="s">
+        <v>268</v>
+      </c>
+      <c r="D266" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="s">
+        <v>188</v>
+      </c>
+      <c r="B267" t="s">
+        <v>309</v>
+      </c>
+      <c r="C267" t="s">
+        <v>268</v>
+      </c>
+      <c r="D267" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="s">
+        <v>188</v>
+      </c>
+      <c r="B268" t="s">
+        <v>323</v>
+      </c>
+      <c r="C268" t="s">
+        <v>268</v>
+      </c>
+      <c r="D268" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="s">
+        <v>188</v>
+      </c>
+      <c r="B269" t="s">
+        <v>323</v>
+      </c>
+      <c r="C269" t="s">
+        <v>268</v>
+      </c>
+      <c r="D269" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="s">
+        <v>188</v>
+      </c>
+      <c r="B270" t="s">
+        <v>323</v>
+      </c>
+      <c r="C270" t="s">
+        <v>268</v>
+      </c>
+      <c r="D270" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="s">
+        <v>188</v>
+      </c>
+      <c r="B271" t="s">
+        <v>323</v>
+      </c>
+      <c r="C271" t="s">
+        <v>268</v>
+      </c>
+      <c r="D271" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="s">
+        <v>188</v>
+      </c>
+      <c r="B272" t="s">
+        <v>323</v>
+      </c>
+      <c r="C272" t="s">
+        <v>268</v>
+      </c>
+      <c r="D272" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="s">
+        <v>188</v>
+      </c>
+      <c r="B273" t="s">
+        <v>324</v>
+      </c>
+      <c r="C273" t="s">
+        <v>268</v>
+      </c>
+      <c r="D273" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="s">
+        <v>188</v>
+      </c>
+      <c r="B274" t="s">
+        <v>325</v>
+      </c>
+      <c r="C274" t="s">
+        <v>268</v>
+      </c>
+      <c r="D274" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="s">
+        <v>188</v>
+      </c>
+      <c r="B275" t="s">
+        <v>301</v>
+      </c>
+      <c r="C275" t="s">
+        <v>268</v>
+      </c>
+      <c r="D275" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="s">
+        <v>188</v>
+      </c>
+      <c r="B276" t="s">
+        <v>196</v>
+      </c>
+      <c r="C276" t="s">
+        <v>268</v>
+      </c>
+      <c r="D276" t="s">
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactored ryanair fare finder due to layout change. Begin of email sender
</commit_message>
<xml_diff>
--- a/src/data/flights.xlsx
+++ b/src/data/flights.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\workspace\Flight Fare Finder\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView windowHeight="12210" windowWidth="28800" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
-    <sheet name="Czech Republic" r:id="rId1" sheetId="1"/>
+    <sheet name="Czech Republic" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Czech Republic'!$A$1:$D$1</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -392,9 +395,6 @@
     <t>Kefallinia</t>
   </si>
   <si>
-    <t>Keflavik</t>
-  </si>
-  <si>
     <t>Iceland</t>
   </si>
   <si>
@@ -1002,13 +1002,15 @@
   </si>
   <si>
     <t>ALMERIA</t>
+  </si>
+  <si>
+    <t>Reykjavik</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1043,17 +1045,17 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normální" xfId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1070,10 +1072,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1108,7 +1110,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1160,7 +1162,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1271,21 +1273,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1302,7 +1304,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1354,26 +1356,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D276"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="H78" sqref="H78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1390,7 +1392,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1404,7 +1406,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1418,7 +1420,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1432,7 +1434,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1446,7 +1448,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1460,7 +1462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1474,7 +1476,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1488,7 +1490,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1502,7 +1504,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1516,7 +1518,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1530,7 +1532,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1544,7 +1546,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1558,7 +1560,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1572,7 +1574,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -1586,7 +1588,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -1600,7 +1602,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1614,7 +1616,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -1628,7 +1630,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -1642,7 +1644,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -1656,7 +1658,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -1670,7 +1672,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -1684,7 +1686,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -1698,7 +1700,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -1712,7 +1714,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -1726,7 +1728,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -1740,7 +1742,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -1754,7 +1756,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -1768,7 +1770,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1782,7 +1784,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -1796,7 +1798,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -1810,7 +1812,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -1824,7 +1826,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -1838,7 +1840,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -1852,7 +1854,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -1866,7 +1868,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -1880,7 +1882,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -1894,7 +1896,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>4</v>
       </c>
@@ -1908,7 +1910,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>4</v>
       </c>
@@ -1922,7 +1924,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>4</v>
       </c>
@@ -1936,7 +1938,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>4</v>
       </c>
@@ -1950,7 +1952,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>4</v>
       </c>
@@ -1964,7 +1966,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>4</v>
       </c>
@@ -1978,7 +1980,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>4</v>
       </c>
@@ -1992,7 +1994,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>4</v>
       </c>
@@ -2006,7 +2008,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -2020,7 +2022,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>4</v>
       </c>
@@ -2034,7 +2036,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>4</v>
       </c>
@@ -2048,7 +2050,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>4</v>
       </c>
@@ -2062,7 +2064,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>4</v>
       </c>
@@ -2076,7 +2078,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>4</v>
       </c>
@@ -2090,7 +2092,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>4</v>
       </c>
@@ -2104,7 +2106,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>4</v>
       </c>
@@ -2118,7 +2120,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>4</v>
       </c>
@@ -2132,7 +2134,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>4</v>
       </c>
@@ -2146,7 +2148,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>4</v>
       </c>
@@ -2160,7 +2162,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>4</v>
       </c>
@@ -2174,7 +2176,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>4</v>
       </c>
@@ -2188,7 +2190,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>4</v>
       </c>
@@ -2202,7 +2204,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>4</v>
       </c>
@@ -2216,7 +2218,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>4</v>
       </c>
@@ -2230,7 +2232,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>4</v>
       </c>
@@ -2244,7 +2246,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>4</v>
       </c>
@@ -2258,7 +2260,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>4</v>
       </c>
@@ -2272,7 +2274,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>4</v>
       </c>
@@ -2286,7 +2288,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>4</v>
       </c>
@@ -2300,7 +2302,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>4</v>
       </c>
@@ -2314,7 +2316,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>4</v>
       </c>
@@ -2328,7 +2330,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>4</v>
       </c>
@@ -2342,7 +2344,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>4</v>
       </c>
@@ -2356,7 +2358,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>4</v>
       </c>
@@ -2370,7 +2372,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>4</v>
       </c>
@@ -2384,7 +2386,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>4</v>
       </c>
@@ -2398,7 +2400,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>4</v>
       </c>
@@ -2412,7 +2414,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>4</v>
       </c>
@@ -2426,7 +2428,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>4</v>
       </c>
@@ -2440,7 +2442,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>4</v>
       </c>
@@ -2454,7 +2456,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>4</v>
       </c>
@@ -2468,7 +2470,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>4</v>
       </c>
@@ -2482,68 +2484,68 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>4</v>
       </c>
       <c r="B80" t="s">
+        <v>325</v>
+      </c>
+      <c r="C80" t="s">
         <v>122</v>
-      </c>
-      <c r="C80" t="s">
-        <v>123</v>
       </c>
       <c r="D80" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>4</v>
       </c>
       <c r="B81" t="s">
+        <v>325</v>
+      </c>
+      <c r="C81" t="s">
         <v>122</v>
-      </c>
-      <c r="C81" t="s">
-        <v>123</v>
       </c>
       <c r="D81" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>4</v>
       </c>
       <c r="B82" t="s">
+        <v>123</v>
+      </c>
+      <c r="C82" t="s">
         <v>124</v>
-      </c>
-      <c r="C82" t="s">
-        <v>125</v>
       </c>
       <c r="D82" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>4</v>
       </c>
       <c r="B83" t="s">
+        <v>123</v>
+      </c>
+      <c r="C83" t="s">
         <v>124</v>
       </c>
-      <c r="C83" t="s">
+      <c r="D83" t="s">
         <v>125</v>
       </c>
-      <c r="D83" t="s">
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>4</v>
+      </c>
+      <c r="B84" t="s">
         <v>126</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="s">
-        <v>4</v>
-      </c>
-      <c r="B84" t="s">
-        <v>127</v>
       </c>
       <c r="C84" t="s">
         <v>20</v>
@@ -2552,12 +2554,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>4</v>
       </c>
       <c r="B85" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C85" t="s">
         <v>55</v>
@@ -2566,26 +2568,26 @@
         <v>7</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>4</v>
       </c>
       <c r="B86" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C86" t="s">
         <v>94</v>
       </c>
       <c r="D86" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>4</v>
+      </c>
+      <c r="B87" t="s">
         <v>130</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="s">
-        <v>4</v>
-      </c>
-      <c r="B87" t="s">
-        <v>131</v>
       </c>
       <c r="C87" t="s">
         <v>9</v>
@@ -2594,12 +2596,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>4</v>
       </c>
       <c r="B88" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C88" t="s">
         <v>12</v>
@@ -2608,26 +2610,26 @@
         <v>10</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>4</v>
       </c>
       <c r="B89" t="s">
+        <v>132</v>
+      </c>
+      <c r="C89" t="s">
         <v>133</v>
-      </c>
-      <c r="C89" t="s">
-        <v>134</v>
       </c>
       <c r="D89" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>4</v>
       </c>
       <c r="B90" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C90" t="s">
         <v>12</v>
@@ -2636,12 +2638,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>4</v>
       </c>
       <c r="B91" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C91" t="s">
         <v>47</v>
@@ -2650,12 +2652,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>4</v>
       </c>
       <c r="B92" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C92" t="s">
         <v>105</v>
@@ -2664,12 +2666,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>4</v>
       </c>
       <c r="B93" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C93" t="s">
         <v>97</v>
@@ -2678,26 +2680,26 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>4</v>
       </c>
       <c r="B94" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C94" t="s">
         <v>97</v>
       </c>
       <c r="D94" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>4</v>
+      </c>
+      <c r="B95" t="s">
         <v>139</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="s">
-        <v>4</v>
-      </c>
-      <c r="B95" t="s">
-        <v>140</v>
       </c>
       <c r="C95" t="s">
         <v>47</v>
@@ -2706,26 +2708,26 @@
         <v>59</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>4</v>
       </c>
       <c r="B96" t="s">
+        <v>140</v>
+      </c>
+      <c r="C96" t="s">
         <v>141</v>
       </c>
-      <c r="C96" t="s">
+      <c r="D96" t="s">
         <v>142</v>
       </c>
-      <c r="D96" t="s">
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>4</v>
+      </c>
+      <c r="B97" t="s">
         <v>143</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="s">
-        <v>4</v>
-      </c>
-      <c r="B97" t="s">
-        <v>144</v>
       </c>
       <c r="C97" t="s">
         <v>47</v>
@@ -2734,12 +2736,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>4</v>
       </c>
       <c r="B98" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C98" t="s">
         <v>47</v>
@@ -2748,26 +2750,26 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>4</v>
       </c>
       <c r="B99" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C99" t="s">
         <v>47</v>
       </c>
       <c r="D99" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>4</v>
+      </c>
+      <c r="B100" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="s">
-        <v>4</v>
-      </c>
-      <c r="B100" t="s">
-        <v>147</v>
       </c>
       <c r="C100" t="s">
         <v>47</v>
@@ -2776,26 +2778,26 @@
         <v>28</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>4</v>
       </c>
       <c r="B101" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C101" t="s">
         <v>47</v>
       </c>
       <c r="D101" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>4</v>
+      </c>
+      <c r="B102" t="s">
         <v>149</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="s">
-        <v>4</v>
-      </c>
-      <c r="B102" t="s">
-        <v>150</v>
       </c>
       <c r="C102" t="s">
         <v>47</v>
@@ -2804,12 +2806,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>4</v>
       </c>
       <c r="B103" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C103" t="s">
         <v>47</v>
@@ -2818,40 +2820,40 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>4</v>
       </c>
       <c r="B104" t="s">
+        <v>150</v>
+      </c>
+      <c r="C104" t="s">
+        <v>150</v>
+      </c>
+      <c r="D104" t="s">
         <v>151</v>
       </c>
-      <c r="C104" t="s">
-        <v>151</v>
-      </c>
-      <c r="D104" t="s">
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>4</v>
+      </c>
+      <c r="B105" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="s">
-        <v>4</v>
-      </c>
-      <c r="B105" t="s">
-        <v>153</v>
       </c>
       <c r="C105" t="s">
         <v>50</v>
       </c>
       <c r="D105" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>4</v>
+      </c>
+      <c r="B106" t="s">
         <v>154</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="s">
-        <v>4</v>
-      </c>
-      <c r="B106" t="s">
-        <v>155</v>
       </c>
       <c r="C106" t="s">
         <v>97</v>
@@ -2860,12 +2862,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>4</v>
       </c>
       <c r="B107" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C107" t="s">
         <v>12</v>
@@ -2874,26 +2876,26 @@
         <v>7</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>4</v>
       </c>
       <c r="B108" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C108" t="s">
         <v>12</v>
       </c>
       <c r="D108" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>4</v>
+      </c>
+      <c r="B109" t="s">
         <v>157</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="s">
-        <v>4</v>
-      </c>
-      <c r="B109" t="s">
-        <v>158</v>
       </c>
       <c r="C109" t="s">
         <v>12</v>
@@ -2902,40 +2904,40 @@
         <v>10</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>4</v>
       </c>
       <c r="B110" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C110" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D110" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>4</v>
       </c>
       <c r="B111" t="s">
+        <v>158</v>
+      </c>
+      <c r="C111" t="s">
+        <v>158</v>
+      </c>
+      <c r="D111" t="s">
         <v>159</v>
       </c>
-      <c r="C111" t="s">
-        <v>159</v>
-      </c>
-      <c r="D111" t="s">
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>4</v>
+      </c>
+      <c r="B112" t="s">
         <v>160</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="s">
-        <v>4</v>
-      </c>
-      <c r="B112" t="s">
-        <v>161</v>
       </c>
       <c r="C112" t="s">
         <v>47</v>
@@ -2944,12 +2946,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>4</v>
       </c>
       <c r="B113" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C113" t="s">
         <v>47</v>
@@ -2958,12 +2960,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>4</v>
       </c>
       <c r="B114" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C114" t="s">
         <v>113</v>
@@ -2972,12 +2974,12 @@
         <v>114</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>4</v>
       </c>
       <c r="B115" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C115" t="s">
         <v>113</v>
@@ -2986,12 +2988,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="116">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>4</v>
       </c>
       <c r="B116" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C116" t="s">
         <v>50</v>
@@ -3000,12 +3002,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="117">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>4</v>
       </c>
       <c r="B117" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C117" t="s">
         <v>12</v>
@@ -3014,12 +3016,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="118">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>4</v>
       </c>
       <c r="B118" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C118" t="s">
         <v>9</v>
@@ -3028,12 +3030,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="119">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>4</v>
       </c>
       <c r="B119" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C119" t="s">
         <v>9</v>
@@ -3042,12 +3044,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="120">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>4</v>
       </c>
       <c r="B120" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C120" t="s">
         <v>9</v>
@@ -3056,12 +3058,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="121">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>4</v>
       </c>
       <c r="B121" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C121" t="s">
         <v>9</v>
@@ -3070,40 +3072,40 @@
         <v>15</v>
       </c>
     </row>
-    <row r="122">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>4</v>
       </c>
       <c r="B122" t="s">
+        <v>166</v>
+      </c>
+      <c r="C122" t="s">
         <v>167</v>
       </c>
-      <c r="C122" t="s">
+      <c r="D122" t="s">
         <v>168</v>
       </c>
-      <c r="D122" t="s">
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>4</v>
+      </c>
+      <c r="B123" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="123">
-      <c r="A123" t="s">
-        <v>4</v>
-      </c>
-      <c r="B123" t="s">
+      <c r="C123" t="s">
         <v>170</v>
       </c>
-      <c r="C123" t="s">
+      <c r="D123" t="s">
         <v>171</v>
       </c>
-      <c r="D123" t="s">
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>4</v>
+      </c>
+      <c r="B124" t="s">
         <v>172</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" t="s">
-        <v>4</v>
-      </c>
-      <c r="B124" t="s">
-        <v>173</v>
       </c>
       <c r="C124" t="s">
         <v>94</v>
@@ -3112,12 +3114,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="125">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>4</v>
       </c>
       <c r="B125" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C125" t="s">
         <v>94</v>
@@ -3126,26 +3128,26 @@
         <v>10</v>
       </c>
     </row>
-    <row r="126">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>4</v>
       </c>
       <c r="B126" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C126" t="s">
         <v>94</v>
       </c>
       <c r="D126" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>4</v>
+      </c>
+      <c r="B127" t="s">
         <v>174</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" t="s">
-        <v>4</v>
-      </c>
-      <c r="B127" t="s">
-        <v>175</v>
       </c>
       <c r="C127" t="s">
         <v>43</v>
@@ -3154,12 +3156,12 @@
         <v>99</v>
       </c>
     </row>
-    <row r="128">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>4</v>
       </c>
       <c r="B128" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C128" t="s">
         <v>50</v>
@@ -3168,12 +3170,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="129">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>4</v>
       </c>
       <c r="B129" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C129" t="s">
         <v>9</v>
@@ -3182,12 +3184,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>4</v>
       </c>
       <c r="B130" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C130" t="s">
         <v>9</v>
@@ -3196,12 +3198,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="131">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>4</v>
       </c>
       <c r="B131" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C131" t="s">
         <v>9</v>
@@ -3210,26 +3212,26 @@
         <v>28</v>
       </c>
     </row>
-    <row r="132">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>4</v>
       </c>
       <c r="B132" t="s">
+        <v>177</v>
+      </c>
+      <c r="C132" t="s">
         <v>178</v>
       </c>
-      <c r="C132" t="s">
+      <c r="D132" t="s">
         <v>179</v>
       </c>
-      <c r="D132" t="s">
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>4</v>
+      </c>
+      <c r="B133" t="s">
         <v>180</v>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" t="s">
-        <v>4</v>
-      </c>
-      <c r="B133" t="s">
-        <v>181</v>
       </c>
       <c r="C133" t="s">
         <v>47</v>
@@ -3238,12 +3240,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="134">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>4</v>
       </c>
       <c r="B134" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C134" t="s">
         <v>50</v>
@@ -3252,40 +3254,40 @@
         <v>7</v>
       </c>
     </row>
-    <row r="135">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>4</v>
       </c>
       <c r="B135" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C135" t="s">
         <v>94</v>
       </c>
       <c r="D135" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>4</v>
+      </c>
+      <c r="B136" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="136">
-      <c r="A136" t="s">
-        <v>4</v>
-      </c>
-      <c r="B136" t="s">
-        <v>185</v>
-      </c>
       <c r="C136" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D136" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="137">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>4</v>
       </c>
       <c r="B137" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C137" t="s">
         <v>9</v>
@@ -3294,12 +3296,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>4</v>
       </c>
       <c r="B138" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C138" t="s">
         <v>40</v>
@@ -3308,26 +3310,26 @@
         <v>41</v>
       </c>
     </row>
-    <row r="139">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>4</v>
       </c>
       <c r="B139" t="s">
+        <v>187</v>
+      </c>
+      <c r="C139" t="s">
         <v>188</v>
-      </c>
-      <c r="C139" t="s">
-        <v>189</v>
       </c>
       <c r="D139" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="140">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>4</v>
       </c>
       <c r="B140" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C140" t="s">
         <v>12</v>
@@ -3336,12 +3338,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="141">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>4</v>
       </c>
       <c r="B141" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C141" t="s">
         <v>50</v>
@@ -3350,12 +3352,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="142">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>4</v>
       </c>
       <c r="B142" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C142" t="s">
         <v>50</v>
@@ -3364,26 +3366,26 @@
         <v>15</v>
       </c>
     </row>
-    <row r="143">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>4</v>
       </c>
       <c r="B143" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C143" t="s">
         <v>50</v>
       </c>
       <c r="D143" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="144">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>4</v>
       </c>
       <c r="B144" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C144" t="s">
         <v>50</v>
@@ -3392,26 +3394,26 @@
         <v>26</v>
       </c>
     </row>
-    <row r="145">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>4</v>
       </c>
       <c r="B145" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C145" t="s">
         <v>50</v>
       </c>
       <c r="D145" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>4</v>
+      </c>
+      <c r="B146" t="s">
         <v>194</v>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" t="s">
-        <v>4</v>
-      </c>
-      <c r="B146" t="s">
-        <v>195</v>
       </c>
       <c r="C146" t="s">
         <v>9</v>
@@ -3420,26 +3422,26 @@
         <v>7</v>
       </c>
     </row>
-    <row r="147">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>4</v>
       </c>
       <c r="B147" t="s">
+        <v>195</v>
+      </c>
+      <c r="C147" t="s">
         <v>196</v>
-      </c>
-      <c r="C147" t="s">
-        <v>197</v>
       </c>
       <c r="D147" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="148">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>4</v>
       </c>
       <c r="B148" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C148" t="s">
         <v>97</v>
@@ -3448,12 +3450,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="149">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>4</v>
       </c>
       <c r="B149" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C149" t="s">
         <v>20</v>
@@ -3462,26 +3464,26 @@
         <v>10</v>
       </c>
     </row>
-    <row r="150">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>4</v>
       </c>
       <c r="B150" t="s">
+        <v>199</v>
+      </c>
+      <c r="C150" t="s">
         <v>200</v>
       </c>
-      <c r="C150" t="s">
+      <c r="D150" t="s">
         <v>201</v>
       </c>
-      <c r="D150" t="s">
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>4</v>
+      </c>
+      <c r="B151" t="s">
         <v>202</v>
-      </c>
-    </row>
-    <row r="151">
-      <c r="A151" t="s">
-        <v>4</v>
-      </c>
-      <c r="B151" t="s">
-        <v>203</v>
       </c>
       <c r="C151" t="s">
         <v>79</v>
@@ -3490,12 +3492,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="152">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>4</v>
       </c>
       <c r="B152" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C152" t="s">
         <v>20</v>
@@ -3504,40 +3506,40 @@
         <v>10</v>
       </c>
     </row>
-    <row r="153">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>4</v>
       </c>
       <c r="B153" t="s">
+        <v>204</v>
+      </c>
+      <c r="C153" t="s">
         <v>205</v>
       </c>
-      <c r="C153" t="s">
+      <c r="D153" t="s">
         <v>206</v>
       </c>
-      <c r="D153" t="s">
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>4</v>
+      </c>
+      <c r="B154" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="154">
-      <c r="A154" t="s">
-        <v>4</v>
-      </c>
-      <c r="B154" t="s">
+      <c r="C154" t="s">
         <v>208</v>
-      </c>
-      <c r="C154" t="s">
-        <v>209</v>
       </c>
       <c r="D154" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="155">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>4</v>
       </c>
       <c r="B155" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C155" t="s">
         <v>9</v>
@@ -3546,12 +3548,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="156">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>4</v>
       </c>
       <c r="B156" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C156" t="s">
         <v>9</v>
@@ -3560,12 +3562,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="157">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>4</v>
       </c>
       <c r="B157" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C157" t="s">
         <v>9</v>
@@ -3574,26 +3576,26 @@
         <v>26</v>
       </c>
     </row>
-    <row r="158">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>4</v>
       </c>
       <c r="B158" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C158" t="s">
         <v>9</v>
       </c>
       <c r="D158" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>4</v>
+      </c>
+      <c r="B159" t="s">
         <v>212</v>
-      </c>
-    </row>
-    <row r="159">
-      <c r="A159" t="s">
-        <v>4</v>
-      </c>
-      <c r="B159" t="s">
-        <v>213</v>
       </c>
       <c r="C159" t="s">
         <v>94</v>
@@ -3602,12 +3604,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="160">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>4</v>
       </c>
       <c r="B160" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C160" t="s">
         <v>94</v>
@@ -3616,12 +3618,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="161">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>4</v>
       </c>
       <c r="B161" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C161" t="s">
         <v>20</v>
@@ -3630,40 +3632,40 @@
         <v>10</v>
       </c>
     </row>
-    <row r="162">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>4</v>
       </c>
       <c r="B162" t="s">
+        <v>215</v>
+      </c>
+      <c r="C162" t="s">
         <v>216</v>
-      </c>
-      <c r="C162" t="s">
-        <v>217</v>
       </c>
       <c r="D162" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="163">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>4</v>
       </c>
       <c r="B163" t="s">
+        <v>215</v>
+      </c>
+      <c r="C163" t="s">
         <v>216</v>
       </c>
-      <c r="C163" t="s">
+      <c r="D163" t="s">
         <v>217</v>
       </c>
-      <c r="D163" t="s">
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>4</v>
+      </c>
+      <c r="B164" t="s">
         <v>218</v>
-      </c>
-    </row>
-    <row r="164">
-      <c r="A164" t="s">
-        <v>4</v>
-      </c>
-      <c r="B164" t="s">
-        <v>219</v>
       </c>
       <c r="C164" t="s">
         <v>12</v>
@@ -3672,26 +3674,26 @@
         <v>10</v>
       </c>
     </row>
-    <row r="165">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>4</v>
       </c>
       <c r="B165" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C165" t="s">
         <v>32</v>
       </c>
       <c r="D165" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>4</v>
+      </c>
+      <c r="B166" t="s">
         <v>221</v>
-      </c>
-    </row>
-    <row r="166">
-      <c r="A166" t="s">
-        <v>4</v>
-      </c>
-      <c r="B166" t="s">
-        <v>222</v>
       </c>
       <c r="C166" t="s">
         <v>113</v>
@@ -3700,40 +3702,40 @@
         <v>114</v>
       </c>
     </row>
-    <row r="167">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>4</v>
       </c>
       <c r="B167" t="s">
+        <v>222</v>
+      </c>
+      <c r="C167" t="s">
         <v>223</v>
-      </c>
-      <c r="C167" t="s">
-        <v>224</v>
       </c>
       <c r="D167" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="168">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>4</v>
       </c>
       <c r="B168" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C168" t="s">
         <v>53</v>
       </c>
       <c r="D168" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>4</v>
+      </c>
+      <c r="B169" t="s">
         <v>226</v>
-      </c>
-    </row>
-    <row r="169">
-      <c r="A169" t="s">
-        <v>4</v>
-      </c>
-      <c r="B169" t="s">
-        <v>227</v>
       </c>
       <c r="C169" t="s">
         <v>86</v>
@@ -3742,12 +3744,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="170">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>4</v>
       </c>
       <c r="B170" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C170" t="s">
         <v>94</v>
@@ -3756,26 +3758,26 @@
         <v>7</v>
       </c>
     </row>
-    <row r="171">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>4</v>
       </c>
       <c r="B171" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C171" t="s">
         <v>94</v>
       </c>
       <c r="D171" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>4</v>
+      </c>
+      <c r="B172" t="s">
         <v>229</v>
-      </c>
-    </row>
-    <row r="172">
-      <c r="A172" t="s">
-        <v>4</v>
-      </c>
-      <c r="B172" t="s">
-        <v>230</v>
       </c>
       <c r="C172" t="s">
         <v>40</v>
@@ -3784,12 +3786,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="173">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>4</v>
       </c>
       <c r="B173" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C173" t="s">
         <v>105</v>
@@ -3798,12 +3800,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="174">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>4</v>
       </c>
       <c r="B174" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C174" t="s">
         <v>105</v>
@@ -3812,12 +3814,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="175">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>4</v>
       </c>
       <c r="B175" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C175" t="s">
         <v>105</v>
@@ -3826,12 +3828,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="176">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>4</v>
       </c>
       <c r="B176" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C176" t="s">
         <v>50</v>
@@ -3840,68 +3842,68 @@
         <v>7</v>
       </c>
     </row>
-    <row r="177">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>4</v>
       </c>
       <c r="B177" t="s">
+        <v>232</v>
+      </c>
+      <c r="C177" t="s">
         <v>233</v>
       </c>
-      <c r="C177" t="s">
+      <c r="D177" t="s">
         <v>234</v>
       </c>
-      <c r="D177" t="s">
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>4</v>
+      </c>
+      <c r="B178" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="178">
-      <c r="A178" t="s">
-        <v>4</v>
-      </c>
-      <c r="B178" t="s">
+      <c r="C178" t="s">
         <v>236</v>
-      </c>
-      <c r="C178" t="s">
-        <v>237</v>
       </c>
       <c r="D178" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="179">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>4</v>
       </c>
       <c r="B179" t="s">
+        <v>235</v>
+      </c>
+      <c r="C179" t="s">
         <v>236</v>
-      </c>
-      <c r="C179" t="s">
-        <v>237</v>
       </c>
       <c r="D179" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="180">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>4</v>
       </c>
       <c r="B180" t="s">
+        <v>235</v>
+      </c>
+      <c r="C180" t="s">
         <v>236</v>
       </c>
-      <c r="C180" t="s">
+      <c r="D180" t="s">
         <v>237</v>
       </c>
-      <c r="D180" t="s">
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>4</v>
+      </c>
+      <c r="B181" t="s">
         <v>238</v>
-      </c>
-    </row>
-    <row r="181">
-      <c r="A181" t="s">
-        <v>4</v>
-      </c>
-      <c r="B181" t="s">
-        <v>239</v>
       </c>
       <c r="C181" t="s">
         <v>12</v>
@@ -3910,12 +3912,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="182">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>4</v>
       </c>
       <c r="B182" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C182" t="s">
         <v>20</v>
@@ -3924,54 +3926,54 @@
         <v>10</v>
       </c>
     </row>
-    <row r="183">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>4</v>
       </c>
       <c r="B183" t="s">
+        <v>240</v>
+      </c>
+      <c r="C183" t="s">
         <v>241</v>
-      </c>
-      <c r="C183" t="s">
-        <v>242</v>
       </c>
       <c r="D183" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="184">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>4</v>
       </c>
       <c r="B184" t="s">
+        <v>242</v>
+      </c>
+      <c r="C184" t="s">
+        <v>170</v>
+      </c>
+      <c r="D184" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>4</v>
+      </c>
+      <c r="B185" t="s">
+        <v>242</v>
+      </c>
+      <c r="C185" t="s">
+        <v>170</v>
+      </c>
+      <c r="D185" t="s">
         <v>243</v>
       </c>
-      <c r="C184" t="s">
-        <v>171</v>
-      </c>
-      <c r="D184" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="185">
-      <c r="A185" t="s">
-        <v>4</v>
-      </c>
-      <c r="B185" t="s">
-        <v>243</v>
-      </c>
-      <c r="C185" t="s">
-        <v>171</v>
-      </c>
-      <c r="D185" t="s">
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>4</v>
+      </c>
+      <c r="B186" t="s">
         <v>244</v>
-      </c>
-    </row>
-    <row r="186">
-      <c r="A186" t="s">
-        <v>4</v>
-      </c>
-      <c r="B186" t="s">
-        <v>245</v>
       </c>
       <c r="C186" t="s">
         <v>50</v>
@@ -3980,12 +3982,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="187">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>4</v>
       </c>
       <c r="B187" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C187" t="s">
         <v>9</v>
@@ -3994,26 +3996,26 @@
         <v>59</v>
       </c>
     </row>
-    <row r="188">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>4</v>
       </c>
       <c r="B188" t="s">
+        <v>246</v>
+      </c>
+      <c r="C188" t="s">
         <v>247</v>
       </c>
-      <c r="C188" t="s">
+      <c r="D188" t="s">
         <v>248</v>
       </c>
-      <c r="D188" t="s">
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>4</v>
+      </c>
+      <c r="B189" t="s">
         <v>249</v>
-      </c>
-    </row>
-    <row r="189">
-      <c r="A189" t="s">
-        <v>4</v>
-      </c>
-      <c r="B189" t="s">
-        <v>250</v>
       </c>
       <c r="C189" t="s">
         <v>94</v>
@@ -4022,12 +4024,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="190">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>4</v>
       </c>
       <c r="B190" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C190" t="s">
         <v>12</v>
@@ -4036,12 +4038,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="191">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>4</v>
       </c>
       <c r="B191" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C191" t="s">
         <v>53</v>
@@ -4050,12 +4052,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="192">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>4</v>
       </c>
       <c r="B192" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C192" t="s">
         <v>105</v>
@@ -4064,12 +4066,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="193">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>4</v>
       </c>
       <c r="B193" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C193" t="s">
         <v>9</v>
@@ -4078,12 +4080,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="194">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>4</v>
       </c>
       <c r="B194" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C194" t="s">
         <v>9</v>
@@ -4092,12 +4094,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="195">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>4</v>
       </c>
       <c r="B195" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C195" t="s">
         <v>9</v>
@@ -4106,12 +4108,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="196">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>4</v>
       </c>
       <c r="B196" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C196" t="s">
         <v>9</v>
@@ -4120,12 +4122,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="197">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>4</v>
       </c>
       <c r="B197" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C197" t="s">
         <v>9</v>
@@ -4134,68 +4136,68 @@
         <v>7</v>
       </c>
     </row>
-    <row r="198">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>4</v>
       </c>
       <c r="B198" t="s">
+        <v>256</v>
+      </c>
+      <c r="C198" t="s">
         <v>257</v>
       </c>
-      <c r="C198" t="s">
+      <c r="D198" t="s">
         <v>258</v>
       </c>
-      <c r="D198" t="s">
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>4</v>
+      </c>
+      <c r="B199" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="199">
-      <c r="A199" t="s">
-        <v>4</v>
-      </c>
-      <c r="B199" t="s">
-        <v>260</v>
-      </c>
       <c r="C199" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D199" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="200">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>4</v>
       </c>
       <c r="B200" t="s">
+        <v>259</v>
+      </c>
+      <c r="C200" t="s">
+        <v>200</v>
+      </c>
+      <c r="D200" t="s">
         <v>260</v>
       </c>
-      <c r="C200" t="s">
-        <v>201</v>
-      </c>
-      <c r="D200" t="s">
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>4</v>
+      </c>
+      <c r="B201" t="s">
         <v>261</v>
-      </c>
-    </row>
-    <row r="201">
-      <c r="A201" t="s">
-        <v>4</v>
-      </c>
-      <c r="B201" t="s">
-        <v>262</v>
       </c>
       <c r="C201" t="s">
         <v>86</v>
       </c>
       <c r="D201" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="202">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>4</v>
       </c>
       <c r="B202" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C202" t="s">
         <v>86</v>
@@ -4204,12 +4206,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="203">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>4</v>
       </c>
       <c r="B203" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C203" t="s">
         <v>20</v>
@@ -4218,12 +4220,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="204">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>4</v>
       </c>
       <c r="B204" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C204" t="s">
         <v>30</v>
@@ -4232,12 +4234,12 @@
         <v>102</v>
       </c>
     </row>
-    <row r="205">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>4</v>
       </c>
       <c r="B205" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C205" t="s">
         <v>30</v>
@@ -4246,995 +4248,993 @@
         <v>26</v>
       </c>
     </row>
-    <row r="206">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
+        <v>265</v>
+      </c>
+      <c r="B206" t="s">
         <v>266</v>
       </c>
-      <c r="B206" t="s">
-        <v>267</v>
-      </c>
       <c r="C206" t="s">
+        <v>267</v>
+      </c>
+      <c r="D206" t="s">
         <v>268</v>
       </c>
-      <c r="D206" t="s">
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>265</v>
+      </c>
+      <c r="B207" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="207">
-      <c r="A207" t="s">
-        <v>266</v>
-      </c>
-      <c r="B207" t="s">
+      <c r="C207" t="s">
+        <v>267</v>
+      </c>
+      <c r="D207" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>265</v>
+      </c>
+      <c r="B208" t="s">
         <v>270</v>
       </c>
-      <c r="C207" t="s">
+      <c r="C208" t="s">
+        <v>267</v>
+      </c>
+      <c r="D208" t="s">
         <v>268</v>
       </c>
-      <c r="D207" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="208">
-      <c r="A208" t="s">
-        <v>266</v>
-      </c>
-      <c r="B208" t="s">
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>265</v>
+      </c>
+      <c r="B209" t="s">
         <v>271</v>
       </c>
-      <c r="C208" t="s">
-        <v>268</v>
-      </c>
-      <c r="D208" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="209">
-      <c r="A209" t="s">
-        <v>266</v>
-      </c>
-      <c r="B209" t="s">
-        <v>272</v>
-      </c>
       <c r="C209" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D209" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="210">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B210" t="s">
+        <v>272</v>
+      </c>
+      <c r="C210" t="s">
+        <v>267</v>
+      </c>
+      <c r="D210" t="s">
         <v>273</v>
       </c>
-      <c r="C210" t="s">
-        <v>268</v>
-      </c>
-      <c r="D210" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="211">
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B211" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C211" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D211" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="212">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B212" t="s">
+        <v>274</v>
+      </c>
+      <c r="C212" t="s">
+        <v>267</v>
+      </c>
+      <c r="D212" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>265</v>
+      </c>
+      <c r="B213" t="s">
         <v>275</v>
       </c>
-      <c r="C212" t="s">
-        <v>268</v>
-      </c>
-      <c r="D212" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="213">
-      <c r="A213" t="s">
-        <v>266</v>
-      </c>
-      <c r="B213" t="s">
+      <c r="C213" t="s">
+        <v>267</v>
+      </c>
+      <c r="D213" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>265</v>
+      </c>
+      <c r="B214" t="s">
         <v>276</v>
       </c>
-      <c r="C213" t="s">
-        <v>268</v>
-      </c>
-      <c r="D213" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="214">
-      <c r="A214" t="s">
-        <v>266</v>
-      </c>
-      <c r="B214" t="s">
-        <v>277</v>
-      </c>
       <c r="C214" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D214" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="215">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B215" t="s">
+        <v>277</v>
+      </c>
+      <c r="C215" t="s">
+        <v>267</v>
+      </c>
+      <c r="D215" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>265</v>
+      </c>
+      <c r="B216" t="s">
         <v>278</v>
       </c>
-      <c r="C215" t="s">
+      <c r="C216" t="s">
+        <v>267</v>
+      </c>
+      <c r="D216" t="s">
         <v>268</v>
       </c>
-      <c r="D215" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="216">
-      <c r="A216" t="s">
-        <v>266</v>
-      </c>
-      <c r="B216" t="s">
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>265</v>
+      </c>
+      <c r="B217" t="s">
         <v>279</v>
       </c>
-      <c r="C216" t="s">
+      <c r="C217" t="s">
+        <v>267</v>
+      </c>
+      <c r="D217" t="s">
         <v>268</v>
       </c>
-      <c r="D216" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="217">
-      <c r="A217" t="s">
-        <v>266</v>
-      </c>
-      <c r="B217" t="s">
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>265</v>
+      </c>
+      <c r="B218" t="s">
         <v>280</v>
       </c>
-      <c r="C217" t="s">
-        <v>268</v>
-      </c>
-      <c r="D217" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="218">
-      <c r="A218" t="s">
-        <v>266</v>
-      </c>
-      <c r="B218" t="s">
-        <v>281</v>
-      </c>
       <c r="C218" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D218" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="219">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B219" t="s">
+        <v>281</v>
+      </c>
+      <c r="C219" t="s">
+        <v>267</v>
+      </c>
+      <c r="D219" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>265</v>
+      </c>
+      <c r="B220" t="s">
         <v>282</v>
       </c>
-      <c r="C219" t="s">
+      <c r="C220" t="s">
+        <v>267</v>
+      </c>
+      <c r="D220" t="s">
         <v>268</v>
       </c>
-      <c r="D219" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="220">
-      <c r="A220" t="s">
-        <v>266</v>
-      </c>
-      <c r="B220" t="s">
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>265</v>
+      </c>
+      <c r="B221" t="s">
         <v>283</v>
       </c>
-      <c r="C220" t="s">
+      <c r="C221" t="s">
+        <v>267</v>
+      </c>
+      <c r="D221" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>265</v>
+      </c>
+      <c r="B222" t="s">
+        <v>285</v>
+      </c>
+      <c r="C222" t="s">
+        <v>267</v>
+      </c>
+      <c r="D222" t="s">
         <v>268</v>
       </c>
-      <c r="D220" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="221">
-      <c r="A221" t="s">
-        <v>266</v>
-      </c>
-      <c r="B221" t="s">
-        <v>284</v>
-      </c>
-      <c r="C221" t="s">
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>265</v>
+      </c>
+      <c r="B223" t="s">
+        <v>286</v>
+      </c>
+      <c r="C223" t="s">
+        <v>267</v>
+      </c>
+      <c r="D223" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>265</v>
+      </c>
+      <c r="B224" t="s">
+        <v>287</v>
+      </c>
+      <c r="C224" t="s">
+        <v>267</v>
+      </c>
+      <c r="D224" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>265</v>
+      </c>
+      <c r="B225" t="s">
+        <v>288</v>
+      </c>
+      <c r="C225" t="s">
+        <v>267</v>
+      </c>
+      <c r="D225" t="s">
         <v>268</v>
       </c>
-      <c r="D221" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="222">
-      <c r="A222" t="s">
-        <v>266</v>
-      </c>
-      <c r="B222" t="s">
-        <v>286</v>
-      </c>
-      <c r="C222" t="s">
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>265</v>
+      </c>
+      <c r="B226" t="s">
+        <v>289</v>
+      </c>
+      <c r="C226" t="s">
+        <v>267</v>
+      </c>
+      <c r="D226" t="s">
         <v>268</v>
       </c>
-      <c r="D222" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="223">
-      <c r="A223" t="s">
-        <v>266</v>
-      </c>
-      <c r="B223" t="s">
-        <v>287</v>
-      </c>
-      <c r="C223" t="s">
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>265</v>
+      </c>
+      <c r="B227" t="s">
+        <v>290</v>
+      </c>
+      <c r="C227" t="s">
+        <v>267</v>
+      </c>
+      <c r="D227" t="s">
         <v>268</v>
       </c>
-      <c r="D223" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="224">
-      <c r="A224" t="s">
-        <v>266</v>
-      </c>
-      <c r="B224" t="s">
-        <v>288</v>
-      </c>
-      <c r="C224" t="s">
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>265</v>
+      </c>
+      <c r="B228" t="s">
+        <v>291</v>
+      </c>
+      <c r="C228" t="s">
+        <v>267</v>
+      </c>
+      <c r="D228" t="s">
         <v>268</v>
       </c>
-      <c r="D224" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="225">
-      <c r="A225" t="s">
-        <v>266</v>
-      </c>
-      <c r="B225" t="s">
-        <v>289</v>
-      </c>
-      <c r="C225" t="s">
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>265</v>
+      </c>
+      <c r="B229" t="s">
+        <v>292</v>
+      </c>
+      <c r="C229" t="s">
+        <v>267</v>
+      </c>
+      <c r="D229" t="s">
         <v>268</v>
       </c>
-      <c r="D225" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="226">
-      <c r="A226" t="s">
-        <v>266</v>
-      </c>
-      <c r="B226" t="s">
-        <v>290</v>
-      </c>
-      <c r="C226" t="s">
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>265</v>
+      </c>
+      <c r="B230" t="s">
+        <v>293</v>
+      </c>
+      <c r="C230" t="s">
+        <v>267</v>
+      </c>
+      <c r="D230" t="s">
         <v>268</v>
       </c>
-      <c r="D226" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="227">
-      <c r="A227" t="s">
-        <v>266</v>
-      </c>
-      <c r="B227" t="s">
-        <v>291</v>
-      </c>
-      <c r="C227" t="s">
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>265</v>
+      </c>
+      <c r="B231" t="s">
+        <v>294</v>
+      </c>
+      <c r="C231" t="s">
+        <v>267</v>
+      </c>
+      <c r="D231" t="s">
         <v>268</v>
       </c>
-      <c r="D227" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="228">
-      <c r="A228" t="s">
-        <v>266</v>
-      </c>
-      <c r="B228" t="s">
-        <v>292</v>
-      </c>
-      <c r="C228" t="s">
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>265</v>
+      </c>
+      <c r="B232" t="s">
+        <v>295</v>
+      </c>
+      <c r="C232" t="s">
+        <v>267</v>
+      </c>
+      <c r="D232" t="s">
         <v>268</v>
       </c>
-      <c r="D228" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="229">
-      <c r="A229" t="s">
-        <v>266</v>
-      </c>
-      <c r="B229" t="s">
-        <v>293</v>
-      </c>
-      <c r="C229" t="s">
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>265</v>
+      </c>
+      <c r="B233" t="s">
+        <v>296</v>
+      </c>
+      <c r="C233" t="s">
+        <v>267</v>
+      </c>
+      <c r="D233" t="s">
         <v>268</v>
       </c>
-      <c r="D229" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="230">
-      <c r="A230" t="s">
-        <v>266</v>
-      </c>
-      <c r="B230" t="s">
-        <v>294</v>
-      </c>
-      <c r="C230" t="s">
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>265</v>
+      </c>
+      <c r="B234" t="s">
+        <v>297</v>
+      </c>
+      <c r="C234" t="s">
+        <v>267</v>
+      </c>
+      <c r="D234" t="s">
         <v>268</v>
       </c>
-      <c r="D230" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="231">
-      <c r="A231" t="s">
-        <v>266</v>
-      </c>
-      <c r="B231" t="s">
-        <v>295</v>
-      </c>
-      <c r="C231" t="s">
-        <v>268</v>
-      </c>
-      <c r="D231" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="232">
-      <c r="A232" t="s">
-        <v>266</v>
-      </c>
-      <c r="B232" t="s">
-        <v>296</v>
-      </c>
-      <c r="C232" t="s">
-        <v>268</v>
-      </c>
-      <c r="D232" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="233">
-      <c r="A233" t="s">
-        <v>266</v>
-      </c>
-      <c r="B233" t="s">
-        <v>297</v>
-      </c>
-      <c r="C233" t="s">
-        <v>268</v>
-      </c>
-      <c r="D233" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="234">
-      <c r="A234" t="s">
-        <v>266</v>
-      </c>
-      <c r="B234" t="s">
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>187</v>
+      </c>
+      <c r="B235" t="s">
         <v>298</v>
       </c>
-      <c r="C234" t="s">
-        <v>268</v>
-      </c>
-      <c r="D234" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="235">
-      <c r="A235" t="s">
-        <v>188</v>
-      </c>
-      <c r="B235" t="s">
+      <c r="C235" t="s">
+        <v>267</v>
+      </c>
+      <c r="D235" t="s">
         <v>299</v>
       </c>
-      <c r="C235" t="s">
-        <v>268</v>
-      </c>
-      <c r="D235" t="s">
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>187</v>
+      </c>
+      <c r="B236" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="236">
-      <c r="A236" t="s">
-        <v>188</v>
-      </c>
-      <c r="B236" t="s">
+      <c r="C236" t="s">
+        <v>267</v>
+      </c>
+      <c r="D236" t="s">
         <v>301</v>
       </c>
-      <c r="C236" t="s">
-        <v>268</v>
-      </c>
-      <c r="D236" t="s">
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>187</v>
+      </c>
+      <c r="B237" t="s">
+        <v>300</v>
+      </c>
+      <c r="C237" t="s">
+        <v>267</v>
+      </c>
+      <c r="D237" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="237">
-      <c r="A237" t="s">
-        <v>188</v>
-      </c>
-      <c r="B237" t="s">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>187</v>
+      </c>
+      <c r="B238" t="s">
+        <v>300</v>
+      </c>
+      <c r="C238" t="s">
+        <v>267</v>
+      </c>
+      <c r="D238" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>187</v>
+      </c>
+      <c r="B239" t="s">
+        <v>300</v>
+      </c>
+      <c r="C239" t="s">
+        <v>267</v>
+      </c>
+      <c r="D239" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>187</v>
+      </c>
+      <c r="B240" t="s">
+        <v>300</v>
+      </c>
+      <c r="C240" t="s">
+        <v>267</v>
+      </c>
+      <c r="D240" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>187</v>
+      </c>
+      <c r="B241" t="s">
+        <v>300</v>
+      </c>
+      <c r="C241" t="s">
+        <v>267</v>
+      </c>
+      <c r="D241" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>187</v>
+      </c>
+      <c r="B242" t="s">
+        <v>306</v>
+      </c>
+      <c r="C242" t="s">
+        <v>267</v>
+      </c>
+      <c r="D242" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>187</v>
+      </c>
+      <c r="B243" t="s">
+        <v>307</v>
+      </c>
+      <c r="C243" t="s">
+        <v>267</v>
+      </c>
+      <c r="D243" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>187</v>
+      </c>
+      <c r="B244" t="s">
+        <v>308</v>
+      </c>
+      <c r="C244" t="s">
+        <v>267</v>
+      </c>
+      <c r="D244" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>187</v>
+      </c>
+      <c r="B245" t="s">
+        <v>300</v>
+      </c>
+      <c r="C245" t="s">
+        <v>267</v>
+      </c>
+      <c r="D245" t="s">
         <v>301</v>
       </c>
-      <c r="C237" t="s">
-        <v>268</v>
-      </c>
-      <c r="D237" t="s">
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>187</v>
+      </c>
+      <c r="B246" t="s">
+        <v>300</v>
+      </c>
+      <c r="C246" t="s">
+        <v>267</v>
+      </c>
+      <c r="D246" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>187</v>
+      </c>
+      <c r="B247" t="s">
+        <v>300</v>
+      </c>
+      <c r="C247" t="s">
+        <v>267</v>
+      </c>
+      <c r="D247" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>187</v>
+      </c>
+      <c r="B248" t="s">
+        <v>300</v>
+      </c>
+      <c r="C248" t="s">
+        <v>267</v>
+      </c>
+      <c r="D248" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>187</v>
+      </c>
+      <c r="B249" t="s">
+        <v>309</v>
+      </c>
+      <c r="C249" t="s">
+        <v>267</v>
+      </c>
+      <c r="D249" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>187</v>
+      </c>
+      <c r="B250" t="s">
+        <v>311</v>
+      </c>
+      <c r="C250" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>187</v>
+      </c>
+      <c r="B251" t="s">
+        <v>312</v>
+      </c>
+      <c r="C251" t="s">
+        <v>267</v>
+      </c>
+      <c r="D251" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>187</v>
+      </c>
+      <c r="B252" t="s">
+        <v>313</v>
+      </c>
+      <c r="C252" t="s">
+        <v>267</v>
+      </c>
+      <c r="D252" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>187</v>
+      </c>
+      <c r="B253" t="s">
+        <v>306</v>
+      </c>
+      <c r="C253" t="s">
+        <v>267</v>
+      </c>
+      <c r="D253" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>187</v>
+      </c>
+      <c r="B254" t="s">
+        <v>314</v>
+      </c>
+      <c r="C254" t="s">
+        <v>267</v>
+      </c>
+      <c r="D254" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>187</v>
+      </c>
+      <c r="B255" t="s">
+        <v>312</v>
+      </c>
+      <c r="C255" t="s">
+        <v>267</v>
+      </c>
+      <c r="D255" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>187</v>
+      </c>
+      <c r="B256" t="s">
+        <v>315</v>
+      </c>
+      <c r="C256" t="s">
+        <v>267</v>
+      </c>
+      <c r="D256" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>187</v>
+      </c>
+      <c r="B257" t="s">
+        <v>316</v>
+      </c>
+      <c r="C257" t="s">
+        <v>267</v>
+      </c>
+      <c r="D257" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>187</v>
+      </c>
+      <c r="B258" t="s">
+        <v>317</v>
+      </c>
+      <c r="C258" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>187</v>
+      </c>
+      <c r="B259" t="s">
+        <v>318</v>
+      </c>
+      <c r="C259" t="s">
+        <v>267</v>
+      </c>
+      <c r="D259" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>187</v>
+      </c>
+      <c r="B260" t="s">
+        <v>226</v>
+      </c>
+      <c r="C260" t="s">
+        <v>267</v>
+      </c>
+      <c r="D260" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>187</v>
+      </c>
+      <c r="B261" t="s">
+        <v>319</v>
+      </c>
+      <c r="C261" t="s">
+        <v>267</v>
+      </c>
+      <c r="D261" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>187</v>
+      </c>
+      <c r="B262" t="s">
+        <v>306</v>
+      </c>
+      <c r="C262" t="s">
+        <v>267</v>
+      </c>
+      <c r="D262" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>187</v>
+      </c>
+      <c r="B263" t="s">
+        <v>195</v>
+      </c>
+      <c r="C263" t="s">
+        <v>267</v>
+      </c>
+      <c r="D263" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>187</v>
+      </c>
+      <c r="B264" t="s">
+        <v>306</v>
+      </c>
+      <c r="C264" t="s">
+        <v>267</v>
+      </c>
+      <c r="D264" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>187</v>
+      </c>
+      <c r="B265" t="s">
+        <v>320</v>
+      </c>
+      <c r="C265" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>187</v>
+      </c>
+      <c r="B266" t="s">
+        <v>321</v>
+      </c>
+      <c r="C266" t="s">
+        <v>267</v>
+      </c>
+      <c r="D266" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>187</v>
+      </c>
+      <c r="B267" t="s">
+        <v>308</v>
+      </c>
+      <c r="C267" t="s">
+        <v>267</v>
+      </c>
+      <c r="D267" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>187</v>
+      </c>
+      <c r="B268" t="s">
+        <v>322</v>
+      </c>
+      <c r="C268" t="s">
+        <v>267</v>
+      </c>
+      <c r="D268" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>187</v>
+      </c>
+      <c r="B269" t="s">
+        <v>322</v>
+      </c>
+      <c r="C269" t="s">
+        <v>267</v>
+      </c>
+      <c r="D269" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>187</v>
+      </c>
+      <c r="B270" t="s">
+        <v>322</v>
+      </c>
+      <c r="C270" t="s">
+        <v>267</v>
+      </c>
+      <c r="D270" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="238">
-      <c r="A238" t="s">
-        <v>188</v>
-      </c>
-      <c r="B238" t="s">
-        <v>301</v>
-      </c>
-      <c r="C238" t="s">
-        <v>268</v>
-      </c>
-      <c r="D238" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="239">
-      <c r="A239" t="s">
-        <v>188</v>
-      </c>
-      <c r="B239" t="s">
-        <v>301</v>
-      </c>
-      <c r="C239" t="s">
-        <v>268</v>
-      </c>
-      <c r="D239" t="s">
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>187</v>
+      </c>
+      <c r="B271" t="s">
+        <v>322</v>
+      </c>
+      <c r="C271" t="s">
+        <v>267</v>
+      </c>
+      <c r="D271" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>187</v>
+      </c>
+      <c r="B272" t="s">
+        <v>322</v>
+      </c>
+      <c r="C272" t="s">
+        <v>267</v>
+      </c>
+      <c r="D272" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="240">
-      <c r="A240" t="s">
-        <v>188</v>
-      </c>
-      <c r="B240" t="s">
-        <v>301</v>
-      </c>
-      <c r="C240" t="s">
-        <v>268</v>
-      </c>
-      <c r="D240" t="s">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>187</v>
+      </c>
+      <c r="B273" t="s">
+        <v>323</v>
+      </c>
+      <c r="C273" t="s">
+        <v>267</v>
+      </c>
+      <c r="D273" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>187</v>
+      </c>
+      <c r="B274" t="s">
+        <v>324</v>
+      </c>
+      <c r="C274" t="s">
+        <v>267</v>
+      </c>
+      <c r="D274" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>187</v>
+      </c>
+      <c r="B275" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="241">
-      <c r="A241" t="s">
-        <v>188</v>
-      </c>
-      <c r="B241" t="s">
-        <v>301</v>
-      </c>
-      <c r="C241" t="s">
-        <v>268</v>
-      </c>
-      <c r="D241" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="242">
-      <c r="A242" t="s">
-        <v>188</v>
-      </c>
-      <c r="B242" t="s">
-        <v>307</v>
-      </c>
-      <c r="C242" t="s">
-        <v>268</v>
-      </c>
-      <c r="D242" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="243">
-      <c r="A243" t="s">
-        <v>188</v>
-      </c>
-      <c r="B243" t="s">
-        <v>308</v>
-      </c>
-      <c r="C243" t="s">
-        <v>268</v>
-      </c>
-      <c r="D243" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="244">
-      <c r="A244" t="s">
-        <v>188</v>
-      </c>
-      <c r="B244" t="s">
-        <v>309</v>
-      </c>
-      <c r="C244" t="s">
-        <v>268</v>
-      </c>
-      <c r="D244" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="245">
-      <c r="A245" t="s">
-        <v>188</v>
-      </c>
-      <c r="B245" t="s">
-        <v>301</v>
-      </c>
-      <c r="C245" t="s">
-        <v>268</v>
-      </c>
-      <c r="D245" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="246">
-      <c r="A246" t="s">
-        <v>188</v>
-      </c>
-      <c r="B246" t="s">
-        <v>301</v>
-      </c>
-      <c r="C246" t="s">
-        <v>268</v>
-      </c>
-      <c r="D246" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="247">
-      <c r="A247" t="s">
-        <v>188</v>
-      </c>
-      <c r="B247" t="s">
-        <v>301</v>
-      </c>
-      <c r="C247" t="s">
-        <v>268</v>
-      </c>
-      <c r="D247" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="248">
-      <c r="A248" t="s">
-        <v>188</v>
-      </c>
-      <c r="B248" t="s">
-        <v>301</v>
-      </c>
-      <c r="C248" t="s">
-        <v>268</v>
-      </c>
-      <c r="D248" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="249">
-      <c r="A249" t="s">
-        <v>188</v>
-      </c>
-      <c r="B249" t="s">
-        <v>310</v>
-      </c>
-      <c r="C249" t="s">
-        <v>268</v>
-      </c>
-      <c r="D249" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="250">
-      <c r="A250" t="s">
-        <v>188</v>
-      </c>
-      <c r="B250" t="s">
-        <v>312</v>
-      </c>
-      <c r="C250" t="s">
-        <v>268</v>
-      </c>
-      <c r="D250"/>
-    </row>
-    <row r="251">
-      <c r="A251" t="s">
-        <v>188</v>
-      </c>
-      <c r="B251" t="s">
-        <v>313</v>
-      </c>
-      <c r="C251" t="s">
-        <v>268</v>
-      </c>
-      <c r="D251" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="252">
-      <c r="A252" t="s">
-        <v>188</v>
-      </c>
-      <c r="B252" t="s">
-        <v>314</v>
-      </c>
-      <c r="C252" t="s">
-        <v>268</v>
-      </c>
-      <c r="D252" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="253">
-      <c r="A253" t="s">
-        <v>188</v>
-      </c>
-      <c r="B253" t="s">
-        <v>307</v>
-      </c>
-      <c r="C253" t="s">
-        <v>268</v>
-      </c>
-      <c r="D253" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="254">
-      <c r="A254" t="s">
-        <v>188</v>
-      </c>
-      <c r="B254" t="s">
-        <v>315</v>
-      </c>
-      <c r="C254" t="s">
-        <v>268</v>
-      </c>
-      <c r="D254" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="255">
-      <c r="A255" t="s">
-        <v>188</v>
-      </c>
-      <c r="B255" t="s">
-        <v>313</v>
-      </c>
-      <c r="C255" t="s">
-        <v>268</v>
-      </c>
-      <c r="D255" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="256">
-      <c r="A256" t="s">
-        <v>188</v>
-      </c>
-      <c r="B256" t="s">
-        <v>316</v>
-      </c>
-      <c r="C256" t="s">
-        <v>268</v>
-      </c>
-      <c r="D256" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="257">
-      <c r="A257" t="s">
-        <v>188</v>
-      </c>
-      <c r="B257" t="s">
-        <v>317</v>
-      </c>
-      <c r="C257" t="s">
-        <v>268</v>
-      </c>
-      <c r="D257" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="258">
-      <c r="A258" t="s">
-        <v>188</v>
-      </c>
-      <c r="B258" t="s">
-        <v>318</v>
-      </c>
-      <c r="C258" t="s">
-        <v>268</v>
-      </c>
-      <c r="D258"/>
-    </row>
-    <row r="259">
-      <c r="A259" t="s">
-        <v>188</v>
-      </c>
-      <c r="B259" t="s">
-        <v>319</v>
-      </c>
-      <c r="C259" t="s">
-        <v>268</v>
-      </c>
-      <c r="D259" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="260">
-      <c r="A260" t="s">
-        <v>188</v>
-      </c>
-      <c r="B260" t="s">
-        <v>227</v>
-      </c>
-      <c r="C260" t="s">
-        <v>268</v>
-      </c>
-      <c r="D260" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="261">
-      <c r="A261" t="s">
-        <v>188</v>
-      </c>
-      <c r="B261" t="s">
-        <v>320</v>
-      </c>
-      <c r="C261" t="s">
-        <v>268</v>
-      </c>
-      <c r="D261" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="262">
-      <c r="A262" t="s">
-        <v>188</v>
-      </c>
-      <c r="B262" t="s">
-        <v>307</v>
-      </c>
-      <c r="C262" t="s">
-        <v>268</v>
-      </c>
-      <c r="D262" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="263">
-      <c r="A263" t="s">
-        <v>188</v>
-      </c>
-      <c r="B263" t="s">
-        <v>196</v>
-      </c>
-      <c r="C263" t="s">
-        <v>268</v>
-      </c>
-      <c r="D263" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="264">
-      <c r="A264" t="s">
-        <v>188</v>
-      </c>
-      <c r="B264" t="s">
-        <v>307</v>
-      </c>
-      <c r="C264" t="s">
-        <v>268</v>
-      </c>
-      <c r="D264" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="265">
-      <c r="A265" t="s">
-        <v>188</v>
-      </c>
-      <c r="B265" t="s">
-        <v>321</v>
-      </c>
-      <c r="C265" t="s">
-        <v>268</v>
-      </c>
-      <c r="D265"/>
-    </row>
-    <row r="266">
-      <c r="A266" t="s">
-        <v>188</v>
-      </c>
-      <c r="B266" t="s">
-        <v>322</v>
-      </c>
-      <c r="C266" t="s">
-        <v>268</v>
-      </c>
-      <c r="D266" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="267">
-      <c r="A267" t="s">
-        <v>188</v>
-      </c>
-      <c r="B267" t="s">
-        <v>309</v>
-      </c>
-      <c r="C267" t="s">
-        <v>268</v>
-      </c>
-      <c r="D267" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="268">
-      <c r="A268" t="s">
-        <v>188</v>
-      </c>
-      <c r="B268" t="s">
-        <v>323</v>
-      </c>
-      <c r="C268" t="s">
-        <v>268</v>
-      </c>
-      <c r="D268" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="269">
-      <c r="A269" t="s">
-        <v>188</v>
-      </c>
-      <c r="B269" t="s">
-        <v>323</v>
-      </c>
-      <c r="C269" t="s">
-        <v>268</v>
-      </c>
-      <c r="D269" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="270">
-      <c r="A270" t="s">
-        <v>188</v>
-      </c>
-      <c r="B270" t="s">
-        <v>323</v>
-      </c>
-      <c r="C270" t="s">
-        <v>268</v>
-      </c>
-      <c r="D270" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="271">
-      <c r="A271" t="s">
-        <v>188</v>
-      </c>
-      <c r="B271" t="s">
-        <v>323</v>
-      </c>
-      <c r="C271" t="s">
-        <v>268</v>
-      </c>
-      <c r="D271" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="272">
-      <c r="A272" t="s">
-        <v>188</v>
-      </c>
-      <c r="B272" t="s">
-        <v>323</v>
-      </c>
-      <c r="C272" t="s">
-        <v>268</v>
-      </c>
-      <c r="D272" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="273">
-      <c r="A273" t="s">
-        <v>188</v>
-      </c>
-      <c r="B273" t="s">
-        <v>324</v>
-      </c>
-      <c r="C273" t="s">
-        <v>268</v>
-      </c>
-      <c r="D273" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="274">
-      <c r="A274" t="s">
-        <v>188</v>
-      </c>
-      <c r="B274" t="s">
-        <v>325</v>
-      </c>
-      <c r="C274" t="s">
-        <v>268</v>
-      </c>
-      <c r="D274" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="275">
-      <c r="A275" t="s">
-        <v>188</v>
-      </c>
-      <c r="B275" t="s">
-        <v>301</v>
-      </c>
       <c r="C275" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D275" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="276">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B276" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C276" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D276" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.78740157499999996" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.78740157499999996"/>
+  <autoFilter ref="A1:D1"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>